<commit_message>
Aula 02 - Criando planilhas e links
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -2,19 +2,34 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
+    <sheet name="Matriz" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="PCEntradasN1" sheetId="4" r:id="rId3"/>
+    <sheet name="PCEntradasN2" sheetId="5" r:id="rId4"/>
+    <sheet name="PCSaídasN1" sheetId="6" r:id="rId5"/>
+    <sheet name="PCSaídasN2" sheetId="7" r:id="rId6"/>
+    <sheet name="RegistroEntradas" sheetId="8" r:id="rId7"/>
+    <sheet name="RegistroSaídas" sheetId="9" r:id="rId8"/>
+    <sheet name="FluxoCaixaConsolidado" sheetId="10" r:id="rId9"/>
+    <sheet name="DetalhaReceita" sheetId="11" r:id="rId10"/>
+    <sheet name="DetalhaDespesa" sheetId="12" r:id="rId11"/>
+    <sheet name="ContasPagar" sheetId="13" r:id="rId12"/>
+    <sheet name="ContasReceber" sheetId="14" r:id="rId13"/>
+    <sheet name="ContasReceberVencidas" sheetId="15" r:id="rId14"/>
+    <sheet name="DashBoardFinanceiroAtual" sheetId="16" r:id="rId15"/>
+    <sheet name="DashBoardFinanceiroMensal" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -33,12 +48,58 @@
   <si>
     <t>Nome do resposável</t>
   </si>
+  <si>
+    <t>TÍTULO</t>
+  </si>
+  <si>
+    <t>PLANO DE CONTAS DE ENTRADA - Nível 1</t>
+  </si>
+  <si>
+    <t>PLANO DE CONTAS DE ENTRADA - Nível 2</t>
+  </si>
+  <si>
+    <t>PLANO DE CONTAS DE SAÍDA - Nível 2</t>
+  </si>
+  <si>
+    <t>PLANO DE CONTAS DE SAÍDA - Nível 1</t>
+  </si>
+  <si>
+    <t>REGISTRO DAS ENTRADAS DE CAIXA</t>
+  </si>
+  <si>
+    <t>REGISTRO DAS SAÍDAS DE CAIXA</t>
+  </si>
+  <si>
+    <t>FLUXO DE CAIXA E RESULTADO MENSAL
+REGIMES DE CAIXA E DE COMPETÊNCIA</t>
+  </si>
+  <si>
+    <t>DETALHAMENTO DE RECEITA</t>
+  </si>
+  <si>
+    <t>DETALHAMENTO DE DESPESA</t>
+  </si>
+  <si>
+    <t>CONTAS A PAGAR</t>
+  </si>
+  <si>
+    <t>CONTAS A RECEBER</t>
+  </si>
+  <si>
+    <t>CONTAS A RECEBER VENCIDAS</t>
+  </si>
+  <si>
+    <t>DASHBOARD FINANCEIRO - POSIÇÃO ATUAL</t>
+  </si>
+  <si>
+    <t>DASHBOARD FINANCEIRO - POSIÇÃO MENSAL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,8 +123,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,6 +151,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -95,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -105,12 +180,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF3399FF"/>
+      <color rgb="FF66CCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -400,7 +485,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Retângulo 6"/>
+        <xdr:cNvPr id="7" name="Retângulo 6">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -412,9 +499,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -470,7 +555,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Retângulo 8"/>
+        <xdr:cNvPr id="9" name="Retângulo 8">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -482,9 +569,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -540,7 +625,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Retângulo 9"/>
+        <xdr:cNvPr id="10" name="Retângulo 9">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -552,9 +639,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -610,7 +695,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Retângulo 10"/>
+        <xdr:cNvPr id="11" name="Retângulo 10">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -622,9 +709,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -680,7 +765,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Retângulo 11"/>
+        <xdr:cNvPr id="12" name="Retângulo 11">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -692,9 +779,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -749,7 +834,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Retângulo 12"/>
+        <xdr:cNvPr id="13" name="Retângulo 12">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -761,9 +848,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -819,7 +904,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Retângulo 13"/>
+        <xdr:cNvPr id="14" name="Retângulo 13">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -831,9 +918,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -889,7 +974,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="Retângulo 14"/>
+        <xdr:cNvPr id="15" name="Retângulo 14">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -901,9 +988,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -959,7 +1044,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Retângulo 15"/>
+        <xdr:cNvPr id="16" name="Retângulo 15">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -971,9 +1058,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -1029,7 +1114,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Retângulo 16"/>
+        <xdr:cNvPr id="17" name="Retângulo 16">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1041,9 +1128,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -1099,7 +1184,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="Retângulo 17"/>
+        <xdr:cNvPr id="18" name="Retângulo 17">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1111,9 +1198,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -1169,7 +1254,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Retângulo 18"/>
+        <xdr:cNvPr id="19" name="Retângulo 18">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1181,9 +1268,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -1239,7 +1324,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="Retângulo 20"/>
+        <xdr:cNvPr id="21" name="Retângulo 20">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1251,9 +1338,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -1309,7 +1394,9 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="Retângulo 23"/>
+        <xdr:cNvPr id="24" name="Retângulo 23">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1321,9 +1408,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
+          <a:srgbClr val="3399FF"/>
         </a:solidFill>
         <a:ln>
           <a:noFill/>
@@ -1385,7 +1470,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1406,6 +1491,1054 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Retângulo 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1200149</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="133350" y="552450"/>
+          <a:ext cx="1200149" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="3399FF"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" b="1"/>
+            <a:t>INÍCIO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1698,11 +2831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N17"/>
+  <sheetPr codeName="Plan1"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1780,4 +2912,1074 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan10"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan11"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan12"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan13"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan14"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan15"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan16"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan2"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan3"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan4"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan5"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan6"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan7"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan8"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Plan9"/>
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+    </row>
+    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Aula 03 - Criando Planilha PCEntradasN1
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -94,12 +94,33 @@
   <si>
     <t>DASHBOARD FINANCEIRO - POSIÇÃO MENSAL</t>
   </si>
+  <si>
+    <t>PLANO DE CONTAS DE ENTRADA NÍVEL 1</t>
+  </si>
+  <si>
+    <t>Nível 1</t>
+  </si>
+  <si>
+    <t>Empréstimos de curto prazo</t>
+  </si>
+  <si>
+    <t>Financiamentos de longo prazo</t>
+  </si>
+  <si>
+    <t>Receitas Financeiras</t>
+  </si>
+  <si>
+    <t>Venda de ativos</t>
+  </si>
+  <si>
+    <t>Vendas de mercadorias</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +146,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
@@ -132,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +186,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -170,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -181,14 +216,27 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
@@ -2542,6 +2590,16 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B4:B9"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nível 1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2834,7 +2892,7 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3489,7 +3547,10 @@
   <sheetPr codeName="Plan3"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3534,13 +3595,65 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3552,6 +3665,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 04 - Planilha PCEntradasN2
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,15 @@
     <sheet name="DashBoardFinanceiroAtual" sheetId="16" r:id="rId15"/>
     <sheet name="DashBoardFinanceiroMensal" sheetId="17" r:id="rId16"/>
   </sheets>
+  <definedNames>
+    <definedName name="PCEntradasN1_Nível_1">TbPCEntradasN1[Nível 1]</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -115,6 +118,36 @@
   <si>
     <t>Vendas de mercadorias</t>
   </si>
+  <si>
+    <t>PLANO DE CONTAS DE ENTRADAS NÍVEL 2</t>
+  </si>
+  <si>
+    <t>Nível 2</t>
+  </si>
+  <si>
+    <t>Empréstimos capital de giro</t>
+  </si>
+  <si>
+    <t>Juros sobre aplicações</t>
+  </si>
+  <si>
+    <t>Mobiliário próprio</t>
+  </si>
+  <si>
+    <t>Eletrodomésticos</t>
+  </si>
+  <si>
+    <t>Informática</t>
+  </si>
+  <si>
+    <t>Livros</t>
+  </si>
+  <si>
+    <t>Móveis</t>
+  </si>
+  <si>
+    <t>Som e imagem</t>
+  </si>
 </sst>
 </file>
 
@@ -193,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -201,11 +234,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -216,18 +290,25 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -235,6 +316,37 @@
           <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -2597,6 +2709,17 @@
   <autoFilter ref="B4:B9"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="2">
+  <autoFilter ref="B4:C12"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nível 1"/>
+    <tableColumn id="2" name="Nível 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3547,9 +3670,9 @@
   <sheetPr codeName="Plan3"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3596,7 +3719,7 @@
       <c r="N2" s="5"/>
     </row>
     <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="5"/>
@@ -3613,7 +3736,7 @@
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="5"/>
@@ -3676,13 +3799,17 @@
   <sheetPr codeName="Plan4"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="44.5703125" customWidth="1"/>
+    <col min="4" max="14" width="8.7109375" customWidth="1"/>
     <col min="15" max="15" width="2.140625" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
@@ -3721,24 +3848,125 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B12">
+      <formula1>PCEntradasN1_Nível_1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -4053,13 +4281,13 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>

</xml_diff>

<commit_message>
Aula 05 - Planilha PCSaídasN1
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,12 @@
   <definedNames>
     <definedName name="PCEntradasN1_Nível_1">TbPCEntradasN1[Nível 1]</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -147,6 +147,27 @@
   </si>
   <si>
     <t>Som e imagem</t>
+  </si>
+  <si>
+    <t>PLANO DE CONTAS DE SAÍDA NÍVEL 1</t>
+  </si>
+  <si>
+    <t>Compra de mercadorias</t>
+  </si>
+  <si>
+    <t>Despesas administrativas</t>
+  </si>
+  <si>
+    <t>Despesas comerciais</t>
+  </si>
+  <si>
+    <t>Despesas financeiras</t>
+  </si>
+  <si>
+    <t>Imposto de renda</t>
+  </si>
+  <si>
+    <t>Impostos sobre as vendas</t>
   </si>
 </sst>
 </file>
@@ -279,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -304,11 +325,46 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2705,7 +2761,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="B4:B9"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -2715,11 +2771,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="4">
   <autoFilter ref="B4:C12"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
     <tableColumn id="2" name="Nível 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1">
+  <autoFilter ref="B4:B10"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Nível 1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3799,9 +3865,9 @@
   <sheetPr codeName="Plan4"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3975,7 +4041,10 @@
   <sheetPr codeName="Plan5"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4020,14 +4089,70 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4038,6 +4163,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 06 - Planilha PCSaídasN2
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -26,13 +26,14 @@
   </sheets>
   <definedNames>
     <definedName name="PCEntradasN1_Nível_1">TbPCEntradasN1[Nível 1]</definedName>
+    <definedName name="PCSaídasN1_Nível_1">TbPCSaídasN1[Nível 1]</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -168,6 +169,30 @@
   </si>
   <si>
     <t>Impostos sobre as vendas</t>
+  </si>
+  <si>
+    <t>PLANO DE CONTAS DE SAÍDA NÍVEL 2</t>
+  </si>
+  <si>
+    <t>Vestuário</t>
+  </si>
+  <si>
+    <t>Comunicação - internet e telefonia</t>
+  </si>
+  <si>
+    <t>Energia elétrica</t>
+  </si>
+  <si>
+    <t>Encargos sobre os salários dos vendedores</t>
+  </si>
+  <si>
+    <t>Salários dos vendedores</t>
+  </si>
+  <si>
+    <t>Juros sobre empréstimos</t>
+  </si>
+  <si>
+    <t>IR sobre o lucro presumido</t>
   </si>
 </sst>
 </file>
@@ -318,6 +343,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -325,23 +353,22 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -350,12 +377,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -364,6 +385,14 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2761,7 +2790,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="B4:B9"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -2771,7 +2800,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="5">
   <autoFilter ref="B4:C12"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
@@ -2786,6 +2815,17 @@
   <autoFilter ref="B4:B10"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="B4:C15"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Nível 1"/>
+    <tableColumn id="2" name="Nível 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3867,7 +3907,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3915,10 +3955,10 @@
       <c r="N2" s="5"/>
     </row>
     <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -3932,10 +3972,10 @@
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="5"/>
@@ -4041,9 +4081,9 @@
   <sheetPr codeName="Plan5"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4107,7 +4147,7 @@
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="5"/>
@@ -4174,13 +4214,17 @@
   <sheetPr codeName="Plan6"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" customWidth="1"/>
+    <col min="4" max="14" width="8.7109375" customWidth="1"/>
     <col min="15" max="15" width="2.140625" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
@@ -4219,24 +4263,146 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B15">
+      <formula1>PCSaídasN1_Nível_1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 07 - Planilha RegistroEntradas
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -193,12 +193,48 @@
   </si>
   <si>
     <t>IR sobre o lucro presumido</t>
+  </si>
+  <si>
+    <t>Data do Caixa Realizado</t>
+  </si>
+  <si>
+    <t>Data da Competência</t>
+  </si>
+  <si>
+    <t>Data do Caixa Previsto</t>
+  </si>
+  <si>
+    <t>Conta Nível 1</t>
+  </si>
+  <si>
+    <t>Conta Nível 2</t>
+  </si>
+  <si>
+    <t>Histórico</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>NF001</t>
+  </si>
+  <si>
+    <t>NF773</t>
+  </si>
+  <si>
+    <t>NF2639</t>
+  </si>
+  <si>
+    <t>NF-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -325,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -340,27 +376,86 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -393,22 +488,6 @@
           <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -427,11 +506,12 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -2790,7 +2870,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="B4:B9"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -2800,7 +2880,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
   <autoFilter ref="B4:C12"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
@@ -2811,7 +2891,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6">
   <autoFilter ref="B4:B10"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -2821,11 +2901,27 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="B4:C15"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
     <tableColumn id="2" name="Nível 2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B3:H7" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="B3:H7"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="4"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="3"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="0"/>
+    <tableColumn id="4" name="Conta Nível 1"/>
+    <tableColumn id="5" name="Conta Nível 2"/>
+    <tableColumn id="6" name="Histórico"/>
+    <tableColumn id="7" name="Valor" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3955,10 +4051,10 @@
       <c r="N2" s="5"/>
     </row>
     <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -3972,10 +4068,10 @@
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="5"/>
@@ -4130,7 +4226,7 @@
       <c r="N2" s="5"/>
     </row>
     <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="9" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="5"/>
@@ -4147,7 +4243,7 @@
       <c r="N3" s="5"/>
     </row>
     <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="5"/>
@@ -4214,7 +4310,7 @@
   <sheetPr codeName="Plan6"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
@@ -4264,10 +4360,10 @@
       <c r="N2" s="5"/>
     </row>
     <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -4411,69 +4507,184 @@
   <sheetPr codeName="Plan7"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="33.140625" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="51.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" customWidth="1"/>
+    <col min="10" max="15" width="0" hidden="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="4" t="s">
+      <c r="H1" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+    <row r="2" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-    </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="2:8" s="21" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="13">
+        <v>43146</v>
+      </c>
+      <c r="C4" s="13">
+        <v>43146</v>
+      </c>
+      <c r="D4" s="13">
+        <v>43146</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="16">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="13">
+        <v>43530</v>
+      </c>
+      <c r="C5" s="13">
+        <v>43466</v>
+      </c>
+      <c r="D5" s="13">
+        <v>43496</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="16">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="13">
+        <v>43467</v>
+      </c>
+      <c r="C6" s="13">
+        <v>43467</v>
+      </c>
+      <c r="D6" s="13">
+        <v>43467</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="16">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13">
+        <v>43535</v>
+      </c>
+      <c r="C7" s="13">
+        <v>43467</v>
+      </c>
+      <c r="D7" s="13">
+        <v>43497</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E7">
+      <formula1>PCEntradasN1_Nível_1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -4575,13 +4786,13 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>

</xml_diff>

<commit_message>
Aula 08 - Planilha RegistroEntradas (Validacao Conta Nivel 2)
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -26,6 +26,8 @@
   </sheets>
   <definedNames>
     <definedName name="PCEntradasN1_Nível_1">TbPCEntradasN1[Nível 1]</definedName>
+    <definedName name="PCEntradasN2_Nível_1">TbPCEntradasN2[Nível 1]</definedName>
+    <definedName name="PCEntradasN2_Nível_2">TbPCEntradasN2[Nível 2]</definedName>
     <definedName name="PCSaídasN1_Nível_1">TbPCSaídasN1[Nível 1]</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="65">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -226,6 +228,9 @@
   </si>
   <si>
     <t>NF-16</t>
+  </si>
+  <si>
+    <t>Geral</t>
   </si>
 </sst>
 </file>
@@ -421,6 +426,37 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
@@ -472,37 +508,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -2880,8 +2885,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C12" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
-  <autoFilter ref="B4:C12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C13" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+  <autoFilter ref="B4:C13"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
     <tableColumn id="2" name="Nível 2"/>
@@ -2891,7 +2896,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
   <autoFilter ref="B4:B10"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -2901,7 +2906,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="B4:C15"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
@@ -2912,16 +2917,16 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B3:H7" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B3:H7" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="B3:H7"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="4"/>
-    <tableColumn id="2" name="Data da Competência" dataDxfId="3"/>
-    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="0"/>
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="6"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="5"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="2"/>
     <tableColumn id="4" name="Conta Nível 1"/>
     <tableColumn id="5" name="Conta Nível 2"/>
     <tableColumn id="6" name="Histórico"/>
-    <tableColumn id="7" name="Valor" dataDxfId="2"/>
+    <tableColumn id="7" name="Valor" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4003,7 +4008,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:N4"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4150,7 +4155,14 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4160,7 +4172,7 @@
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B13">
       <formula1>PCEntradasN1_Nível_1</formula1>
     </dataValidation>
   </dataValidations>
@@ -4312,7 +4324,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4509,7 +4521,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4655,7 +4667,7 @@
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
         <v>63</v>
@@ -4675,9 +4687,12 @@
     <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E7">
       <formula1>PCEntradasN1_Nível_1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F7">
+      <formula1>OFFSET(PCEntradasN2_Nível_2,MATCH(E4,PCEntradasN2_Nível_1,0)-1,0,COUNTIF(PCEntradasN2_Nível_1,E4))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Aula 09 - Planilha RegistroSaídas
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="68">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -231,6 +231,15 @@
   </si>
   <si>
     <t>Geral</t>
+  </si>
+  <si>
+    <t>NF1234</t>
+  </si>
+  <si>
+    <t>NF2187</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -313,7 +322,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -362,11 +371,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -420,11 +438,70 @@
     <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <border>
         <bottom style="thin">
@@ -2875,7 +2952,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="B4:B9"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -2885,7 +2962,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C13" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C13" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7">
   <autoFilter ref="B4:C13"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
@@ -2896,7 +2973,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15">
   <autoFilter ref="B4:B10"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -2906,7 +2983,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="B4:C15"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
@@ -2917,16 +2994,32 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B3:H7" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B3:H7" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="B3:H7"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="6"/>
-    <tableColumn id="2" name="Data da Competência" dataDxfId="5"/>
-    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="2"/>
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="13"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="12"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="9"/>
     <tableColumn id="4" name="Conta Nível 1"/>
     <tableColumn id="5" name="Conta Nível 2"/>
     <tableColumn id="6" name="Histórico"/>
-    <tableColumn id="7" name="Valor" dataDxfId="4"/>
+    <tableColumn id="7" name="Valor" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TbRegistroSaídas" displayName="TbRegistroSaídas" ref="B3:H7" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5">
+  <autoFilter ref="B3:H7"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="3"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="2"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="1"/>
+    <tableColumn id="4" name="Conta Nível 1"/>
+    <tableColumn id="5" name="Conta Nível 2"/>
+    <tableColumn id="6" name="Histórico"/>
+    <tableColumn id="7" name="Valor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4191,7 +4284,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B10"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4519,9 +4612,9 @@
   <sheetPr codeName="Plan7"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4708,18 +4801,26 @@
   <sheetPr codeName="Plan8"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -4728,17 +4829,11 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -4746,31 +4841,143 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-    </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="3" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="13">
+        <v>43147</v>
+      </c>
+      <c r="C4" s="13">
+        <v>43147</v>
+      </c>
+      <c r="D4" s="13">
+        <v>43147</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="16">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="13">
+        <v>43531</v>
+      </c>
+      <c r="C5" s="13">
+        <v>43466</v>
+      </c>
+      <c r="D5" s="13">
+        <v>43496</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="16">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="13">
+        <v>43496</v>
+      </c>
+      <c r="C6" s="13">
+        <v>43466</v>
+      </c>
+      <c r="D6" s="13">
+        <v>43496</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="16">
+        <v>4615.2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13">
+        <v>43496</v>
+      </c>
+      <c r="C7" s="13">
+        <v>43466</v>
+      </c>
+      <c r="D7" s="13">
+        <v>43496</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="16">
+        <v>15384</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E7">
+      <formula1>PCSaídasN1_Nível_1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Aula 10 - Planilha RegistroSaidas (Validacao Conta Nivel 2)
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -29,13 +29,15 @@
     <definedName name="PCEntradasN2_Nível_1">TbPCEntradasN2[Nível 1]</definedName>
     <definedName name="PCEntradasN2_Nível_2">TbPCEntradasN2[Nível 2]</definedName>
     <definedName name="PCSaídasN1_Nível_1">TbPCSaídasN1[Nível 1]</definedName>
+    <definedName name="PCSaídasN2_Nível_1">TbPCSaídasN2[Nível 1]</definedName>
+    <definedName name="PCSaídasN2_Nível_2">TbPCSaídasN2[Nível 2]</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="68">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -2983,8 +2985,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C15" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="B4:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C16" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="B4:C16"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
     <tableColumn id="2" name="Nível 2"/>
@@ -4417,7 +4419,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4588,14 +4590,21 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:C3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B16">
       <formula1>PCSaídasN1_Nível_1</formula1>
     </dataValidation>
   </dataValidations>
@@ -4803,7 +4812,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4968,9 +4977,12 @@
     <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E7">
       <formula1>PCSaídasN1_Nível_1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4:F7">
+      <formula1>OFFSET(PCSaídasN2_Nível_2,MATCH(E4,PCSaídasN2_Nível_1,0)-1,0,COUNTIF(PCSaídasN2_Nível_1,E4))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Aula 12 - Iniciando planilha FluxoCaixaConsolidado
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1601" uniqueCount="538">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -1574,16 +1574,95 @@
   </si>
   <si>
     <t>NF4931</t>
+  </si>
+  <si>
+    <t>ANO &gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>FLUXO DE CAIXA - REGIME DE CAIXA (Realizado)</t>
+  </si>
+  <si>
+    <t>ESPECIFICAÇÃO</t>
+  </si>
+  <si>
+    <t>SAÍDA</t>
+  </si>
+  <si>
+    <t>SALDO FINAL</t>
+  </si>
+  <si>
+    <t>JAN</t>
+  </si>
+  <si>
+    <t>FEV</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>ABR</t>
+  </si>
+  <si>
+    <t>MAI</t>
+  </si>
+  <si>
+    <t>JUN</t>
+  </si>
+  <si>
+    <t>JUL</t>
+  </si>
+  <si>
+    <t>AGO</t>
+  </si>
+  <si>
+    <t>SET</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>NOV</t>
+  </si>
+  <si>
+    <t>DEZ</t>
+  </si>
+  <si>
+    <t>ENTRADAS</t>
+  </si>
+  <si>
+    <t>SALDO INICIAL</t>
+  </si>
+  <si>
+    <t>FLUXO DE CAIXA - REGIME DE COMPETÊNCIA (Contábil)</t>
+  </si>
+  <si>
+    <t>RESULTADO MENSAL - REGIME DE COMPETÊNCIA</t>
+  </si>
+  <si>
+    <t>TOTAL DE ENTRADAS</t>
+  </si>
+  <si>
+    <t>TOTAL DE SAÍDAS</t>
+  </si>
+  <si>
+    <t>LUCRO</t>
+  </si>
+  <si>
+    <t>PREJUÍZO</t>
+  </si>
+  <si>
+    <t>ACUMULADO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1623,8 +1702,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1655,8 +1758,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1714,11 +1823,143 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1780,6 +2021,63 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -11353,7 +11651,7 @@
   <sheetPr codeName="Plan8"/>
   <dimension ref="A1:O232"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
@@ -16705,15 +17003,17 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan9"/>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="14" width="13.7109375" customWidth="1"/>
     <col min="15" max="15" width="2.140625" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
@@ -16752,21 +17052,402 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
     </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="30" t="s">
+        <v>512</v>
+      </c>
+      <c r="C3" s="28">
+        <v>2019</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
     <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="29" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="33" t="s">
+        <v>514</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>517</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>518</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>520</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>521</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>522</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>523</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>524</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>525</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>526</v>
+      </c>
+      <c r="M7" s="31" t="s">
+        <v>527</v>
+      </c>
+      <c r="N7" s="32" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="43" t="s">
+        <v>530</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="35"/>
+    </row>
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="43" t="s">
+        <v>529</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="35"/>
+    </row>
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="43" t="s">
+        <v>515</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="35"/>
+    </row>
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="46" t="s">
+        <v>516</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="37"/>
+    </row>
     <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="38" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="33" t="s">
+        <v>514</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>517</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>518</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="F14" s="31" t="s">
+        <v>520</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>521</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>522</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>523</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>524</v>
+      </c>
+      <c r="K14" s="31" t="s">
+        <v>525</v>
+      </c>
+      <c r="L14" s="31" t="s">
+        <v>526</v>
+      </c>
+      <c r="M14" s="31" t="s">
+        <v>527</v>
+      </c>
+      <c r="N14" s="32" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="43" t="s">
+        <v>530</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="35"/>
+    </row>
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="43" t="s">
+        <v>529</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="35"/>
+    </row>
+    <row r="17" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="43" t="s">
+        <v>515</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="35"/>
+    </row>
+    <row r="18" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="46" t="s">
+        <v>516</v>
+      </c>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="37"/>
+    </row>
+    <row r="19" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="38" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="33" t="s">
+        <v>514</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>517</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>518</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>519</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>520</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>521</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>522</v>
+      </c>
+      <c r="I21" s="31" t="s">
+        <v>523</v>
+      </c>
+      <c r="J21" s="31" t="s">
+        <v>524</v>
+      </c>
+      <c r="K21" s="31" t="s">
+        <v>525</v>
+      </c>
+      <c r="L21" s="31" t="s">
+        <v>526</v>
+      </c>
+      <c r="M21" s="31" t="s">
+        <v>527</v>
+      </c>
+      <c r="N21" s="32" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="43" t="s">
+        <v>533</v>
+      </c>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="35"/>
+    </row>
+    <row r="23" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="43" t="s">
+        <v>534</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="35"/>
+    </row>
+    <row r="24" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="44" t="s">
+        <v>535</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="42"/>
+    </row>
+    <row r="25" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="45" t="s">
+        <v>536</v>
+      </c>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="40"/>
+    </row>
+    <row r="26" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="45" t="s">
+        <v>537</v>
+      </c>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="40"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J1:N1"/>

</xml_diff>

<commit_message>
Aula 17 - Planilha DetalhaDespesa
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="732" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -32,17 +32,22 @@
     <definedName name="PCSaídasN2_Nível_1">TbPCSaídasN2[Nível 1]</definedName>
     <definedName name="PCSaídasN2_Nível_2">TbPCSaídasN2[Nível 2]</definedName>
     <definedName name="SegmentaçãodeDados_Ano_Competência">#N/A</definedName>
+    <definedName name="SegmentaçãodeDados_Ano_Competência1">#N/A</definedName>
     <definedName name="SegmentaçãodeDados_Mês_Competência">#N/A</definedName>
+    <definedName name="SegmentaçãodeDados_Mês_Competência1">#N/A</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
     <pivotCache cacheId="5" r:id="rId17"/>
+    <pivotCache cacheId="11" r:id="rId18"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId18"/>
         <x14:slicerCache r:id="rId19"/>
+        <x14:slicerCache r:id="rId20"/>
+        <x14:slicerCache r:id="rId21"/>
+        <x14:slicerCache r:id="rId22"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -53,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="546">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -3897,6 +3902,152 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1028700</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Mês Competência 1"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Mês Competência 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3771900" y="552450"/>
+              <a:ext cx="2143125" cy="981075"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100"/>
+                <a:t>Esta forma representa um slicer. Os slicers podem ser usados, no mínimo, no Excel 2010.
+Caso a forma tenha sido modificada em uma versão anterior do Excel, ou a pasta de trabalho tenha sido salva no Excel 2003 ou
+anterior, o slicer não poderá ser usado.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1028700</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Ano Competência 1"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Ano Competência 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1495425" y="552450"/>
+              <a:ext cx="2143125" cy="981075"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100"/>
+                <a:t>Esta forma representa um slicer. Os slicers podem ser usados, no mínimo, no Excel 2010.
+Caso a forma tenha sido modificada em uma versão anterior do Excel, ou a pasta de trabalho tenha sido salva no Excel 2003 ou
+anterior, o slicer não poderá ser usado.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4881,6 +5032,79 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Autor" refreshedDate="43944.492473148151" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="229">
+  <cacheSource type="worksheet">
+    <worksheetSource name="TbRegistroSaídas"/>
+  </cacheSource>
+  <cacheFields count="11">
+    <cacheField name="Data do Caixa Realizado" numFmtId="14">
+      <sharedItems containsDate="1" containsMixedTypes="1" minDate="2017-09-02T00:00:00" maxDate="2019-07-19T00:00:00"/>
+    </cacheField>
+    <cacheField name="Data da Competência" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2017-08-10T00:00:00" maxDate="2019-07-01T00:00:00"/>
+    </cacheField>
+    <cacheField name="Data do Caixa Previsto" numFmtId="14">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2017-09-02T00:00:00" maxDate="2019-08-10T00:00:00"/>
+    </cacheField>
+    <cacheField name="Conta Nível 1" numFmtId="0">
+      <sharedItems count="1">
+        <s v="Compra de mercadorias"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Conta Nível 2" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Som e imagem"/>
+        <s v="Vestuário"/>
+        <s v="Informática"/>
+        <s v="Livros"/>
+        <s v="Eletrodomésticos"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Histórico" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Valor" numFmtId="44">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="131" maxValue="4947"/>
+    </cacheField>
+    <cacheField name="Mês Caixa" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="12"/>
+    </cacheField>
+    <cacheField name="Ano Caixa" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="2019"/>
+    </cacheField>
+    <cacheField name="Mês Competência" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="12" count="12">
+        <n v="8"/>
+        <n v="9"/>
+        <n v="10"/>
+        <n v="11"/>
+        <n v="12"/>
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
+        <n v="7"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Ano Competência" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2017" maxValue="2019" count="3">
+        <n v="2017"/>
+        <n v="2018"/>
+        <n v="2019"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition pivotCacheId="2"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="231">
   <r>
@@ -7881,6 +8105,2988 @@
     <x v="1"/>
     <s v="NF3701"/>
     <n v="3446"/>
+    <n v="7"/>
+    <n v="2019"/>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="229">
+  <r>
+    <d v="2017-10-07T00:00:00"/>
+    <d v="2017-08-10T00:00:00"/>
+    <d v="2017-10-07T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF4400"/>
+    <n v="4021"/>
+    <n v="10"/>
+    <n v="2017"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-09-17T00:00:00"/>
+    <d v="2017-08-13T00:00:00"/>
+    <d v="2017-09-17T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF5356"/>
+    <n v="651"/>
+    <n v="9"/>
+    <n v="2017"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-09-05T00:00:00"/>
+    <d v="2017-08-18T00:00:00"/>
+    <d v="2017-09-05T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF1847"/>
+    <n v="131"/>
+    <n v="9"/>
+    <n v="2017"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-09-26T00:00:00"/>
+    <d v="2017-08-23T00:00:00"/>
+    <d v="2017-09-26T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF7011"/>
+    <n v="803"/>
+    <n v="9"/>
+    <n v="2017"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-09-24T00:00:00"/>
+    <d v="2017-08-24T00:00:00"/>
+    <d v="2017-09-24T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7746"/>
+    <n v="4460"/>
+    <n v="9"/>
+    <n v="2017"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-09-02T00:00:00"/>
+    <d v="2017-08-25T00:00:00"/>
+    <d v="2017-09-02T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF1507"/>
+    <n v="299"/>
+    <n v="9"/>
+    <n v="2017"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-10-06T00:00:00"/>
+    <d v="2017-08-29T00:00:00"/>
+    <d v="2017-10-06T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF5445"/>
+    <n v="618"/>
+    <n v="10"/>
+    <n v="2017"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-09-12T00:00:00"/>
+    <d v="2017-09-01T00:00:00"/>
+    <d v="2017-09-02T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7526"/>
+    <n v="2505"/>
+    <n v="9"/>
+    <n v="2017"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-09-09T00:00:00"/>
+    <d v="2017-09-04T00:00:00"/>
+    <d v="2017-09-09T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF7559"/>
+    <n v="817"/>
+    <n v="9"/>
+    <n v="2017"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2017-09-06T00:00:00"/>
+    <d v="2017-09-06T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF9357"/>
+    <n v="1565"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2017-09-12T00:00:00"/>
+    <d v="2017-10-12T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF3898"/>
+    <n v="1357"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-09-13T00:00:00"/>
+    <d v="2017-09-13T00:00:00"/>
+    <d v="2017-09-13T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF7275"/>
+    <n v="4739"/>
+    <n v="9"/>
+    <n v="2017"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-09-14T00:00:00"/>
+    <d v="2017-09-14T00:00:00"/>
+    <d v="2017-09-14T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF9591"/>
+    <n v="4675"/>
+    <n v="9"/>
+    <n v="2017"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-09-26T00:00:00"/>
+    <d v="2017-09-19T00:00:00"/>
+    <d v="2017-09-26T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF3104"/>
+    <n v="1797"/>
+    <n v="9"/>
+    <n v="2017"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-11-04T00:00:00"/>
+    <d v="2017-09-24T00:00:00"/>
+    <d v="2017-11-04T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF3440"/>
+    <n v="888"/>
+    <n v="11"/>
+    <n v="2017"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2017-09-25T00:00:00"/>
+    <d v="2017-10-07T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF9195"/>
+    <n v="2784"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-10-02T00:00:00"/>
+    <d v="2017-09-25T00:00:00"/>
+    <d v="2017-10-02T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF1821"/>
+    <n v="707"/>
+    <n v="10"/>
+    <n v="2017"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-11-03T00:00:00"/>
+    <d v="2017-09-28T00:00:00"/>
+    <d v="2017-11-03T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF5625"/>
+    <n v="229"/>
+    <n v="11"/>
+    <n v="2017"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-10-01T00:00:00"/>
+    <d v="2017-10-01T00:00:00"/>
+    <d v="2017-10-01T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7471"/>
+    <n v="2894"/>
+    <n v="10"/>
+    <n v="2017"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-10-22T00:00:00"/>
+    <d v="2017-10-04T00:00:00"/>
+    <d v="2017-10-22T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF9225"/>
+    <n v="4516"/>
+    <n v="10"/>
+    <n v="2017"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-10-23T00:00:00"/>
+    <d v="2017-10-06T00:00:00"/>
+    <d v="2017-10-23T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF3883"/>
+    <n v="885"/>
+    <n v="10"/>
+    <n v="2017"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-11-07T00:00:00"/>
+    <d v="2017-10-09T00:00:00"/>
+    <d v="2017-11-07T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF9408"/>
+    <n v="1509"/>
+    <n v="11"/>
+    <n v="2017"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-10-14T00:00:00"/>
+    <d v="2017-10-14T00:00:00"/>
+    <d v="2017-10-14T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF1517"/>
+    <n v="145"/>
+    <n v="10"/>
+    <n v="2017"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-10-23T00:00:00"/>
+    <d v="2017-10-16T00:00:00"/>
+    <d v="2017-10-23T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF8626"/>
+    <n v="1311"/>
+    <n v="10"/>
+    <n v="2017"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-10-18T00:00:00"/>
+    <d v="2017-10-18T00:00:00"/>
+    <d v="2017-10-18T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4936"/>
+    <n v="4182"/>
+    <n v="10"/>
+    <n v="2017"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-11-26T00:00:00"/>
+    <d v="2017-10-24T00:00:00"/>
+    <d v="2017-10-29T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF7062"/>
+    <n v="339"/>
+    <n v="11"/>
+    <n v="2017"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-12-02T00:00:00"/>
+    <d v="2017-10-29T00:00:00"/>
+    <d v="2017-11-29T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF3172"/>
+    <n v="1788"/>
+    <n v="12"/>
+    <n v="2017"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-12-20T00:00:00"/>
+    <d v="2017-11-03T00:00:00"/>
+    <d v="2017-12-20T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF5821"/>
+    <n v="1171"/>
+    <n v="12"/>
+    <n v="2017"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-11-05T00:00:00"/>
+    <d v="2017-11-05T00:00:00"/>
+    <d v="2017-11-05T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF8137"/>
+    <n v="4059"/>
+    <n v="11"/>
+    <n v="2017"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-11-08T00:00:00"/>
+    <d v="2017-11-08T00:00:00"/>
+    <d v="2017-11-08T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF8083"/>
+    <n v="4919"/>
+    <n v="11"/>
+    <n v="2017"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-12-18T00:00:00"/>
+    <d v="2017-11-12T00:00:00"/>
+    <d v="2017-12-18T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF9597"/>
+    <n v="3224"/>
+    <n v="12"/>
+    <n v="2017"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-12-26T00:00:00"/>
+    <d v="2017-11-15T00:00:00"/>
+    <d v="2017-12-26T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF2065"/>
+    <n v="3725"/>
+    <n v="12"/>
+    <n v="2017"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-11-17T00:00:00"/>
+    <d v="2017-11-17T00:00:00"/>
+    <d v="2017-11-17T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF3192"/>
+    <n v="312"/>
+    <n v="11"/>
+    <n v="2017"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2018-01-12T00:00:00"/>
+    <d v="2017-11-18T00:00:00"/>
+    <d v="2018-01-12T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF1977"/>
+    <n v="4773"/>
+    <n v="1"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2018-01-01T00:00:00"/>
+    <d v="2017-11-19T00:00:00"/>
+    <d v="2017-11-19T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF3208"/>
+    <n v="228"/>
+    <n v="1"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-11-22T00:00:00"/>
+    <d v="2017-11-22T00:00:00"/>
+    <d v="2017-11-22T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF9545"/>
+    <n v="450"/>
+    <n v="11"/>
+    <n v="2017"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2018-01-03T00:00:00"/>
+    <d v="2017-11-23T00:00:00"/>
+    <d v="2018-01-03T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF3100"/>
+    <n v="1155"/>
+    <n v="1"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-12-01T00:00:00"/>
+    <d v="2017-11-30T00:00:00"/>
+    <d v="2017-12-01T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7746"/>
+    <n v="1967"/>
+    <n v="12"/>
+    <n v="2017"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-12-27T00:00:00"/>
+    <d v="2017-12-01T00:00:00"/>
+    <d v="2017-12-27T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF1179"/>
+    <n v="2741"/>
+    <n v="12"/>
+    <n v="2017"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2018-01-25T00:00:00"/>
+    <d v="2017-12-02T00:00:00"/>
+    <d v="2018-01-25T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF3829"/>
+    <n v="1130"/>
+    <n v="1"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-12-06T00:00:00"/>
+    <d v="2017-12-06T00:00:00"/>
+    <d v="2017-12-06T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF6865"/>
+    <n v="4835"/>
+    <n v="12"/>
+    <n v="2017"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-12-08T00:00:00"/>
+    <d v="2017-12-08T00:00:00"/>
+    <d v="2017-12-08T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF4400"/>
+    <n v="1411"/>
+    <n v="12"/>
+    <n v="2017"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-12-30T00:00:00"/>
+    <d v="2017-12-10T00:00:00"/>
+    <d v="2017-12-30T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF9617"/>
+    <n v="457"/>
+    <n v="12"/>
+    <n v="2017"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2017-12-15T00:00:00"/>
+    <d v="2018-02-11T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF5659"/>
+    <n v="2623"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-12-29T00:00:00"/>
+    <d v="2017-12-17T00:00:00"/>
+    <d v="2017-12-29T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF6102"/>
+    <n v="3440"/>
+    <n v="12"/>
+    <n v="2017"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2018-01-11T00:00:00"/>
+    <d v="2017-12-20T00:00:00"/>
+    <d v="2018-01-11T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF8162"/>
+    <n v="3993"/>
+    <n v="1"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2018-02-20T00:00:00"/>
+    <d v="2017-12-21T00:00:00"/>
+    <d v="2018-02-17T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4573"/>
+    <n v="3273"/>
+    <n v="2"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-12-25T00:00:00"/>
+    <d v="2017-12-25T00:00:00"/>
+    <d v="2017-12-25T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF8503"/>
+    <n v="4494"/>
+    <n v="12"/>
+    <n v="2017"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2018-01-24T00:00:00"/>
+    <d v="2017-12-27T00:00:00"/>
+    <d v="2018-01-24T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF3380"/>
+    <n v="2511"/>
+    <n v="1"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2017-12-29T00:00:00"/>
+    <d v="2017-12-29T00:00:00"/>
+    <d v="2017-12-29T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF6566"/>
+    <n v="2015"/>
+    <n v="12"/>
+    <n v="2017"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2017-12-31T00:00:00"/>
+    <d v="2018-02-20T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF5838"/>
+    <n v="3413"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2018-01-08T00:00:00"/>
+    <d v="2018-01-03T00:00:00"/>
+    <d v="2018-01-08T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF1174"/>
+    <n v="4087"/>
+    <n v="1"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-01-17T00:00:00"/>
+    <d v="2018-01-06T00:00:00"/>
+    <d v="2018-01-17T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF2942"/>
+    <n v="2441"/>
+    <n v="1"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-01-09T00:00:00"/>
+    <d v="2018-01-09T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF8563"/>
+    <n v="3598"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-01-10T00:00:00"/>
+    <d v="2018-01-10T00:00:00"/>
+    <d v="2018-01-10T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF8237"/>
+    <n v="4895"/>
+    <n v="1"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-01-12T00:00:00"/>
+    <d v="2018-01-12T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4859"/>
+    <n v="971"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-02-06T00:00:00"/>
+    <d v="2018-01-13T00:00:00"/>
+    <d v="2018-02-06T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF1529"/>
+    <n v="556"/>
+    <n v="2"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-02-13T00:00:00"/>
+    <d v="2018-01-14T00:00:00"/>
+    <d v="2018-02-13T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF6931"/>
+    <n v="1977"/>
+    <n v="2"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-01-16T00:00:00"/>
+    <d v="2018-01-16T00:00:00"/>
+    <d v="2018-01-16T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7559"/>
+    <n v="2951"/>
+    <n v="1"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-02-02T00:00:00"/>
+    <d v="2018-01-20T00:00:00"/>
+    <d v="2018-01-20T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF9620"/>
+    <n v="2535"/>
+    <n v="2"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-02-10T00:00:00"/>
+    <d v="2018-01-21T00:00:00"/>
+    <d v="2018-02-10T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF4547"/>
+    <n v="3057"/>
+    <n v="2"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-02-09T00:00:00"/>
+    <d v="2018-01-23T00:00:00"/>
+    <d v="2018-02-09T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF6004"/>
+    <n v="3152"/>
+    <n v="2"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-01-25T00:00:00"/>
+    <d v="2018-01-25T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF3415"/>
+    <n v="2247"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-03-19T00:00:00"/>
+    <d v="2018-01-27T00:00:00"/>
+    <d v="2018-01-27T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF1603"/>
+    <n v="2456"/>
+    <n v="3"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-04-25T00:00:00"/>
+    <d v="2018-01-29T00:00:00"/>
+    <d v="2018-01-29T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF8784"/>
+    <n v="3801"/>
+    <n v="4"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-01-31T00:00:00"/>
+    <d v="2018-01-31T00:00:00"/>
+    <d v="2018-01-31T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF1826"/>
+    <n v="3049"/>
+    <n v="1"/>
+    <n v="2018"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-02-04T00:00:00"/>
+    <d v="2018-02-04T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF7390"/>
+    <n v="3255"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-02-05T00:00:00"/>
+    <d v="2018-02-05T00:00:00"/>
+    <d v="2018-02-05T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7009"/>
+    <n v="2074"/>
+    <n v="2"/>
+    <n v="2018"/>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-02-06T00:00:00"/>
+    <d v="2018-02-06T00:00:00"/>
+    <d v="2018-02-06T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7629"/>
+    <n v="3606"/>
+    <n v="2"/>
+    <n v="2018"/>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-03-18T00:00:00"/>
+    <d v="2018-02-07T00:00:00"/>
+    <d v="2018-03-18T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF2748"/>
+    <n v="4867"/>
+    <n v="3"/>
+    <n v="2018"/>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-03-16T00:00:00"/>
+    <d v="2018-02-09T00:00:00"/>
+    <d v="2018-03-16T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF5961"/>
+    <n v="702"/>
+    <n v="3"/>
+    <n v="2018"/>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-02-19T00:00:00"/>
+    <d v="2018-02-14T00:00:00"/>
+    <d v="2018-02-19T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF7680"/>
+    <n v="2801"/>
+    <n v="2"/>
+    <n v="2018"/>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-04-29T00:00:00"/>
+    <d v="2018-02-15T00:00:00"/>
+    <d v="2018-03-10T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF9629"/>
+    <n v="4438"/>
+    <n v="4"/>
+    <n v="2018"/>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-04-08T00:00:00"/>
+    <d v="2018-02-20T00:00:00"/>
+    <d v="2018-04-08T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF5978"/>
+    <n v="3835"/>
+    <n v="4"/>
+    <n v="2018"/>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-03-01T00:00:00"/>
+    <d v="2018-03-01T00:00:00"/>
+    <d v="2018-03-01T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF5651"/>
+    <n v="3893"/>
+    <n v="3"/>
+    <n v="2018"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-03-04T00:00:00"/>
+    <d v="2018-03-04T00:00:00"/>
+    <d v="2018-03-04T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7772"/>
+    <n v="1970"/>
+    <n v="3"/>
+    <n v="2018"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-04-29T00:00:00"/>
+    <d v="2018-03-05T00:00:00"/>
+    <d v="2018-04-29T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF5401"/>
+    <n v="729"/>
+    <n v="4"/>
+    <n v="2018"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-03-29T00:00:00"/>
+    <d v="2018-03-07T00:00:00"/>
+    <d v="2018-03-29T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF9115"/>
+    <n v="474"/>
+    <n v="3"/>
+    <n v="2018"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-03-09T00:00:00"/>
+    <d v="2018-03-09T00:00:00"/>
+    <d v="2018-03-09T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF4115"/>
+    <n v="3164"/>
+    <n v="3"/>
+    <n v="2018"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-03-14T00:00:00"/>
+    <d v="2018-03-14T00:00:00"/>
+    <d v="2018-03-14T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF5683"/>
+    <n v="3113"/>
+    <n v="3"/>
+    <n v="2018"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-04-11T00:00:00"/>
+    <d v="2018-03-17T00:00:00"/>
+    <d v="2018-04-11T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF7027"/>
+    <n v="789"/>
+    <n v="4"/>
+    <n v="2018"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-06-21T00:00:00"/>
+    <d v="2018-03-21T00:00:00"/>
+    <d v="2018-04-01T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF7168"/>
+    <n v="3521"/>
+    <n v="6"/>
+    <n v="2018"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-03-28T00:00:00"/>
+    <d v="2018-03-24T00:00:00"/>
+    <d v="2018-03-28T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4972"/>
+    <n v="4947"/>
+    <n v="3"/>
+    <n v="2018"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-03-25T00:00:00"/>
+    <d v="2018-03-25T00:00:00"/>
+    <d v="2018-03-25T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF7283"/>
+    <n v="1527"/>
+    <n v="3"/>
+    <n v="2018"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-05-14T00:00:00"/>
+    <d v="2018-04-01T00:00:00"/>
+    <d v="2018-05-14T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF6320"/>
+    <n v="764"/>
+    <n v="5"/>
+    <n v="2018"/>
+    <x v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-04-12T00:00:00"/>
+    <d v="2018-04-03T00:00:00"/>
+    <d v="2018-04-12T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF7850"/>
+    <n v="2463"/>
+    <n v="4"/>
+    <n v="2018"/>
+    <x v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-04-05T00:00:00"/>
+    <d v="2018-04-05T00:00:00"/>
+    <d v="2018-04-05T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF2420"/>
+    <n v="2111"/>
+    <n v="4"/>
+    <n v="2018"/>
+    <x v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-04-06T00:00:00"/>
+    <d v="2018-04-06T00:00:00"/>
+    <d v="2018-04-06T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF6764"/>
+    <n v="1144"/>
+    <n v="4"/>
+    <n v="2018"/>
+    <x v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-05-20T00:00:00"/>
+    <d v="2018-04-10T00:00:00"/>
+    <d v="2018-05-20T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF6382"/>
+    <n v="597"/>
+    <n v="5"/>
+    <n v="2018"/>
+    <x v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-04-16T00:00:00"/>
+    <d v="2018-04-16T00:00:00"/>
+    <d v="2018-04-16T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF8079"/>
+    <n v="3445"/>
+    <n v="4"/>
+    <n v="2018"/>
+    <x v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-04-22T00:00:00"/>
+    <d v="2018-05-02T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF2434"/>
+    <n v="1996"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-04-28T00:00:00"/>
+    <d v="2018-04-28T00:00:00"/>
+    <d v="2018-04-28T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF3230"/>
+    <n v="1254"/>
+    <n v="4"/>
+    <n v="2018"/>
+    <x v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-05-03T00:00:00"/>
+    <d v="2018-04-29T00:00:00"/>
+    <d v="2018-05-03T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF8847"/>
+    <n v="905"/>
+    <n v="5"/>
+    <n v="2018"/>
+    <x v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-05-02T00:00:00"/>
+    <d v="2018-05-31T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF8053"/>
+    <n v="2975"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-05-03T00:00:00"/>
+    <d v="2018-05-08T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF2454"/>
+    <n v="4807"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-06-13T00:00:00"/>
+    <d v="2018-05-10T00:00:00"/>
+    <d v="2018-06-13T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF8252"/>
+    <n v="1882"/>
+    <n v="6"/>
+    <n v="2018"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-06-27T00:00:00"/>
+    <d v="2018-05-15T00:00:00"/>
+    <d v="2018-06-27T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF6573"/>
+    <n v="3932"/>
+    <n v="6"/>
+    <n v="2018"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-05-18T00:00:00"/>
+    <d v="2018-05-18T00:00:00"/>
+    <d v="2018-05-18T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF8780"/>
+    <n v="701"/>
+    <n v="5"/>
+    <n v="2018"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-05-19T00:00:00"/>
+    <d v="2018-06-27T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF6166"/>
+    <n v="2651"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-07-01T00:00:00"/>
+    <d v="2018-05-26T00:00:00"/>
+    <d v="2018-07-01T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF8437"/>
+    <n v="3792"/>
+    <n v="7"/>
+    <n v="2018"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-07-25T00:00:00"/>
+    <d v="2018-05-28T00:00:00"/>
+    <d v="2018-07-25T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF6635"/>
+    <n v="611"/>
+    <n v="7"/>
+    <n v="2018"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-07-11T00:00:00"/>
+    <d v="2018-05-31T00:00:00"/>
+    <d v="2018-07-11T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF8734"/>
+    <n v="3431"/>
+    <n v="7"/>
+    <n v="2018"/>
+    <x v="9"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-06-02T00:00:00"/>
+    <d v="2018-06-02T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4208"/>
+    <n v="3670"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-06-08T00:00:00"/>
+    <d v="2018-06-04T00:00:00"/>
+    <d v="2018-06-08T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4923"/>
+    <n v="4320"/>
+    <n v="6"/>
+    <n v="2018"/>
+    <x v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-06-05T00:00:00"/>
+    <d v="2018-06-05T00:00:00"/>
+    <d v="2018-06-05T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF6782"/>
+    <n v="1809"/>
+    <n v="6"/>
+    <n v="2018"/>
+    <x v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-07-25T00:00:00"/>
+    <d v="2018-06-07T00:00:00"/>
+    <d v="2018-07-25T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF6280"/>
+    <n v="667"/>
+    <n v="7"/>
+    <n v="2018"/>
+    <x v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-06-11T00:00:00"/>
+    <d v="2018-06-11T00:00:00"/>
+    <d v="2018-06-11T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF7827"/>
+    <n v="1613"/>
+    <n v="6"/>
+    <n v="2018"/>
+    <x v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-07-28T00:00:00"/>
+    <d v="2018-06-17T00:00:00"/>
+    <d v="2018-07-28T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF5357"/>
+    <n v="3756"/>
+    <n v="7"/>
+    <n v="2018"/>
+    <x v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-06-20T00:00:00"/>
+    <d v="2018-06-20T00:00:00"/>
+    <d v="2018-06-20T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF8188"/>
+    <n v="3672"/>
+    <n v="6"/>
+    <n v="2018"/>
+    <x v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-06-26T00:00:00"/>
+    <d v="2018-07-07T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4640"/>
+    <n v="658"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-08-24T00:00:00"/>
+    <d v="2018-06-29T00:00:00"/>
+    <d v="2018-08-24T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF2293"/>
+    <n v="4762"/>
+    <n v="8"/>
+    <n v="2018"/>
+    <x v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-07-09T00:00:00"/>
+    <d v="2018-07-02T00:00:00"/>
+    <d v="2018-07-09T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF2933"/>
+    <n v="2186"/>
+    <n v="7"/>
+    <n v="2018"/>
+    <x v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-07-03T00:00:00"/>
+    <d v="2018-07-24T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF4384"/>
+    <n v="3411"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-07-24T00:00:00"/>
+    <d v="2018-07-08T00:00:00"/>
+    <d v="2018-07-24T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF8316"/>
+    <n v="2524"/>
+    <n v="7"/>
+    <n v="2018"/>
+    <x v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-08-01T00:00:00"/>
+    <d v="2018-07-10T00:00:00"/>
+    <d v="2018-08-01T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF1506"/>
+    <n v="1709"/>
+    <n v="8"/>
+    <n v="2018"/>
+    <x v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-07-15T00:00:00"/>
+    <d v="2018-07-15T00:00:00"/>
+    <d v="2018-07-15T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4913"/>
+    <n v="3181"/>
+    <n v="7"/>
+    <n v="2018"/>
+    <x v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-09-07T00:00:00"/>
+    <d v="2018-07-16T00:00:00"/>
+    <d v="2018-07-16T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF8526"/>
+    <n v="1108"/>
+    <n v="9"/>
+    <n v="2018"/>
+    <x v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-07-17T00:00:00"/>
+    <d v="2018-07-17T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF9873"/>
+    <n v="2777"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-09-14T00:00:00"/>
+    <d v="2018-07-19T00:00:00"/>
+    <d v="2018-09-14T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF9870"/>
+    <n v="3793"/>
+    <n v="9"/>
+    <n v="2018"/>
+    <x v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-08-12T00:00:00"/>
+    <d v="2018-07-21T00:00:00"/>
+    <d v="2018-08-12T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF5563"/>
+    <n v="4217"/>
+    <n v="8"/>
+    <n v="2018"/>
+    <x v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-07-28T00:00:00"/>
+    <d v="2018-07-28T00:00:00"/>
+    <d v="2018-07-28T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF5510"/>
+    <n v="4850"/>
+    <n v="7"/>
+    <n v="2018"/>
+    <x v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-07-30T00:00:00"/>
+    <d v="2018-07-30T00:00:00"/>
+    <d v="2018-07-30T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF1440"/>
+    <n v="4309"/>
+    <n v="7"/>
+    <n v="2018"/>
+    <x v="11"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-08-02T00:00:00"/>
+    <d v="2018-08-01T00:00:00"/>
+    <d v="2018-08-02T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF2709"/>
+    <n v="4462"/>
+    <n v="8"/>
+    <n v="2018"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-10-02T00:00:00"/>
+    <d v="2018-08-07T00:00:00"/>
+    <d v="2018-10-02T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF9886"/>
+    <n v="4947"/>
+    <n v="10"/>
+    <n v="2018"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-09-25T00:00:00"/>
+    <d v="2018-08-10T00:00:00"/>
+    <d v="2018-09-25T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF6993"/>
+    <n v="902"/>
+    <n v="9"/>
+    <n v="2018"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-09-23T00:00:00"/>
+    <d v="2018-08-12T00:00:00"/>
+    <d v="2018-09-23T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF9126"/>
+    <n v="432"/>
+    <n v="9"/>
+    <n v="2018"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-09-13T00:00:00"/>
+    <d v="2018-08-15T00:00:00"/>
+    <d v="2018-09-13T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF3531"/>
+    <n v="4084"/>
+    <n v="9"/>
+    <n v="2018"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-09-16T00:00:00"/>
+    <d v="2018-08-22T00:00:00"/>
+    <d v="2018-09-16T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF6599"/>
+    <n v="1054"/>
+    <n v="9"/>
+    <n v="2018"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-09-09T00:00:00"/>
+    <d v="2018-08-23T00:00:00"/>
+    <d v="2018-09-09T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF9323"/>
+    <n v="4608"/>
+    <n v="9"/>
+    <n v="2018"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-08-28T00:00:00"/>
+    <d v="2018-08-28T00:00:00"/>
+    <d v="2018-08-28T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF3529"/>
+    <n v="1238"/>
+    <n v="8"/>
+    <n v="2018"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-09-27T00:00:00"/>
+    <d v="2018-09-03T00:00:00"/>
+    <d v="2018-09-27T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF5824"/>
+    <n v="1342"/>
+    <n v="9"/>
+    <n v="2018"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-10-29T00:00:00"/>
+    <d v="2018-09-07T00:00:00"/>
+    <d v="2018-10-29T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF3860"/>
+    <n v="2936"/>
+    <n v="10"/>
+    <n v="2018"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-10-08T00:00:00"/>
+    <d v="2018-09-08T00:00:00"/>
+    <d v="2018-10-08T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7260"/>
+    <n v="875"/>
+    <n v="10"/>
+    <n v="2018"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-09-10T00:00:00"/>
+    <d v="2018-09-10T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF2238"/>
+    <n v="159"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-09-15T00:00:00"/>
+    <d v="2018-09-15T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7342"/>
+    <n v="2933"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-11-01T00:00:00"/>
+    <d v="2018-09-15T00:00:00"/>
+    <d v="2018-11-01T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF8517"/>
+    <n v="4944"/>
+    <n v="11"/>
+    <n v="2018"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-10-04T00:00:00"/>
+    <d v="2018-09-19T00:00:00"/>
+    <d v="2018-10-04T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF9366"/>
+    <n v="4173"/>
+    <n v="10"/>
+    <n v="2018"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-10-02T00:00:00"/>
+    <d v="2018-09-24T00:00:00"/>
+    <d v="2018-10-02T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF4973"/>
+    <n v="2065"/>
+    <n v="10"/>
+    <n v="2018"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-11-18T00:00:00"/>
+    <d v="2018-09-28T00:00:00"/>
+    <d v="2018-11-18T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF1111"/>
+    <n v="521"/>
+    <n v="11"/>
+    <n v="2018"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-10-01T00:00:00"/>
+    <d v="2018-11-13T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF8344"/>
+    <n v="819"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-10-04T00:00:00"/>
+    <d v="2018-10-04T00:00:00"/>
+    <d v="2018-10-04T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF8750"/>
+    <n v="1260"/>
+    <n v="10"/>
+    <n v="2018"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-10-16T00:00:00"/>
+    <d v="2018-10-10T00:00:00"/>
+    <d v="2018-10-16T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF7616"/>
+    <n v="2998"/>
+    <n v="10"/>
+    <n v="2018"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-01-03T00:00:00"/>
+    <d v="2018-10-12T00:00:00"/>
+    <d v="2018-10-31T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF3536"/>
+    <n v="4287"/>
+    <n v="1"/>
+    <n v="2019"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-12-14T00:00:00"/>
+    <d v="2018-10-14T00:00:00"/>
+    <d v="2018-10-14T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF9376"/>
+    <n v="2015"/>
+    <n v="12"/>
+    <n v="2018"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-12-15T00:00:00"/>
+    <d v="2018-10-20T00:00:00"/>
+    <d v="2018-12-15T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF1222"/>
+    <n v="3369"/>
+    <n v="12"/>
+    <n v="2018"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-10-21T00:00:00"/>
+    <d v="2018-10-21T00:00:00"/>
+    <d v="2018-10-21T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF3914"/>
+    <n v="4851"/>
+    <n v="10"/>
+    <n v="2018"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-12-15T00:00:00"/>
+    <d v="2018-10-25T00:00:00"/>
+    <d v="2018-12-15T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7447"/>
+    <n v="2178"/>
+    <n v="12"/>
+    <n v="2018"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-11-20T00:00:00"/>
+    <d v="2018-10-27T00:00:00"/>
+    <d v="2018-11-20T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF5088"/>
+    <n v="4052"/>
+    <n v="11"/>
+    <n v="2018"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-10-30T00:00:00"/>
+    <d v="2018-10-30T00:00:00"/>
+    <d v="2018-10-30T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF7858"/>
+    <n v="2864"/>
+    <n v="10"/>
+    <n v="2018"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-12-27T00:00:00"/>
+    <d v="2018-11-01T00:00:00"/>
+    <d v="2018-12-27T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7692"/>
+    <n v="2425"/>
+    <n v="12"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-01-01T00:00:00"/>
+    <d v="2018-11-03T00:00:00"/>
+    <d v="2019-01-01T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF7390"/>
+    <n v="1542"/>
+    <n v="1"/>
+    <n v="2019"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-12-12T00:00:00"/>
+    <d v="2018-11-08T00:00:00"/>
+    <d v="2018-12-12T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF6262"/>
+    <n v="1736"/>
+    <n v="12"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-01-20T00:00:00"/>
+    <d v="2018-11-11T00:00:00"/>
+    <d v="2019-01-09T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF9573"/>
+    <n v="1628"/>
+    <n v="1"/>
+    <n v="2019"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-11-13T00:00:00"/>
+    <d v="2018-11-13T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF8087"/>
+    <n v="3853"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-12-17T00:00:00"/>
+    <d v="2018-11-17T00:00:00"/>
+    <d v="2018-12-17T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF5909"/>
+    <n v="883"/>
+    <n v="12"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-11-27T00:00:00"/>
+    <d v="2018-11-17T00:00:00"/>
+    <d v="2018-11-17T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4172"/>
+    <n v="976"/>
+    <n v="11"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-11-20T00:00:00"/>
+    <d v="2018-11-20T00:00:00"/>
+    <d v="2018-11-20T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF8957"/>
+    <n v="2663"/>
+    <n v="11"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-11-26T00:00:00"/>
+    <d v="2018-11-26T00:00:00"/>
+    <d v="2018-11-26T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF2981"/>
+    <n v="4888"/>
+    <n v="11"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-11-29T00:00:00"/>
+    <d v="2018-11-29T00:00:00"/>
+    <d v="2018-11-29T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF5104"/>
+    <n v="2030"/>
+    <n v="11"/>
+    <n v="2018"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-01-20T00:00:00"/>
+    <d v="2018-12-02T00:00:00"/>
+    <d v="2019-01-20T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF3942"/>
+    <n v="2117"/>
+    <n v="1"/>
+    <n v="2019"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-01-29T00:00:00"/>
+    <d v="2018-12-04T00:00:00"/>
+    <d v="2019-01-29T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF6376"/>
+    <n v="1236"/>
+    <n v="1"/>
+    <n v="2019"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-12-31T00:00:00"/>
+    <d v="2018-12-09T00:00:00"/>
+    <d v="2018-12-31T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7518"/>
+    <n v="426"/>
+    <n v="12"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-12-10T00:00:00"/>
+    <d v="2018-12-10T00:00:00"/>
+    <d v="2018-12-10T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF5359"/>
+    <n v="3956"/>
+    <n v="12"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2018-12-14T00:00:00"/>
+    <d v="2019-01-15T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF5153"/>
+    <n v="3042"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2018-12-15T00:00:00"/>
+    <d v="2018-12-15T00:00:00"/>
+    <d v="2018-12-15T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF3127"/>
+    <n v="1434"/>
+    <n v="12"/>
+    <n v="2018"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-01-22T00:00:00"/>
+    <d v="2018-12-18T00:00:00"/>
+    <d v="2019-01-22T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF7641"/>
+    <n v="1782"/>
+    <n v="1"/>
+    <n v="2019"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-02-18T00:00:00"/>
+    <d v="2018-12-25T00:00:00"/>
+    <d v="2019-02-18T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF2758"/>
+    <n v="365"/>
+    <n v="2"/>
+    <n v="2019"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-01-26T00:00:00"/>
+    <d v="2018-12-27T00:00:00"/>
+    <d v="2019-01-26T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF9279"/>
+    <n v="2757"/>
+    <n v="1"/>
+    <n v="2019"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-02-19T00:00:00"/>
+    <d v="2018-12-30T00:00:00"/>
+    <d v="2019-02-19T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF2386"/>
+    <n v="2112"/>
+    <n v="2"/>
+    <n v="2019"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2019-01-02T00:00:00"/>
+    <d v="2019-01-02T00:00:00"/>
+    <d v="2019-01-02T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF6751"/>
+    <n v="2190"/>
+    <n v="1"/>
+    <n v="2019"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-01-20T00:00:00"/>
+    <d v="2019-01-04T00:00:00"/>
+    <d v="2019-01-20T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF9460"/>
+    <n v="2998"/>
+    <n v="1"/>
+    <n v="2019"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-02-05T00:00:00"/>
+    <d v="2019-01-11T00:00:00"/>
+    <d v="2019-02-05T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF5556"/>
+    <n v="3808"/>
+    <n v="2"/>
+    <n v="2019"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-04-14T00:00:00"/>
+    <d v="2019-01-14T00:00:00"/>
+    <d v="2019-01-30T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4918"/>
+    <n v="4928"/>
+    <n v="4"/>
+    <n v="2019"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-01-17T00:00:00"/>
+    <d v="2019-01-17T00:00:00"/>
+    <d v="2019-01-17T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF1763"/>
+    <n v="4179"/>
+    <n v="1"/>
+    <n v="2019"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-02-03T00:00:00"/>
+    <d v="2019-01-19T00:00:00"/>
+    <d v="2019-02-03T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF2024"/>
+    <n v="4896"/>
+    <n v="2"/>
+    <n v="2019"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-01-22T00:00:00"/>
+    <d v="2019-01-22T00:00:00"/>
+    <d v="2019-01-22T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF8079"/>
+    <n v="4092"/>
+    <n v="1"/>
+    <n v="2019"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-01-27T00:00:00"/>
+    <d v="2019-01-27T00:00:00"/>
+    <d v="2019-01-27T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF6383"/>
+    <n v="2956"/>
+    <n v="1"/>
+    <n v="2019"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2019-01-31T00:00:00"/>
+    <d v="2019-02-13T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF3919"/>
+    <n v="533"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-02-24T00:00:00"/>
+    <d v="2019-02-01T00:00:00"/>
+    <d v="2019-02-24T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF1390"/>
+    <n v="3519"/>
+    <n v="2"/>
+    <n v="2019"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-02-03T00:00:00"/>
+    <d v="2019-02-03T00:00:00"/>
+    <d v="2019-02-03T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF2500"/>
+    <n v="757"/>
+    <n v="2"/>
+    <n v="2019"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2019-02-07T00:00:00"/>
+    <d v="2019-02-07T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF2427"/>
+    <n v="2688"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-02-09T00:00:00"/>
+    <d v="2019-02-09T00:00:00"/>
+    <d v="2019-02-09T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF4680"/>
+    <n v="340"/>
+    <n v="2"/>
+    <n v="2019"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-02-12T00:00:00"/>
+    <d v="2019-02-10T00:00:00"/>
+    <d v="2019-02-12T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF7019"/>
+    <n v="4204"/>
+    <n v="2"/>
+    <n v="2019"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-03-31T00:00:00"/>
+    <d v="2019-02-12T00:00:00"/>
+    <d v="2019-03-31T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF4961"/>
+    <n v="3695"/>
+    <n v="3"/>
+    <n v="2019"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-02-21T00:00:00"/>
+    <d v="2019-02-21T00:00:00"/>
+    <d v="2019-02-21T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF4608"/>
+    <n v="4148"/>
+    <n v="2"/>
+    <n v="2019"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2019-02-25T00:00:00"/>
+    <d v="2019-02-25T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF1913"/>
+    <n v="4303"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-03-07T00:00:00"/>
+    <d v="2019-02-27T00:00:00"/>
+    <d v="2019-03-07T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF5844"/>
+    <n v="2674"/>
+    <n v="3"/>
+    <n v="2019"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-04-14T00:00:00"/>
+    <d v="2019-03-02T00:00:00"/>
+    <d v="2019-04-14T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF7813"/>
+    <n v="1720"/>
+    <n v="4"/>
+    <n v="2019"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-04-12T00:00:00"/>
+    <d v="2019-03-06T00:00:00"/>
+    <d v="2019-04-12T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF6780"/>
+    <n v="1854"/>
+    <n v="4"/>
+    <n v="2019"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-03-08T00:00:00"/>
+    <d v="2019-03-08T00:00:00"/>
+    <d v="2019-03-08T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF9599"/>
+    <n v="2568"/>
+    <n v="3"/>
+    <n v="2019"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2019-03-08T00:00:00"/>
+    <d v="2019-04-17T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF8659"/>
+    <n v="3690"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-04-15T00:00:00"/>
+    <d v="2019-03-10T00:00:00"/>
+    <d v="2019-04-15T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF4652"/>
+    <n v="3746"/>
+    <n v="4"/>
+    <n v="2019"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-03-12T00:00:00"/>
+    <d v="2019-03-12T00:00:00"/>
+    <d v="2019-03-12T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF3068"/>
+    <n v="4360"/>
+    <n v="3"/>
+    <n v="2019"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-04-21T00:00:00"/>
+    <d v="2019-03-13T00:00:00"/>
+    <d v="2019-04-21T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF7141"/>
+    <n v="1753"/>
+    <n v="4"/>
+    <n v="2019"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-03-19T00:00:00"/>
+    <d v="2019-03-16T00:00:00"/>
+    <d v="2019-03-19T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF3366"/>
+    <n v="1421"/>
+    <n v="3"/>
+    <n v="2019"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-03-19T00:00:00"/>
+    <d v="2019-03-19T00:00:00"/>
+    <d v="2019-03-19T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF8853"/>
+    <n v="3565"/>
+    <n v="3"/>
+    <n v="2019"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-05-01T00:00:00"/>
+    <d v="2019-03-22T00:00:00"/>
+    <d v="2019-05-01T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7681"/>
+    <n v="1961"/>
+    <n v="5"/>
+    <n v="2019"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-03-27T00:00:00"/>
+    <d v="2019-03-27T00:00:00"/>
+    <d v="2019-03-27T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF1441"/>
+    <n v="4854"/>
+    <n v="3"/>
+    <n v="2019"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-04-02T00:00:00"/>
+    <d v="2019-04-02T00:00:00"/>
+    <d v="2019-04-02T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF9964"/>
+    <n v="3453"/>
+    <n v="4"/>
+    <n v="2019"/>
+    <x v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-04-05T00:00:00"/>
+    <d v="2019-04-03T00:00:00"/>
+    <d v="2019-04-05T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF9101"/>
+    <n v="3341"/>
+    <n v="4"/>
+    <n v="2019"/>
+    <x v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2019-04-06T00:00:00"/>
+    <d v="2019-05-20T00:00:00"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="NF3185"/>
+    <n v="2707"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-07-01T00:00:00"/>
+    <d v="2019-04-08T00:00:00"/>
+    <d v="2019-05-18T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF2836"/>
+    <n v="1582"/>
+    <n v="7"/>
+    <n v="2019"/>
+    <x v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-04-23T00:00:00"/>
+    <d v="2019-04-10T00:00:00"/>
+    <d v="2019-04-10T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7779"/>
+    <n v="3889"/>
+    <n v="4"/>
+    <n v="2019"/>
+    <x v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-04-29T00:00:00"/>
+    <d v="2019-04-14T00:00:00"/>
+    <d v="2019-04-29T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF5919"/>
+    <n v="2303"/>
+    <n v="4"/>
+    <n v="2019"/>
+    <x v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-04-17T00:00:00"/>
+    <d v="2019-04-17T00:00:00"/>
+    <d v="2019-04-17T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF1620"/>
+    <n v="802"/>
+    <n v="4"/>
+    <n v="2019"/>
+    <x v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2019-04-19T00:00:00"/>
+    <d v="2019-05-04T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF3801"/>
+    <n v="4513"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-05-01T00:00:00"/>
+    <d v="2019-04-21T00:00:00"/>
+    <d v="2019-05-01T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF8086"/>
+    <n v="3908"/>
+    <n v="5"/>
+    <n v="2019"/>
+    <x v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-07-15T00:00:00"/>
+    <d v="2019-04-25T00:00:00"/>
+    <d v="2019-06-19T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4964"/>
+    <n v="156"/>
+    <n v="7"/>
+    <n v="2019"/>
+    <x v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-06-06T00:00:00"/>
+    <d v="2019-04-27T00:00:00"/>
+    <d v="2019-06-06T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF6112"/>
+    <n v="457"/>
+    <n v="6"/>
+    <n v="2019"/>
+    <x v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-06-08T00:00:00"/>
+    <d v="2019-05-03T00:00:00"/>
+    <d v="2019-06-08T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF2333"/>
+    <n v="3536"/>
+    <n v="6"/>
+    <n v="2019"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-05-10T00:00:00"/>
+    <d v="2019-05-05T00:00:00"/>
+    <d v="2019-05-10T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF7121"/>
+    <n v="1809"/>
+    <n v="5"/>
+    <n v="2019"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-05-28T00:00:00"/>
+    <d v="2019-05-06T00:00:00"/>
+    <d v="2019-05-28T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF8208"/>
+    <n v="4172"/>
+    <n v="5"/>
+    <n v="2019"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-06-07T00:00:00"/>
+    <d v="2019-05-07T00:00:00"/>
+    <d v="2019-06-07T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF1320"/>
+    <n v="3827"/>
+    <n v="6"/>
+    <n v="2019"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-06-29T00:00:00"/>
+    <d v="2019-05-09T00:00:00"/>
+    <d v="2019-06-29T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF9162"/>
+    <n v="1700"/>
+    <n v="6"/>
+    <n v="2019"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-05-29T00:00:00"/>
+    <d v="2019-05-10T00:00:00"/>
+    <d v="2019-05-29T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF1497"/>
+    <n v="2090"/>
+    <n v="5"/>
+    <n v="2019"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-05-13T00:00:00"/>
+    <d v="2019-05-13T00:00:00"/>
+    <d v="2019-05-13T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF8398"/>
+    <n v="3230"/>
+    <n v="5"/>
+    <n v="2019"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-05-16T00:00:00"/>
+    <d v="2019-05-16T00:00:00"/>
+    <d v="2019-05-16T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF1274"/>
+    <n v="4030"/>
+    <n v="5"/>
+    <n v="2019"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-05-19T00:00:00"/>
+    <d v="2019-05-19T00:00:00"/>
+    <d v="2019-05-19T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF1599"/>
+    <n v="1367"/>
+    <n v="5"/>
+    <n v="2019"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-06-10T00:00:00"/>
+    <d v="2019-05-22T00:00:00"/>
+    <d v="2019-06-10T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF6880"/>
+    <n v="3945"/>
+    <n v="6"/>
+    <n v="2019"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-05-25T00:00:00"/>
+    <d v="2019-05-25T00:00:00"/>
+    <d v="2019-05-25T00:00:00"/>
+    <x v="0"/>
+    <x v="4"/>
+    <s v="NF3246"/>
+    <n v="4518"/>
+    <n v="5"/>
+    <n v="2019"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2019-05-29T00:00:00"/>
+    <d v="2019-06-29T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4547"/>
+    <n v="3086"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="9"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-06-12T00:00:00"/>
+    <d v="2019-06-03T00:00:00"/>
+    <d v="2019-06-12T00:00:00"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="NF5900"/>
+    <n v="297"/>
+    <n v="6"/>
+    <n v="2019"/>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-06-23T00:00:00"/>
+    <d v="2019-06-07T00:00:00"/>
+    <d v="2019-06-23T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF2566"/>
+    <n v="3226"/>
+    <n v="6"/>
+    <n v="2019"/>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-06-09T00:00:00"/>
+    <d v="2019-06-09T00:00:00"/>
+    <d v="2019-06-09T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF1823"/>
+    <n v="2338"/>
+    <n v="6"/>
+    <n v="2019"/>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-07-18T00:00:00"/>
+    <d v="2019-06-16T00:00:00"/>
+    <d v="2019-07-18T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF9109"/>
+    <n v="3773"/>
+    <n v="7"/>
+    <n v="2019"/>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v=""/>
+    <d v="2019-06-19T00:00:00"/>
+    <d v="2019-08-09T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF4812"/>
+    <n v="2759"/>
+    <n v="0"/>
+    <n v="0"/>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-06-21T00:00:00"/>
+    <d v="2019-06-21T00:00:00"/>
+    <d v="2019-06-21T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF9082"/>
+    <n v="1425"/>
+    <n v="6"/>
+    <n v="2019"/>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-06-23T00:00:00"/>
+    <d v="2019-06-23T00:00:00"/>
+    <d v="2019-06-23T00:00:00"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="NF3611"/>
+    <n v="332"/>
+    <n v="6"/>
+    <n v="2019"/>
+    <x v="10"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <d v="2019-07-07T00:00:00"/>
+    <d v="2019-06-30T00:00:00"/>
+    <d v="2019-07-07T00:00:00"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="NF4931"/>
+    <n v="2819"/>
     <n v="7"/>
     <n v="2019"/>
     <x v="10"/>
@@ -7909,6 +11115,145 @@
         <item x="4"/>
         <item x="1"/>
         <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="44" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="13">
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="3"/>
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="9"/>
+  </colFields>
+  <colItems count="13">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="10" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Soma de Valor" fld="6" baseField="4" baseItem="2" numFmtId="4"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TdDetalhaDespesa" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B6:O14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="11">
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -8071,10 +11416,60 @@
 </slicerCacheDefinition>
 </file>
 
+<file path=xl/slicerCaches/slicerCache3.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaçãodeDados_Mês_Competência1" sourceName="Mês Competência">
+  <pivotTables>
+    <pivotTable tabId="12" name="TdDetalhaDespesa"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="2">
+      <items count="12">
+        <i x="5" s="1"/>
+        <i x="6" s="1"/>
+        <i x="7" s="1"/>
+        <i x="8" s="1"/>
+        <i x="9" s="1"/>
+        <i x="10" s="1"/>
+        <i x="11" s="1"/>
+        <i x="0" s="1"/>
+        <i x="1" s="1"/>
+        <i x="2" s="1"/>
+        <i x="3" s="1"/>
+        <i x="4" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache4.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaçãodeDados_Ano_Competência1" sourceName="Ano Competência">
+  <pivotTables>
+    <pivotTable tabId="12" name="TdDetalhaDespesa"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="2">
+      <items count="3">
+        <i x="0"/>
+        <i x="1" s="1"/>
+        <i x="2"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <slicer name="Mês Competência" cache="SegmentaçãodeDados_Mês_Competência" caption="Mês Competência" columnCount="6" rowHeight="241300"/>
   <slicer name="Ano Competência" cache="SegmentaçãodeDados_Ano_Competência" caption="Ano Competência" columnCount="2" rowHeight="241300"/>
+</slicers>
+</file>
+
+<file path=xl/slicers/slicer2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <slicer name="Mês Competência 1" cache="SegmentaçãodeDados_Mês_Competência1" caption="Mês Competência" columnCount="6" rowHeight="241300"/>
+  <slicer name="Ano Competência 1" cache="SegmentaçãodeDados_Ano_Competência1" caption="Ano Competência" columnCount="2" rowHeight="241300"/>
 </slicers>
 </file>
 
@@ -8551,7 +11946,7 @@
   <sheetPr codeName="Plan10"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -8968,18 +12363,19 @@
   <sheetPr codeName="Plan11"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="15" width="11.7109375" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
@@ -8994,11 +12390,12 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="1"/>
+      <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="2:14" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -9012,25 +12409,371 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
-    </row>
-    <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="47" t="s">
+        <v>541</v>
+      </c>
+      <c r="C4" s="48">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="47" t="s">
+        <v>545</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="47" t="s">
+        <v>542</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="K7">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <v>11</v>
+      </c>
+      <c r="N7">
+        <v>12</v>
+      </c>
+      <c r="O7" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="50">
+        <v>41773</v>
+      </c>
+      <c r="D8" s="50">
+        <v>25578</v>
+      </c>
+      <c r="E8" s="50">
+        <v>24127</v>
+      </c>
+      <c r="F8" s="50">
+        <v>14679</v>
+      </c>
+      <c r="G8" s="50">
+        <v>24782</v>
+      </c>
+      <c r="H8" s="50">
+        <v>24927</v>
+      </c>
+      <c r="I8" s="50">
+        <v>34065</v>
+      </c>
+      <c r="J8" s="50">
+        <v>21727</v>
+      </c>
+      <c r="K8" s="50">
+        <v>19948</v>
+      </c>
+      <c r="L8" s="50">
+        <v>28693</v>
+      </c>
+      <c r="M8" s="50">
+        <v>22624</v>
+      </c>
+      <c r="N8" s="50">
+        <v>19227</v>
+      </c>
+      <c r="O8" s="50">
+        <v>302150</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="50">
+        <v>3057</v>
+      </c>
+      <c r="D9" s="50">
+        <v>3255</v>
+      </c>
+      <c r="E9" s="50">
+        <v>5837</v>
+      </c>
+      <c r="F9" s="50">
+        <v>2760</v>
+      </c>
+      <c r="G9" s="50">
+        <v>1882</v>
+      </c>
+      <c r="H9" s="50">
+        <v>1613</v>
+      </c>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50">
+        <v>9987</v>
+      </c>
+      <c r="K9" s="50">
+        <v>5001</v>
+      </c>
+      <c r="L9" s="50">
+        <v>10149</v>
+      </c>
+      <c r="M9" s="50">
+        <v>1542</v>
+      </c>
+      <c r="N9" s="50">
+        <v>3956</v>
+      </c>
+      <c r="O9" s="50">
+        <v>49039</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="50">
+        <v>6054</v>
+      </c>
+      <c r="D10" s="50">
+        <v>8702</v>
+      </c>
+      <c r="E10" s="50">
+        <v>474</v>
+      </c>
+      <c r="F10" s="50">
+        <v>2463</v>
+      </c>
+      <c r="G10" s="50">
+        <v>6406</v>
+      </c>
+      <c r="H10" s="50">
+        <v>10243</v>
+      </c>
+      <c r="I10" s="50">
+        <v>14461</v>
+      </c>
+      <c r="J10" s="50">
+        <v>4084</v>
+      </c>
+      <c r="K10" s="50">
+        <v>521</v>
+      </c>
+      <c r="L10" s="50">
+        <v>819</v>
+      </c>
+      <c r="M10" s="50">
+        <v>7204</v>
+      </c>
+      <c r="N10" s="50"/>
+      <c r="O10" s="50">
+        <v>61431</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="49" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="50">
+        <v>2247</v>
+      </c>
+      <c r="D11" s="50">
+        <v>3503</v>
+      </c>
+      <c r="E11" s="50">
+        <v>3893</v>
+      </c>
+      <c r="F11" s="50">
+        <v>4867</v>
+      </c>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50">
+        <v>1108</v>
+      </c>
+      <c r="J11" s="50">
+        <v>4462</v>
+      </c>
+      <c r="K11" s="50">
+        <v>159</v>
+      </c>
+      <c r="L11" s="50">
+        <v>9436</v>
+      </c>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50">
+        <v>29675</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="50">
+        <v>12821</v>
+      </c>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50">
+        <v>4543</v>
+      </c>
+      <c r="H12" s="50">
+        <v>3756</v>
+      </c>
+      <c r="I12" s="50">
+        <v>7688</v>
+      </c>
+      <c r="J12" s="50">
+        <v>2140</v>
+      </c>
+      <c r="K12" s="50">
+        <v>4173</v>
+      </c>
+      <c r="L12" s="50">
+        <v>1260</v>
+      </c>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50">
+        <v>3894</v>
+      </c>
+      <c r="O12" s="50">
+        <v>40275</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="50">
+        <v>17594</v>
+      </c>
+      <c r="D13" s="50">
+        <v>10118</v>
+      </c>
+      <c r="E13" s="50">
+        <v>13923</v>
+      </c>
+      <c r="F13" s="50">
+        <v>4589</v>
+      </c>
+      <c r="G13" s="50">
+        <v>11951</v>
+      </c>
+      <c r="H13" s="50">
+        <v>9315</v>
+      </c>
+      <c r="I13" s="50">
+        <v>10808</v>
+      </c>
+      <c r="J13" s="50">
+        <v>1054</v>
+      </c>
+      <c r="K13" s="50">
+        <v>10094</v>
+      </c>
+      <c r="L13" s="50">
+        <v>7029</v>
+      </c>
+      <c r="M13" s="50">
+        <v>13878</v>
+      </c>
+      <c r="N13" s="50">
+        <v>11377</v>
+      </c>
+      <c r="O13" s="50">
+        <v>121730</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="48" t="s">
+        <v>543</v>
+      </c>
+      <c r="C14" s="50">
+        <v>41773</v>
+      </c>
+      <c r="D14" s="50">
+        <v>25578</v>
+      </c>
+      <c r="E14" s="50">
+        <v>24127</v>
+      </c>
+      <c r="F14" s="50">
+        <v>14679</v>
+      </c>
+      <c r="G14" s="50">
+        <v>24782</v>
+      </c>
+      <c r="H14" s="50">
+        <v>24927</v>
+      </c>
+      <c r="I14" s="50">
+        <v>34065</v>
+      </c>
+      <c r="J14" s="50">
+        <v>21727</v>
+      </c>
+      <c r="K14" s="50">
+        <v>19948</v>
+      </c>
+      <c r="L14" s="50">
+        <v>28693</v>
+      </c>
+      <c r="M14" s="50">
+        <v>22624</v>
+      </c>
+      <c r="N14" s="50">
+        <v>19227</v>
+      </c>
+      <c r="O14" s="50">
+        <v>302150</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -19228,7 +22971,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 22 - Dashboard anual Saldo do caixa
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="879" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="879" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -22,25 +22,25 @@
     <sheet name="ContasReceber" sheetId="14" r:id="rId13"/>
     <sheet name="ContasReceberVencidas" sheetId="15" r:id="rId14"/>
     <sheet name="DashBoardFinanceiroAtual" sheetId="16" r:id="rId15"/>
-    <sheet name="DashBoardFinanceiroAnual" sheetId="18" r:id="rId16"/>
-    <sheet name="DashBoardFinanceiroAnualD" sheetId="19" r:id="rId17"/>
-    <sheet name="DashBoardFinanceiroAtualD" sheetId="20" r:id="rId18"/>
+    <sheet name="DashBoardFinanceiroAtualD" sheetId="20" r:id="rId16"/>
+    <sheet name="DashBoardFinanceiroAnual" sheetId="18" r:id="rId17"/>
+    <sheet name="DashBoardFinanceiroAnualD" sheetId="19" r:id="rId18"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId19"/>
   </externalReferences>
   <definedNames>
-    <definedName name="PCEntradasN1_Nível_1" localSheetId="15">TbPCEntradasN1[Nível 1]</definedName>
+    <definedName name="PCEntradasN1_Nível_1" localSheetId="16">TbPCEntradasN1[Nível 1]</definedName>
     <definedName name="PCEntradasN1_Nível_1">TbPCEntradasN1[Nível 1]</definedName>
-    <definedName name="PCEntradasN2_Nível_1" localSheetId="15">TbPCEntradasN2[Nível 1]</definedName>
+    <definedName name="PCEntradasN2_Nível_1" localSheetId="16">TbPCEntradasN2[Nível 1]</definedName>
     <definedName name="PCEntradasN2_Nível_1">TbPCEntradasN2[Nível 1]</definedName>
-    <definedName name="PCEntradasN2_Nível_2" localSheetId="15">TbPCEntradasN2[Nível 2]</definedName>
+    <definedName name="PCEntradasN2_Nível_2" localSheetId="16">TbPCEntradasN2[Nível 2]</definedName>
     <definedName name="PCEntradasN2_Nível_2">TbPCEntradasN2[Nível 2]</definedName>
-    <definedName name="PCSaídasN1_Nível_1" localSheetId="15">TbPCSaídasN1[Nível 1]</definedName>
+    <definedName name="PCSaídasN1_Nível_1" localSheetId="16">TbPCSaídasN1[Nível 1]</definedName>
     <definedName name="PCSaídasN1_Nível_1">TbPCSaídasN1[Nível 1]</definedName>
-    <definedName name="PCSaídasN2_Nível_1" localSheetId="15">TbPCSaídasN2[Nível 1]</definedName>
+    <definedName name="PCSaídasN2_Nível_1" localSheetId="16">TbPCSaídasN2[Nível 1]</definedName>
     <definedName name="PCSaídasN2_Nível_1">TbPCSaídasN2[Nível 1]</definedName>
-    <definedName name="PCSaídasN2_Nível_2" localSheetId="15">TbPCSaídasN2[Nível 2]</definedName>
+    <definedName name="PCSaídasN2_Nível_2" localSheetId="16">TbPCSaídasN2[Nível 2]</definedName>
     <definedName name="PCSaídasN2_Nível_2">TbPCSaídasN2[Nível 2]</definedName>
     <definedName name="SegmentaçãodeDados_Ano_Competência">#N/A</definedName>
     <definedName name="SegmentaçãodeDados_Ano_Competência1">#N/A</definedName>
@@ -2678,7 +2678,7 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -3079,13 +3079,31 @@
     <xf numFmtId="14" fontId="28" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="28" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -14899,7 +14917,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="36">
   <autoFilter ref="B4:B9"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -14909,7 +14927,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C13" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C13" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34">
   <autoFilter ref="B4:C13"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
@@ -14920,7 +14938,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32">
   <autoFilter ref="B4:B10"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -14930,7 +14948,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C16" totalsRowShown="0" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C16" totalsRowShown="0" headerRowDxfId="31">
   <autoFilter ref="B4:C16"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
@@ -14941,35 +14959,35 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B3:O234" totalsRowShown="0" headerRowDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B3:O234" totalsRowShown="0" headerRowDxfId="30">
   <autoFilter ref="B3:O234"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="27"/>
-    <tableColumn id="2" name="Data da Competência" dataDxfId="26"/>
-    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="25"/>
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="29"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="28"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="27"/>
     <tableColumn id="4" name="Conta Nível 1"/>
     <tableColumn id="5" name="Conta Nível 2"/>
     <tableColumn id="6" name="Histórico"/>
-    <tableColumn id="7" name="Valor" dataDxfId="24"/>
-    <tableColumn id="8" name="Mês Caixa" dataDxfId="23">
+    <tableColumn id="7" name="Valor" dataDxfId="26"/>
+    <tableColumn id="8" name="Mês Caixa" dataDxfId="25">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]="",0,MONTH(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Ano Caixa" dataDxfId="22">
+    <tableColumn id="9" name="Ano Caixa" dataDxfId="24">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]="",0,YEAR(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Mês Competência" dataDxfId="21">
+    <tableColumn id="10" name="Mês Competência" dataDxfId="23">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data da Competência]]="",0,MONTH(TbRegistroEntradas[[#This Row],[Data da Competência]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Ano Competência" dataDxfId="20">
+    <tableColumn id="11" name="Ano Competência" dataDxfId="22">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data da Competência]]="",0,YEAR(TbRegistroEntradas[[#This Row],[Data da Competência]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Mês Previsto" dataDxfId="6">
+    <tableColumn id="12" name="Mês Previsto" dataDxfId="8">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]="",0,MONTH(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Ano Previsto" dataDxfId="5">
+    <tableColumn id="13" name="Ano Previsto" dataDxfId="7">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]="",0,YEAR(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Conta Vencida" dataDxfId="4">
+    <tableColumn id="14" name="Conta Vencida" dataDxfId="6">
       <calculatedColumnFormula>IF(AND(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]&lt;TODAY(),TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]=""),"Vencida","Não Vencida")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -14978,41 +14996,32 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TbRegistroSaídas" displayName="TbRegistroSaídas" ref="B3:N232" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17">
-  <autoFilter ref="B3:N232">
-    <filterColumn colId="0">
-      <filters blank="1"/>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <dateGroupItem year="2018" dateTimeGrouping="year"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TbRegistroSaídas" displayName="TbRegistroSaídas" ref="B3:N232" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19">
+  <autoFilter ref="B3:N232"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="16"/>
-    <tableColumn id="2" name="Data da Competência" dataDxfId="15"/>
-    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="14"/>
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="18"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="17"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="16"/>
     <tableColumn id="4" name="Conta Nível 1"/>
     <tableColumn id="5" name="Conta Nível 2"/>
     <tableColumn id="6" name="Histórico"/>
-    <tableColumn id="7" name="Valor" dataDxfId="13"/>
-    <tableColumn id="8" name="Mês Caixa" dataDxfId="12">
+    <tableColumn id="7" name="Valor" dataDxfId="15"/>
+    <tableColumn id="8" name="Mês Caixa" dataDxfId="14">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data do Caixa Realizado]]="",0,MONTH(TbRegistroSaídas[[#This Row],[Data do Caixa Realizado]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Ano Caixa" dataDxfId="11">
+    <tableColumn id="9" name="Ano Caixa" dataDxfId="13">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data do Caixa Realizado]]="",0,YEAR(TbRegistroSaídas[[#This Row],[Data do Caixa Realizado]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Mês Competência" dataDxfId="10">
+    <tableColumn id="10" name="Mês Competência" dataDxfId="12">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data da Competência]]="",0,MONTH(TbRegistroSaídas[[#This Row],[Data da Competência]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Ano Competência" dataDxfId="9">
+    <tableColumn id="11" name="Ano Competência" dataDxfId="11">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data da Competência]]="",0,YEAR(TbRegistroSaídas[[#This Row],[Data da Competência]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Mês Previsto" dataDxfId="8">
+    <tableColumn id="12" name="Mês Previsto" dataDxfId="10">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data do Caixa Previsto]]="",0,MONTH(TbRegistroSaídas[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Ano Previsto" dataDxfId="7">
+    <tableColumn id="13" name="Ano Previsto" dataDxfId="9">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data do Caixa Previsto]]="",0,YEAR(TbRegistroSaídas[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -15310,9 +15319,7 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17382,7 +17389,7 @@
     <mergeCell ref="F13:G13"/>
   </mergeCells>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17397,9 +17404,842 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L46"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="112"/>
+      <c r="B1" s="113" t="s">
+        <v>603</v>
+      </c>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="113"/>
+      <c r="G1" s="113"/>
+      <c r="H1" s="113"/>
+      <c r="I1" s="113"/>
+      <c r="J1" s="113"/>
+      <c r="K1" s="113"/>
+      <c r="L1" s="113"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="112"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="112"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="114" t="s">
+        <v>565</v>
+      </c>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="114" t="s">
+        <v>566</v>
+      </c>
+      <c r="K3" s="115" t="s">
+        <v>567</v>
+      </c>
+      <c r="L3" s="116"/>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="112"/>
+      <c r="B4" s="115" t="s">
+        <v>568</v>
+      </c>
+      <c r="C4" s="117"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="118" t="s">
+        <v>569</v>
+      </c>
+      <c r="G4" s="119" t="s">
+        <v>570</v>
+      </c>
+      <c r="H4" s="118" t="s">
+        <v>571</v>
+      </c>
+      <c r="I4" s="112"/>
+      <c r="J4" s="120" t="str">
+        <f>[1]DashBoardFinanceiroAtual!K4</f>
+        <v>Livros</v>
+      </c>
+      <c r="K4" s="118" t="s">
+        <v>572</v>
+      </c>
+      <c r="L4" s="118" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="112"/>
+      <c r="B5" s="115" t="s">
+        <v>604</v>
+      </c>
+      <c r="C5" s="145"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="121">
+        <v>1</v>
+      </c>
+      <c r="G5" s="122"/>
+      <c r="H5" s="122"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="122"/>
+      <c r="K5" s="122"/>
+      <c r="L5" s="123" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="112"/>
+      <c r="B6" s="112"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112">
+        <v>2</v>
+      </c>
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="112"/>
+      <c r="J6" s="124"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="115" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="112"/>
+      <c r="B7" s="114" t="s">
+        <v>575</v>
+      </c>
+      <c r="C7" s="112"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="112">
+        <v>3</v>
+      </c>
+      <c r="G7" s="124"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="112"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="115" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="112"/>
+      <c r="B8" s="121" t="s">
+        <v>577</v>
+      </c>
+      <c r="C8" s="125"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112">
+        <v>4</v>
+      </c>
+      <c r="G8" s="124"/>
+      <c r="H8" s="124"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="124"/>
+      <c r="L8" s="115" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="112"/>
+      <c r="B9" s="112" t="s">
+        <v>579</v>
+      </c>
+      <c r="C9" s="126"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="112">
+        <v>5</v>
+      </c>
+      <c r="G9" s="124"/>
+      <c r="H9" s="124"/>
+      <c r="I9" s="112"/>
+      <c r="J9" s="124"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="115" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="112"/>
+      <c r="B10" s="112" t="s">
+        <v>581</v>
+      </c>
+      <c r="C10" s="126"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="112">
+        <v>6</v>
+      </c>
+      <c r="G10" s="124"/>
+      <c r="H10" s="124"/>
+      <c r="I10" s="112"/>
+      <c r="J10" s="124"/>
+      <c r="K10" s="124"/>
+      <c r="L10" s="115" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="112"/>
+      <c r="B11" s="127" t="s">
+        <v>583</v>
+      </c>
+      <c r="C11" s="128"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112">
+        <v>7</v>
+      </c>
+      <c r="G11" s="124"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="112"/>
+      <c r="J11" s="124"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="115" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="112"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="112">
+        <v>8</v>
+      </c>
+      <c r="G12" s="124"/>
+      <c r="H12" s="124"/>
+      <c r="I12" s="112"/>
+      <c r="J12" s="124"/>
+      <c r="K12" s="124"/>
+      <c r="L12" s="115" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="112"/>
+      <c r="B13" s="129" t="s">
+        <v>586</v>
+      </c>
+      <c r="C13" s="129"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112">
+        <v>9</v>
+      </c>
+      <c r="G13" s="124"/>
+      <c r="H13" s="124"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="124"/>
+      <c r="K13" s="124"/>
+      <c r="L13" s="115" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="112"/>
+      <c r="B14" s="130" t="s">
+        <v>588</v>
+      </c>
+      <c r="C14" s="130"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112">
+        <v>10</v>
+      </c>
+      <c r="G14" s="124"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="112"/>
+      <c r="J14" s="124"/>
+      <c r="K14" s="124"/>
+      <c r="L14" s="115" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="112"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112">
+        <v>11</v>
+      </c>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="124"/>
+      <c r="K15" s="124"/>
+      <c r="L15" s="115" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="112"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="112"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="127">
+        <v>12</v>
+      </c>
+      <c r="G16" s="132"/>
+      <c r="H16" s="132"/>
+      <c r="I16" s="112"/>
+      <c r="J16" s="132"/>
+      <c r="K16" s="132"/>
+      <c r="L16" s="133" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="112"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="112"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="112"/>
+      <c r="H17" s="112"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="112"/>
+      <c r="K17" s="112"/>
+      <c r="L17" s="112"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="112"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="112"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="112"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="112"/>
+      <c r="K18" s="112"/>
+      <c r="L18" s="112"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="112"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="112"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="112"/>
+      <c r="F19" s="112"/>
+      <c r="G19" s="112"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="112"/>
+      <c r="K19" s="112"/>
+      <c r="L19" s="112"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="112"/>
+      <c r="B20" s="114" t="s">
+        <v>592</v>
+      </c>
+      <c r="C20" s="112"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="134"/>
+      <c r="F20" s="112"/>
+      <c r="G20" s="112"/>
+      <c r="H20" s="112"/>
+      <c r="I20" s="112"/>
+      <c r="J20" s="112"/>
+      <c r="K20" s="112"/>
+      <c r="L20" s="112"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="112"/>
+      <c r="B21" s="118" t="s">
+        <v>593</v>
+      </c>
+      <c r="C21" s="119" t="s">
+        <v>594</v>
+      </c>
+      <c r="D21" s="119" t="s">
+        <v>595</v>
+      </c>
+      <c r="E21" s="119" t="s">
+        <v>554</v>
+      </c>
+      <c r="F21" s="112"/>
+      <c r="G21" s="112"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="112"/>
+      <c r="L21" s="112"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="112"/>
+      <c r="B22" s="135"/>
+      <c r="C22" s="136"/>
+      <c r="D22" s="136"/>
+      <c r="E22" s="136"/>
+      <c r="F22" s="112"/>
+      <c r="G22" s="112"/>
+      <c r="H22" s="112"/>
+      <c r="I22" s="112"/>
+      <c r="J22" s="112"/>
+      <c r="K22" s="112"/>
+      <c r="L22" s="112"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="112"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="112"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="112"/>
+      <c r="H23" s="112"/>
+      <c r="I23" s="112"/>
+      <c r="J23" s="112"/>
+      <c r="K23" s="112"/>
+      <c r="L23" s="112"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="112"/>
+      <c r="B24" s="112"/>
+      <c r="C24" s="112"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="112"/>
+      <c r="F24" s="112"/>
+      <c r="G24" s="112"/>
+      <c r="H24" s="112"/>
+      <c r="I24" s="112"/>
+      <c r="J24" s="112"/>
+      <c r="K24" s="112"/>
+      <c r="L24" s="112"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="112"/>
+      <c r="B25" s="114" t="s">
+        <v>596</v>
+      </c>
+      <c r="C25" s="112"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="112"/>
+      <c r="F25" s="112"/>
+      <c r="G25" s="114" t="s">
+        <v>597</v>
+      </c>
+      <c r="H25" s="112"/>
+      <c r="I25" s="112"/>
+      <c r="J25" s="112"/>
+      <c r="K25" s="112"/>
+      <c r="L25" s="112"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="112"/>
+      <c r="B26" s="118" t="s">
+        <v>593</v>
+      </c>
+      <c r="C26" s="119" t="s">
+        <v>598</v>
+      </c>
+      <c r="D26" s="119" t="s">
+        <v>562</v>
+      </c>
+      <c r="E26" s="119" t="s">
+        <v>599</v>
+      </c>
+      <c r="F26" s="112"/>
+      <c r="G26" s="118" t="s">
+        <v>593</v>
+      </c>
+      <c r="H26" s="119" t="s">
+        <v>598</v>
+      </c>
+      <c r="I26" s="119" t="s">
+        <v>562</v>
+      </c>
+      <c r="J26" s="119" t="s">
+        <v>599</v>
+      </c>
+      <c r="K26" s="112"/>
+      <c r="L26" s="112"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="112"/>
+      <c r="B27" s="135"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="137"/>
+      <c r="E27" s="137"/>
+      <c r="F27" s="112"/>
+      <c r="G27" s="135"/>
+      <c r="H27" s="137"/>
+      <c r="I27" s="137"/>
+      <c r="J27" s="137"/>
+      <c r="K27" s="112"/>
+      <c r="L27" s="112"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="112"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="112"/>
+      <c r="G28" s="112"/>
+      <c r="H28" s="112"/>
+      <c r="I28" s="112"/>
+      <c r="J28" s="112"/>
+      <c r="K28" s="112"/>
+      <c r="L28" s="112"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="112"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="112"/>
+      <c r="E29" s="112"/>
+      <c r="F29" s="112"/>
+      <c r="G29" s="112"/>
+      <c r="H29" s="112"/>
+      <c r="I29" s="112"/>
+      <c r="J29" s="112"/>
+      <c r="K29" s="112"/>
+      <c r="L29" s="112"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="112"/>
+      <c r="B30" s="114" t="s">
+        <v>600</v>
+      </c>
+      <c r="C30" s="112"/>
+      <c r="D30" s="112"/>
+      <c r="E30" s="112"/>
+      <c r="F30" s="112"/>
+      <c r="G30" s="114" t="s">
+        <v>601</v>
+      </c>
+      <c r="H30" s="138">
+        <f>C4</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="112"/>
+      <c r="J30" s="112"/>
+      <c r="K30" s="112"/>
+      <c r="L30" s="112"/>
+    </row>
+    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="112"/>
+      <c r="B31" s="139" t="s">
+        <v>593</v>
+      </c>
+      <c r="C31" s="123" t="s">
+        <v>579</v>
+      </c>
+      <c r="D31" s="123" t="s">
+        <v>581</v>
+      </c>
+      <c r="E31" s="123" t="s">
+        <v>602</v>
+      </c>
+      <c r="F31" s="112"/>
+      <c r="G31" s="118" t="s">
+        <v>569</v>
+      </c>
+      <c r="H31" s="140" t="str">
+        <f>[1]DashBoardFinanceiroAtual!K14</f>
+        <v>Vestuário</v>
+      </c>
+      <c r="I31" s="112"/>
+      <c r="J31" s="112"/>
+      <c r="K31" s="112"/>
+      <c r="L31" s="112"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="112"/>
+      <c r="B32" s="141"/>
+      <c r="C32" s="142"/>
+      <c r="D32" s="142"/>
+      <c r="E32" s="143"/>
+      <c r="F32" s="112"/>
+      <c r="G32" s="112">
+        <v>1</v>
+      </c>
+      <c r="H32" s="124"/>
+      <c r="I32" s="112"/>
+      <c r="J32" s="112"/>
+      <c r="K32" s="112"/>
+      <c r="L32" s="112"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="112"/>
+      <c r="B33" s="112"/>
+      <c r="C33" s="112"/>
+      <c r="D33" s="112"/>
+      <c r="E33" s="112"/>
+      <c r="F33" s="112"/>
+      <c r="G33" s="112">
+        <v>2</v>
+      </c>
+      <c r="H33" s="124"/>
+      <c r="I33" s="112"/>
+      <c r="J33" s="112"/>
+      <c r="K33" s="112"/>
+      <c r="L33" s="112"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="112"/>
+      <c r="B34" s="112"/>
+      <c r="C34" s="112"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="112">
+        <v>3</v>
+      </c>
+      <c r="H34" s="124"/>
+      <c r="I34" s="112"/>
+      <c r="J34" s="112"/>
+      <c r="K34" s="112"/>
+      <c r="L34" s="112"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="112"/>
+      <c r="B35" s="112"/>
+      <c r="C35" s="112"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="112"/>
+      <c r="F35" s="112"/>
+      <c r="G35" s="112">
+        <v>4</v>
+      </c>
+      <c r="H35" s="124"/>
+      <c r="I35" s="112"/>
+      <c r="J35" s="112"/>
+      <c r="K35" s="112"/>
+      <c r="L35" s="112"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="112"/>
+      <c r="B36" s="112"/>
+      <c r="C36" s="112"/>
+      <c r="D36" s="112"/>
+      <c r="E36" s="112"/>
+      <c r="F36" s="112"/>
+      <c r="G36" s="112">
+        <v>5</v>
+      </c>
+      <c r="H36" s="124"/>
+      <c r="I36" s="112"/>
+      <c r="J36" s="112"/>
+      <c r="K36" s="112"/>
+      <c r="L36" s="112"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="112"/>
+      <c r="B37" s="112"/>
+      <c r="C37" s="112"/>
+      <c r="D37" s="112"/>
+      <c r="E37" s="112"/>
+      <c r="F37" s="112"/>
+      <c r="G37" s="112">
+        <v>6</v>
+      </c>
+      <c r="H37" s="124"/>
+      <c r="I37" s="112"/>
+      <c r="J37" s="112"/>
+      <c r="K37" s="112"/>
+      <c r="L37" s="112"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="112"/>
+      <c r="B38" s="112"/>
+      <c r="C38" s="112"/>
+      <c r="D38" s="112"/>
+      <c r="E38" s="112"/>
+      <c r="F38" s="112"/>
+      <c r="G38" s="112">
+        <v>7</v>
+      </c>
+      <c r="H38" s="124"/>
+      <c r="I38" s="112"/>
+      <c r="J38" s="112"/>
+      <c r="K38" s="112"/>
+      <c r="L38" s="112"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="112"/>
+      <c r="B39" s="112"/>
+      <c r="C39" s="112"/>
+      <c r="D39" s="112"/>
+      <c r="E39" s="112"/>
+      <c r="F39" s="112"/>
+      <c r="G39" s="112">
+        <v>8</v>
+      </c>
+      <c r="H39" s="124"/>
+      <c r="I39" s="112"/>
+      <c r="J39" s="112"/>
+      <c r="K39" s="112"/>
+      <c r="L39" s="112"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="112"/>
+      <c r="B40" s="112"/>
+      <c r="C40" s="112"/>
+      <c r="D40" s="112"/>
+      <c r="E40" s="112"/>
+      <c r="F40" s="112"/>
+      <c r="G40" s="112">
+        <v>9</v>
+      </c>
+      <c r="H40" s="124"/>
+      <c r="I40" s="112"/>
+      <c r="J40" s="112"/>
+      <c r="K40" s="112"/>
+      <c r="L40" s="112"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="112"/>
+      <c r="B41" s="112"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
+      <c r="F41" s="112"/>
+      <c r="G41" s="112">
+        <v>10</v>
+      </c>
+      <c r="H41" s="124"/>
+      <c r="I41" s="112"/>
+      <c r="J41" s="112"/>
+      <c r="K41" s="112"/>
+      <c r="L41" s="112"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="112"/>
+      <c r="B42" s="112"/>
+      <c r="C42" s="112"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="112"/>
+      <c r="F42" s="112"/>
+      <c r="G42" s="112">
+        <v>11</v>
+      </c>
+      <c r="H42" s="124"/>
+      <c r="I42" s="112"/>
+      <c r="J42" s="112"/>
+      <c r="K42" s="112"/>
+      <c r="L42" s="112"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="112"/>
+      <c r="B43" s="112"/>
+      <c r="C43" s="112"/>
+      <c r="D43" s="112"/>
+      <c r="E43" s="112"/>
+      <c r="F43" s="112"/>
+      <c r="G43" s="127">
+        <v>12</v>
+      </c>
+      <c r="H43" s="124"/>
+      <c r="I43" s="112"/>
+      <c r="J43" s="112"/>
+      <c r="K43" s="112"/>
+      <c r="L43" s="112"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="112"/>
+      <c r="B44" s="112"/>
+      <c r="C44" s="112"/>
+      <c r="D44" s="112"/>
+      <c r="E44" s="112"/>
+      <c r="F44" s="112"/>
+      <c r="G44" s="118" t="s">
+        <v>554</v>
+      </c>
+      <c r="H44" s="144"/>
+      <c r="I44" s="112"/>
+      <c r="J44" s="112"/>
+      <c r="K44" s="112"/>
+      <c r="L44" s="112"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="112"/>
+      <c r="B45" s="112"/>
+      <c r="C45" s="112"/>
+      <c r="D45" s="112"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="112"/>
+      <c r="G45" s="112"/>
+      <c r="H45" s="112"/>
+      <c r="I45" s="112"/>
+      <c r="J45" s="112"/>
+      <c r="K45" s="112"/>
+      <c r="L45" s="112"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G46" s="112"/>
+      <c r="H46" s="112"/>
+      <c r="I46" s="112"/>
+      <c r="J46" s="112"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17479,8 +18319,9 @@
       <c r="K4" s="109"/>
     </row>
     <row r="5" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="56">
-        <v>1234</v>
+      <c r="B5" s="147">
+        <f>DashBoardFinanceiroAnualD!$C$11</f>
+        <v>21057</v>
       </c>
       <c r="C5" s="53"/>
       <c r="D5" s="57"/>
@@ -17731,7 +18572,12 @@
     <mergeCell ref="F13:G13"/>
   </mergeCells>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17744,12 +18590,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17823,7 +18669,10 @@
       <c r="B4" s="115" t="s">
         <v>568</v>
       </c>
-      <c r="C4" s="117"/>
+      <c r="C4" s="146">
+        <f>DashBoardFinanceiroAnual!$K$2</f>
+        <v>2019</v>
+      </c>
       <c r="D4" s="112"/>
       <c r="E4" s="112"/>
       <c r="F4" s="118" t="s">
@@ -17908,7 +18757,10 @@
       <c r="B8" s="121" t="s">
         <v>577</v>
       </c>
-      <c r="C8" s="125"/>
+      <c r="C8" s="125">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Ano Caixa],"&lt;"&amp;$C$4,TbRegistroEntradas[Ano Caixa],"&lt;&gt;0")-SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],"&lt;"&amp;$C$4,TbRegistroSaídas[Ano Caixa],"&lt;&gt;0")</f>
+        <v>55108</v>
+      </c>
       <c r="D8" s="112"/>
       <c r="E8" s="112"/>
       <c r="F8" s="112">
@@ -17928,7 +18780,10 @@
       <c r="B9" s="112" t="s">
         <v>579</v>
       </c>
-      <c r="C9" s="126"/>
+      <c r="C9" s="126">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Ano Caixa],"="&amp;$C$4)</f>
+        <v>129286</v>
+      </c>
       <c r="D9" s="112"/>
       <c r="E9" s="112"/>
       <c r="F9" s="112">
@@ -17948,7 +18803,10 @@
       <c r="B10" s="112" t="s">
         <v>581</v>
       </c>
-      <c r="C10" s="126"/>
+      <c r="C10" s="126">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],"="&amp;$C$4)</f>
+        <v>163337</v>
+      </c>
       <c r="D10" s="112"/>
       <c r="E10" s="112"/>
       <c r="F10" s="112">
@@ -17968,7 +18826,10 @@
       <c r="B11" s="127" t="s">
         <v>583</v>
       </c>
-      <c r="C11" s="128"/>
+      <c r="C11" s="128">
+        <f>C8+(C9-C10)</f>
+        <v>21057</v>
+      </c>
       <c r="D11" s="112"/>
       <c r="E11" s="112"/>
       <c r="F11" s="112">
@@ -18564,838 +19425,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="1.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="112"/>
-      <c r="B1" s="113" t="s">
-        <v>603</v>
-      </c>
-      <c r="C1" s="113"/>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="112"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="112"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="114" t="s">
-        <v>565</v>
-      </c>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="114" t="s">
-        <v>566</v>
-      </c>
-      <c r="K3" s="115" t="s">
-        <v>567</v>
-      </c>
-      <c r="L3" s="116"/>
-    </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="112"/>
-      <c r="B4" s="115" t="s">
-        <v>568</v>
-      </c>
-      <c r="C4" s="117"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="118" t="s">
-        <v>569</v>
-      </c>
-      <c r="G4" s="119" t="s">
-        <v>570</v>
-      </c>
-      <c r="H4" s="118" t="s">
-        <v>571</v>
-      </c>
-      <c r="I4" s="112"/>
-      <c r="J4" s="120" t="str">
-        <f>[1]DashBoardFinanceiroAtual!K4</f>
-        <v>Livros</v>
-      </c>
-      <c r="K4" s="118" t="s">
-        <v>572</v>
-      </c>
-      <c r="L4" s="118" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="112"/>
-      <c r="B5" s="115" t="s">
-        <v>604</v>
-      </c>
-      <c r="C5" s="145"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="121">
-        <v>1</v>
-      </c>
-      <c r="G5" s="122"/>
-      <c r="H5" s="122"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="122"/>
-      <c r="K5" s="122"/>
-      <c r="L5" s="123" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="112"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112">
-        <v>2</v>
-      </c>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="112"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="124"/>
-      <c r="L6" s="115" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="112"/>
-      <c r="B7" s="114" t="s">
-        <v>575</v>
-      </c>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112">
-        <v>3</v>
-      </c>
-      <c r="G7" s="124"/>
-      <c r="H7" s="124"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="124"/>
-      <c r="L7" s="115" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="112"/>
-      <c r="B8" s="121" t="s">
-        <v>577</v>
-      </c>
-      <c r="C8" s="125"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112">
-        <v>4</v>
-      </c>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="124"/>
-      <c r="L8" s="115" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="112"/>
-      <c r="B9" s="112" t="s">
-        <v>579</v>
-      </c>
-      <c r="C9" s="126"/>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112">
-        <v>5</v>
-      </c>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="112"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="115" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="112"/>
-      <c r="B10" s="112" t="s">
-        <v>581</v>
-      </c>
-      <c r="C10" s="126"/>
-      <c r="D10" s="112"/>
-      <c r="E10" s="112"/>
-      <c r="F10" s="112">
-        <v>6</v>
-      </c>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="112"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
-      <c r="L10" s="115" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="112"/>
-      <c r="B11" s="127" t="s">
-        <v>583</v>
-      </c>
-      <c r="C11" s="128"/>
-      <c r="D11" s="112"/>
-      <c r="E11" s="112"/>
-      <c r="F11" s="112">
-        <v>7</v>
-      </c>
-      <c r="G11" s="124"/>
-      <c r="H11" s="124"/>
-      <c r="I11" s="112"/>
-      <c r="J11" s="124"/>
-      <c r="K11" s="124"/>
-      <c r="L11" s="115" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="112"/>
-      <c r="B12" s="112"/>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="112"/>
-      <c r="F12" s="112">
-        <v>8</v>
-      </c>
-      <c r="G12" s="124"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="112"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="124"/>
-      <c r="L12" s="115" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="112"/>
-      <c r="B13" s="129" t="s">
-        <v>586</v>
-      </c>
-      <c r="C13" s="129"/>
-      <c r="D13" s="125"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="112">
-        <v>9</v>
-      </c>
-      <c r="G13" s="124"/>
-      <c r="H13" s="124"/>
-      <c r="I13" s="112"/>
-      <c r="J13" s="124"/>
-      <c r="K13" s="124"/>
-      <c r="L13" s="115" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="112"/>
-      <c r="B14" s="130" t="s">
-        <v>588</v>
-      </c>
-      <c r="C14" s="130"/>
-      <c r="D14" s="131"/>
-      <c r="E14" s="112"/>
-      <c r="F14" s="112">
-        <v>10</v>
-      </c>
-      <c r="G14" s="124"/>
-      <c r="H14" s="124"/>
-      <c r="I14" s="112"/>
-      <c r="J14" s="124"/>
-      <c r="K14" s="124"/>
-      <c r="L14" s="115" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="112"/>
-      <c r="B15" s="112"/>
-      <c r="C15" s="112"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="112"/>
-      <c r="F15" s="112">
-        <v>11</v>
-      </c>
-      <c r="G15" s="124"/>
-      <c r="H15" s="124"/>
-      <c r="I15" s="112"/>
-      <c r="J15" s="124"/>
-      <c r="K15" s="124"/>
-      <c r="L15" s="115" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="112"/>
-      <c r="B16" s="112"/>
-      <c r="C16" s="112"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="112"/>
-      <c r="F16" s="127">
-        <v>12</v>
-      </c>
-      <c r="G16" s="132"/>
-      <c r="H16" s="132"/>
-      <c r="I16" s="112"/>
-      <c r="J16" s="132"/>
-      <c r="K16" s="132"/>
-      <c r="L16" s="133" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="112"/>
-      <c r="B17" s="112"/>
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="112"/>
-      <c r="I17" s="112"/>
-      <c r="J17" s="112"/>
-      <c r="K17" s="112"/>
-      <c r="L17" s="112"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="112"/>
-      <c r="B18" s="112"/>
-      <c r="C18" s="112"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="112"/>
-      <c r="I18" s="112"/>
-      <c r="J18" s="112"/>
-      <c r="K18" s="112"/>
-      <c r="L18" s="112"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="112"/>
-      <c r="B19" s="112"/>
-      <c r="C19" s="112"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="112"/>
-      <c r="F19" s="112"/>
-      <c r="G19" s="112"/>
-      <c r="H19" s="112"/>
-      <c r="I19" s="112"/>
-      <c r="J19" s="112"/>
-      <c r="K19" s="112"/>
-      <c r="L19" s="112"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="112"/>
-      <c r="B20" s="114" t="s">
-        <v>592</v>
-      </c>
-      <c r="C20" s="112"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="134"/>
-      <c r="F20" s="112"/>
-      <c r="G20" s="112"/>
-      <c r="H20" s="112"/>
-      <c r="I20" s="112"/>
-      <c r="J20" s="112"/>
-      <c r="K20" s="112"/>
-      <c r="L20" s="112"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="112"/>
-      <c r="B21" s="118" t="s">
-        <v>593</v>
-      </c>
-      <c r="C21" s="119" t="s">
-        <v>594</v>
-      </c>
-      <c r="D21" s="119" t="s">
-        <v>595</v>
-      </c>
-      <c r="E21" s="119" t="s">
-        <v>554</v>
-      </c>
-      <c r="F21" s="112"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="112"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="112"/>
-      <c r="K21" s="112"/>
-      <c r="L21" s="112"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="112"/>
-      <c r="B22" s="135"/>
-      <c r="C22" s="136"/>
-      <c r="D22" s="136"/>
-      <c r="E22" s="136"/>
-      <c r="F22" s="112"/>
-      <c r="G22" s="112"/>
-      <c r="H22" s="112"/>
-      <c r="I22" s="112"/>
-      <c r="J22" s="112"/>
-      <c r="K22" s="112"/>
-      <c r="L22" s="112"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="112"/>
-      <c r="B23" s="112"/>
-      <c r="C23" s="112"/>
-      <c r="D23" s="112"/>
-      <c r="E23" s="112"/>
-      <c r="F23" s="112"/>
-      <c r="G23" s="112"/>
-      <c r="H23" s="112"/>
-      <c r="I23" s="112"/>
-      <c r="J23" s="112"/>
-      <c r="K23" s="112"/>
-      <c r="L23" s="112"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="112"/>
-      <c r="B24" s="112"/>
-      <c r="C24" s="112"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="112"/>
-      <c r="F24" s="112"/>
-      <c r="G24" s="112"/>
-      <c r="H24" s="112"/>
-      <c r="I24" s="112"/>
-      <c r="J24" s="112"/>
-      <c r="K24" s="112"/>
-      <c r="L24" s="112"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="112"/>
-      <c r="B25" s="114" t="s">
-        <v>596</v>
-      </c>
-      <c r="C25" s="112"/>
-      <c r="D25" s="112"/>
-      <c r="E25" s="112"/>
-      <c r="F25" s="112"/>
-      <c r="G25" s="114" t="s">
-        <v>597</v>
-      </c>
-      <c r="H25" s="112"/>
-      <c r="I25" s="112"/>
-      <c r="J25" s="112"/>
-      <c r="K25" s="112"/>
-      <c r="L25" s="112"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="112"/>
-      <c r="B26" s="118" t="s">
-        <v>593</v>
-      </c>
-      <c r="C26" s="119" t="s">
-        <v>598</v>
-      </c>
-      <c r="D26" s="119" t="s">
-        <v>562</v>
-      </c>
-      <c r="E26" s="119" t="s">
-        <v>599</v>
-      </c>
-      <c r="F26" s="112"/>
-      <c r="G26" s="118" t="s">
-        <v>593</v>
-      </c>
-      <c r="H26" s="119" t="s">
-        <v>598</v>
-      </c>
-      <c r="I26" s="119" t="s">
-        <v>562</v>
-      </c>
-      <c r="J26" s="119" t="s">
-        <v>599</v>
-      </c>
-      <c r="K26" s="112"/>
-      <c r="L26" s="112"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="112"/>
-      <c r="B27" s="135"/>
-      <c r="C27" s="137"/>
-      <c r="D27" s="137"/>
-      <c r="E27" s="137"/>
-      <c r="F27" s="112"/>
-      <c r="G27" s="135"/>
-      <c r="H27" s="137"/>
-      <c r="I27" s="137"/>
-      <c r="J27" s="137"/>
-      <c r="K27" s="112"/>
-      <c r="L27" s="112"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="112"/>
-      <c r="B28" s="112"/>
-      <c r="C28" s="112"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="112"/>
-      <c r="F28" s="112"/>
-      <c r="G28" s="112"/>
-      <c r="H28" s="112"/>
-      <c r="I28" s="112"/>
-      <c r="J28" s="112"/>
-      <c r="K28" s="112"/>
-      <c r="L28" s="112"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="112"/>
-      <c r="B29" s="112"/>
-      <c r="C29" s="112"/>
-      <c r="D29" s="112"/>
-      <c r="E29" s="112"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="112"/>
-      <c r="H29" s="112"/>
-      <c r="I29" s="112"/>
-      <c r="J29" s="112"/>
-      <c r="K29" s="112"/>
-      <c r="L29" s="112"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="112"/>
-      <c r="B30" s="114" t="s">
-        <v>600</v>
-      </c>
-      <c r="C30" s="112"/>
-      <c r="D30" s="112"/>
-      <c r="E30" s="112"/>
-      <c r="F30" s="112"/>
-      <c r="G30" s="114" t="s">
-        <v>601</v>
-      </c>
-      <c r="H30" s="138">
-        <f>C4</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="112"/>
-      <c r="J30" s="112"/>
-      <c r="K30" s="112"/>
-      <c r="L30" s="112"/>
-    </row>
-    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="112"/>
-      <c r="B31" s="139" t="s">
-        <v>593</v>
-      </c>
-      <c r="C31" s="123" t="s">
-        <v>579</v>
-      </c>
-      <c r="D31" s="123" t="s">
-        <v>581</v>
-      </c>
-      <c r="E31" s="123" t="s">
-        <v>602</v>
-      </c>
-      <c r="F31" s="112"/>
-      <c r="G31" s="118" t="s">
-        <v>569</v>
-      </c>
-      <c r="H31" s="140" t="str">
-        <f>[1]DashBoardFinanceiroAtual!K14</f>
-        <v>Vestuário</v>
-      </c>
-      <c r="I31" s="112"/>
-      <c r="J31" s="112"/>
-      <c r="K31" s="112"/>
-      <c r="L31" s="112"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="112"/>
-      <c r="B32" s="141"/>
-      <c r="C32" s="142"/>
-      <c r="D32" s="142"/>
-      <c r="E32" s="143"/>
-      <c r="F32" s="112"/>
-      <c r="G32" s="112">
-        <v>1</v>
-      </c>
-      <c r="H32" s="124"/>
-      <c r="I32" s="112"/>
-      <c r="J32" s="112"/>
-      <c r="K32" s="112"/>
-      <c r="L32" s="112"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="112"/>
-      <c r="B33" s="112"/>
-      <c r="C33" s="112"/>
-      <c r="D33" s="112"/>
-      <c r="E33" s="112"/>
-      <c r="F33" s="112"/>
-      <c r="G33" s="112">
-        <v>2</v>
-      </c>
-      <c r="H33" s="124"/>
-      <c r="I33" s="112"/>
-      <c r="J33" s="112"/>
-      <c r="K33" s="112"/>
-      <c r="L33" s="112"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="112"/>
-      <c r="B34" s="112"/>
-      <c r="C34" s="112"/>
-      <c r="D34" s="112"/>
-      <c r="E34" s="112"/>
-      <c r="F34" s="112"/>
-      <c r="G34" s="112">
-        <v>3</v>
-      </c>
-      <c r="H34" s="124"/>
-      <c r="I34" s="112"/>
-      <c r="J34" s="112"/>
-      <c r="K34" s="112"/>
-      <c r="L34" s="112"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="112"/>
-      <c r="B35" s="112"/>
-      <c r="C35" s="112"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="112"/>
-      <c r="F35" s="112"/>
-      <c r="G35" s="112">
-        <v>4</v>
-      </c>
-      <c r="H35" s="124"/>
-      <c r="I35" s="112"/>
-      <c r="J35" s="112"/>
-      <c r="K35" s="112"/>
-      <c r="L35" s="112"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="112"/>
-      <c r="B36" s="112"/>
-      <c r="C36" s="112"/>
-      <c r="D36" s="112"/>
-      <c r="E36" s="112"/>
-      <c r="F36" s="112"/>
-      <c r="G36" s="112">
-        <v>5</v>
-      </c>
-      <c r="H36" s="124"/>
-      <c r="I36" s="112"/>
-      <c r="J36" s="112"/>
-      <c r="K36" s="112"/>
-      <c r="L36" s="112"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="112"/>
-      <c r="B37" s="112"/>
-      <c r="C37" s="112"/>
-      <c r="D37" s="112"/>
-      <c r="E37" s="112"/>
-      <c r="F37" s="112"/>
-      <c r="G37" s="112">
-        <v>6</v>
-      </c>
-      <c r="H37" s="124"/>
-      <c r="I37" s="112"/>
-      <c r="J37" s="112"/>
-      <c r="K37" s="112"/>
-      <c r="L37" s="112"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="112"/>
-      <c r="B38" s="112"/>
-      <c r="C38" s="112"/>
-      <c r="D38" s="112"/>
-      <c r="E38" s="112"/>
-      <c r="F38" s="112"/>
-      <c r="G38" s="112">
-        <v>7</v>
-      </c>
-      <c r="H38" s="124"/>
-      <c r="I38" s="112"/>
-      <c r="J38" s="112"/>
-      <c r="K38" s="112"/>
-      <c r="L38" s="112"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="112"/>
-      <c r="B39" s="112"/>
-      <c r="C39" s="112"/>
-      <c r="D39" s="112"/>
-      <c r="E39" s="112"/>
-      <c r="F39" s="112"/>
-      <c r="G39" s="112">
-        <v>8</v>
-      </c>
-      <c r="H39" s="124"/>
-      <c r="I39" s="112"/>
-      <c r="J39" s="112"/>
-      <c r="K39" s="112"/>
-      <c r="L39" s="112"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="112"/>
-      <c r="B40" s="112"/>
-      <c r="C40" s="112"/>
-      <c r="D40" s="112"/>
-      <c r="E40" s="112"/>
-      <c r="F40" s="112"/>
-      <c r="G40" s="112">
-        <v>9</v>
-      </c>
-      <c r="H40" s="124"/>
-      <c r="I40" s="112"/>
-      <c r="J40" s="112"/>
-      <c r="K40" s="112"/>
-      <c r="L40" s="112"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="112"/>
-      <c r="B41" s="112"/>
-      <c r="C41" s="112"/>
-      <c r="D41" s="112"/>
-      <c r="E41" s="112"/>
-      <c r="F41" s="112"/>
-      <c r="G41" s="112">
-        <v>10</v>
-      </c>
-      <c r="H41" s="124"/>
-      <c r="I41" s="112"/>
-      <c r="J41" s="112"/>
-      <c r="K41" s="112"/>
-      <c r="L41" s="112"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="112"/>
-      <c r="B42" s="112"/>
-      <c r="C42" s="112"/>
-      <c r="D42" s="112"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="112"/>
-      <c r="G42" s="112">
-        <v>11</v>
-      </c>
-      <c r="H42" s="124"/>
-      <c r="I42" s="112"/>
-      <c r="J42" s="112"/>
-      <c r="K42" s="112"/>
-      <c r="L42" s="112"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="112"/>
-      <c r="B43" s="112"/>
-      <c r="C43" s="112"/>
-      <c r="D43" s="112"/>
-      <c r="E43" s="112"/>
-      <c r="F43" s="112"/>
-      <c r="G43" s="127">
-        <v>12</v>
-      </c>
-      <c r="H43" s="124"/>
-      <c r="I43" s="112"/>
-      <c r="J43" s="112"/>
-      <c r="K43" s="112"/>
-      <c r="L43" s="112"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" s="112"/>
-      <c r="B44" s="112"/>
-      <c r="C44" s="112"/>
-      <c r="D44" s="112"/>
-      <c r="E44" s="112"/>
-      <c r="F44" s="112"/>
-      <c r="G44" s="118" t="s">
-        <v>554</v>
-      </c>
-      <c r="H44" s="144"/>
-      <c r="I44" s="112"/>
-      <c r="J44" s="112"/>
-      <c r="K44" s="112"/>
-      <c r="L44" s="112"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="112"/>
-      <c r="B45" s="112"/>
-      <c r="C45" s="112"/>
-      <c r="D45" s="112"/>
-      <c r="E45" s="112"/>
-      <c r="F45" s="112"/>
-      <c r="G45" s="112"/>
-      <c r="H45" s="112"/>
-      <c r="I45" s="112"/>
-      <c r="J45" s="112"/>
-      <c r="K45" s="112"/>
-      <c r="L45" s="112"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G46" s="112"/>
-      <c r="H46" s="112"/>
-      <c r="I46" s="112"/>
-      <c r="J46" s="112"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20131,8 +20161,8 @@
   <dimension ref="B1:O234"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="3" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H135" sqref="H135:H234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32022,9 +32052,9 @@
   <sheetPr codeName="Plan8"/>
   <dimension ref="B1:N232"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H47" sqref="H47:H157"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H232" sqref="H3:H232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32108,7 +32138,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="4" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13">
         <v>43015</v>
       </c>
@@ -32155,7 +32185,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13">
         <v>42995</v>
       </c>
@@ -32202,7 +32232,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13">
         <v>42983</v>
       </c>
@@ -32249,7 +32279,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="7" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13">
         <v>43004</v>
       </c>
@@ -32296,7 +32326,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="8" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13">
         <v>43002</v>
       </c>
@@ -32343,7 +32373,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13">
         <v>42980</v>
       </c>
@@ -32390,7 +32420,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13">
         <v>43014</v>
       </c>
@@ -32437,7 +32467,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13">
         <v>42990</v>
       </c>
@@ -32484,7 +32514,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="12" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13">
         <v>42987</v>
       </c>
@@ -32531,7 +32561,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="13" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>69</v>
       </c>
@@ -32578,7 +32608,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="14" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
         <v>69</v>
       </c>
@@ -32625,7 +32655,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="15" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="13">
         <v>42991</v>
       </c>
@@ -32672,7 +32702,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="16" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="13">
         <v>42992</v>
       </c>
@@ -32719,7 +32749,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="17" spans="2:14" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="13">
         <v>43004</v>
       </c>
@@ -32766,7 +32796,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="18" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="13">
         <v>43043</v>
       </c>
@@ -32813,7 +32843,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="19" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="13" t="s">
         <v>69</v>
       </c>
@@ -32860,7 +32890,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="13">
         <v>43010</v>
       </c>
@@ -32907,7 +32937,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="21" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="13">
         <v>43042</v>
       </c>
@@ -32954,7 +32984,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="22" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="13">
         <v>43009</v>
       </c>
@@ -33001,7 +33031,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="23" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="13">
         <v>43030</v>
       </c>
@@ -33048,7 +33078,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="24" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="13">
         <v>43031</v>
       </c>
@@ -33095,7 +33125,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="25" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="13">
         <v>43046</v>
       </c>
@@ -33142,7 +33172,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="26" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" s="13">
         <v>43022</v>
       </c>
@@ -33189,7 +33219,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="27" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" s="13">
         <v>43031</v>
       </c>
@@ -33236,7 +33266,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="28" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="13">
         <v>43026</v>
       </c>
@@ -33283,7 +33313,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="29" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="13">
         <v>43065</v>
       </c>
@@ -33330,7 +33360,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="30" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="13">
         <v>43071</v>
       </c>
@@ -33377,7 +33407,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="31" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="13">
         <v>43089</v>
       </c>
@@ -33424,7 +33454,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="32" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="13">
         <v>43044</v>
       </c>
@@ -33471,7 +33501,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="33" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="13">
         <v>43047</v>
       </c>
@@ -33518,7 +33548,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="34" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="13">
         <v>43087</v>
       </c>
@@ -33565,7 +33595,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="35" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="13">
         <v>43095</v>
       </c>
@@ -33612,7 +33642,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="36" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="13">
         <v>43056</v>
       </c>
@@ -33659,7 +33689,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="37" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="13">
         <v>43112</v>
       </c>
@@ -33706,7 +33736,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="38" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="13">
         <v>43101</v>
       </c>
@@ -33753,7 +33783,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="39" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="13">
         <v>43061</v>
       </c>
@@ -33800,7 +33830,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="40" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="13">
         <v>43103</v>
       </c>
@@ -33847,7 +33877,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="41" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="13">
         <v>43070</v>
       </c>
@@ -33894,7 +33924,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="42" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="13">
         <v>43096</v>
       </c>
@@ -33941,7 +33971,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="43" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="13">
         <v>43125</v>
       </c>
@@ -33988,7 +34018,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="44" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" s="13">
         <v>43075</v>
       </c>
@@ -34035,7 +34065,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="45" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" s="13">
         <v>43077</v>
       </c>
@@ -34082,7 +34112,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="46" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B46" s="13">
         <v>43099</v>
       </c>
@@ -34176,7 +34206,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="48" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" s="13">
         <v>43098</v>
       </c>
@@ -34223,7 +34253,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="49" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B49" s="13">
         <v>43111</v>
       </c>
@@ -34270,7 +34300,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="50" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B50" s="13">
         <v>43151</v>
       </c>
@@ -34317,7 +34347,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="51" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51" s="13">
         <v>43094</v>
       </c>
@@ -34364,7 +34394,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="52" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B52" s="13">
         <v>43124</v>
       </c>
@@ -34411,7 +34441,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="53" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53" s="13">
         <v>43098</v>
       </c>
@@ -34505,7 +34535,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="55" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55" s="13">
         <v>43108</v>
       </c>
@@ -34552,7 +34582,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="56" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" s="13">
         <v>43117</v>
       </c>
@@ -34646,7 +34676,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="58" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B58" s="13">
         <v>43110</v>
       </c>
@@ -34740,7 +34770,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="60" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B60" s="13">
         <v>43137</v>
       </c>
@@ -34787,7 +34817,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="61" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" s="13">
         <v>43144</v>
       </c>
@@ -34834,7 +34864,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="62" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B62" s="13">
         <v>43116</v>
       </c>
@@ -34881,7 +34911,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="63" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B63" s="13">
         <v>43133</v>
       </c>
@@ -34928,7 +34958,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="64" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B64" s="13">
         <v>43141</v>
       </c>
@@ -34975,7 +35005,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="65" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B65" s="13">
         <v>43140</v>
       </c>
@@ -35069,7 +35099,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="67" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B67" s="13">
         <v>43178</v>
       </c>
@@ -35116,7 +35146,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="68" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B68" s="13">
         <v>43215</v>
       </c>
@@ -35163,7 +35193,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="69" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B69" s="13">
         <v>43131</v>
       </c>
@@ -35257,7 +35287,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="71" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B71" s="13">
         <v>43136</v>
       </c>
@@ -35304,7 +35334,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="72" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B72" s="13">
         <v>43137</v>
       </c>
@@ -35351,7 +35381,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="73" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B73" s="13">
         <v>43177</v>
       </c>
@@ -35398,7 +35428,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="74" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B74" s="13">
         <v>43175</v>
       </c>
@@ -35445,7 +35475,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="75" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B75" s="13">
         <v>43150</v>
       </c>
@@ -35492,7 +35522,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="76" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B76" s="13">
         <v>43219</v>
       </c>
@@ -35539,7 +35569,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="77" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B77" s="13">
         <v>43198</v>
       </c>
@@ -35586,7 +35616,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="78" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B78" s="13">
         <v>43160</v>
       </c>
@@ -35633,7 +35663,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="79" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B79" s="13">
         <v>43163</v>
       </c>
@@ -35680,7 +35710,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="80" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B80" s="13">
         <v>43219</v>
       </c>
@@ -35727,7 +35757,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="81" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B81" s="13">
         <v>43188</v>
       </c>
@@ -35774,7 +35804,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="82" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B82" s="13">
         <v>43168</v>
       </c>
@@ -35821,7 +35851,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="83" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B83" s="13">
         <v>43173</v>
       </c>
@@ -35868,7 +35898,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="84" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B84" s="13">
         <v>43201</v>
       </c>
@@ -35915,7 +35945,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="85" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B85" s="13">
         <v>43272</v>
       </c>
@@ -35962,7 +35992,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="86" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B86" s="13">
         <v>43187</v>
       </c>
@@ -36009,7 +36039,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="87" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B87" s="13">
         <v>43184</v>
       </c>
@@ -36056,7 +36086,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="88" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B88" s="13">
         <v>43234</v>
       </c>
@@ -36103,7 +36133,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="89" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B89" s="13">
         <v>43202</v>
       </c>
@@ -36150,7 +36180,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="90" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B90" s="13">
         <v>43195</v>
       </c>
@@ -36197,7 +36227,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="91" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B91" s="13">
         <v>43196</v>
       </c>
@@ -36244,7 +36274,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="92" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B92" s="13">
         <v>43240</v>
       </c>
@@ -36291,7 +36321,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="93" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B93" s="13">
         <v>43206</v>
       </c>
@@ -36385,7 +36415,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="95" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B95" s="13">
         <v>43218</v>
       </c>
@@ -36432,7 +36462,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="96" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B96" s="13">
         <v>43223</v>
       </c>
@@ -36573,7 +36603,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="99" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B99" s="13">
         <v>43264</v>
       </c>
@@ -36620,7 +36650,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="100" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B100" s="13">
         <v>43278</v>
       </c>
@@ -36667,7 +36697,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="101" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B101" s="13">
         <v>43238</v>
       </c>
@@ -36761,7 +36791,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="103" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B103" s="13">
         <v>43282</v>
       </c>
@@ -36808,7 +36838,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="104" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B104" s="13">
         <v>43306</v>
       </c>
@@ -36855,7 +36885,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="105" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B105" s="13">
         <v>43292</v>
       </c>
@@ -36949,7 +36979,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="107" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B107" s="13">
         <v>43259</v>
       </c>
@@ -36996,7 +37026,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="108" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B108" s="13">
         <v>43256</v>
       </c>
@@ -37043,7 +37073,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="109" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B109" s="13">
         <v>43306</v>
       </c>
@@ -37090,7 +37120,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="110" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B110" s="13">
         <v>43262</v>
       </c>
@@ -37137,7 +37167,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="111" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B111" s="13">
         <v>43309</v>
       </c>
@@ -37184,7 +37214,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="112" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B112" s="13">
         <v>43271</v>
       </c>
@@ -37278,7 +37308,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="114" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B114" s="13">
         <v>43336</v>
       </c>
@@ -37325,7 +37355,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="115" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B115" s="13">
         <v>43290</v>
       </c>
@@ -37419,7 +37449,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="117" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B117" s="13">
         <v>43305</v>
       </c>
@@ -37466,7 +37496,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="118" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B118" s="13">
         <v>43313</v>
       </c>
@@ -37513,7 +37543,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="119" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B119" s="13">
         <v>43296</v>
       </c>
@@ -37560,7 +37590,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="120" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B120" s="13">
         <v>43350</v>
       </c>
@@ -37654,7 +37684,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="122" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B122" s="13">
         <v>43357</v>
       </c>
@@ -37701,7 +37731,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="123" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B123" s="13">
         <v>43324</v>
       </c>
@@ -37748,7 +37778,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="124" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B124" s="13">
         <v>43309</v>
       </c>
@@ -37795,7 +37825,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="125" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B125" s="13">
         <v>43311</v>
       </c>
@@ -37842,7 +37872,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="126" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B126" s="13">
         <v>43314</v>
       </c>
@@ -37889,7 +37919,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="127" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B127" s="13">
         <v>43375</v>
       </c>
@@ -37936,7 +37966,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="128" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B128" s="13">
         <v>43368</v>
       </c>
@@ -37983,7 +38013,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="129" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B129" s="13">
         <v>43366</v>
       </c>
@@ -38030,7 +38060,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="130" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B130" s="13">
         <v>43356</v>
       </c>
@@ -38077,7 +38107,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="131" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B131" s="13">
         <v>43359</v>
       </c>
@@ -38124,7 +38154,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="132" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B132" s="13">
         <v>43352</v>
       </c>
@@ -38171,7 +38201,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="133" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B133" s="13">
         <v>43340</v>
       </c>
@@ -38218,7 +38248,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="134" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B134" s="13">
         <v>43370</v>
       </c>
@@ -38265,7 +38295,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="135" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B135" s="13">
         <v>43402</v>
       </c>
@@ -38312,7 +38342,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="136" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B136" s="13">
         <v>43381</v>
       </c>
@@ -38453,7 +38483,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="139" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B139" s="13">
         <v>43405</v>
       </c>
@@ -38500,7 +38530,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="140" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B140" s="13">
         <v>43377</v>
       </c>
@@ -38547,7 +38577,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="141" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B141" s="13">
         <v>43375</v>
       </c>
@@ -38594,7 +38624,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="142" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B142" s="13">
         <v>43422</v>
       </c>
@@ -38688,7 +38718,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="144" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B144" s="13">
         <v>43377</v>
       </c>
@@ -38735,7 +38765,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="145" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B145" s="13">
         <v>43389</v>
       </c>
@@ -38782,7 +38812,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="146" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B146" s="13">
         <v>43468</v>
       </c>
@@ -38829,7 +38859,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="147" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B147" s="13">
         <v>43448</v>
       </c>
@@ -38876,7 +38906,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="148" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B148" s="13">
         <v>43449</v>
       </c>
@@ -38923,7 +38953,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="149" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B149" s="13">
         <v>43394</v>
       </c>
@@ -38970,7 +39000,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="150" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B150" s="13">
         <v>43449</v>
       </c>
@@ -39017,7 +39047,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="151" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B151" s="13">
         <v>43424</v>
       </c>
@@ -39064,7 +39094,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="152" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B152" s="13">
         <v>43403</v>
       </c>
@@ -39111,7 +39141,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="153" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B153" s="13">
         <v>43461</v>
       </c>
@@ -39158,7 +39188,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="154" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B154" s="13">
         <v>43466</v>
       </c>
@@ -39205,7 +39235,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="155" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B155" s="13">
         <v>43446</v>
       </c>
@@ -39252,7 +39282,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="156" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B156" s="13">
         <v>43485</v>
       </c>
@@ -39346,7 +39376,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="158" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B158" s="13">
         <v>43451</v>
       </c>
@@ -39393,7 +39423,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="159" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B159" s="13">
         <v>43431</v>
       </c>
@@ -39440,7 +39470,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="160" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B160" s="13">
         <v>43424</v>
       </c>
@@ -39487,7 +39517,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="161" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B161" s="13">
         <v>43430</v>
       </c>
@@ -39534,7 +39564,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="162" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B162" s="13">
         <v>43433</v>
       </c>
@@ -39581,7 +39611,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="163" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B163" s="13">
         <v>43485</v>
       </c>
@@ -39628,7 +39658,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="164" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B164" s="13">
         <v>43494</v>
       </c>
@@ -39675,7 +39705,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="165" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B165" s="13">
         <v>43465</v>
       </c>
@@ -39722,7 +39752,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="166" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B166" s="13">
         <v>43444</v>
       </c>
@@ -39769,7 +39799,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="167" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B167" s="13" t="s">
         <v>69</v>
       </c>
@@ -39816,7 +39846,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="168" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B168" s="13">
         <v>43449</v>
       </c>
@@ -39863,7 +39893,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="169" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B169" s="13">
         <v>43487</v>
       </c>
@@ -39910,7 +39940,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="170" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B170" s="13">
         <v>43514</v>
       </c>
@@ -39957,7 +39987,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="171" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B171" s="13">
         <v>43491</v>
       </c>
@@ -40004,7 +40034,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="172" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B172" s="13">
         <v>43515</v>
       </c>
@@ -40051,7 +40081,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="173" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B173" s="13">
         <v>43467</v>
       </c>
@@ -40098,7 +40128,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="174" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B174" s="13">
         <v>43485</v>
       </c>
@@ -40145,7 +40175,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="175" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B175" s="13">
         <v>43501</v>
       </c>
@@ -40192,7 +40222,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="176" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B176" s="13">
         <v>43569</v>
       </c>
@@ -40239,7 +40269,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="177" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B177" s="13">
         <v>43482</v>
       </c>
@@ -40286,7 +40316,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="178" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B178" s="13">
         <v>43499</v>
       </c>
@@ -40333,7 +40363,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="179" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B179" s="13">
         <v>43487</v>
       </c>
@@ -40380,7 +40410,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="180" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B180" s="13">
         <v>43492</v>
       </c>
@@ -40427,7 +40457,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="181" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B181" s="13" t="s">
         <v>69</v>
       </c>
@@ -40474,7 +40504,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="182" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B182" s="13">
         <v>43520</v>
       </c>
@@ -40521,7 +40551,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="183" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B183" s="13">
         <v>43499</v>
       </c>
@@ -40568,7 +40598,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="184" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B184" s="13" t="s">
         <v>69</v>
       </c>
@@ -40615,7 +40645,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="185" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B185" s="13">
         <v>43505</v>
       </c>
@@ -40662,7 +40692,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="186" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B186" s="13">
         <v>43508</v>
       </c>
@@ -40709,7 +40739,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="187" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B187" s="13">
         <v>43555</v>
       </c>
@@ -40756,7 +40786,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="188" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B188" s="13">
         <v>43517</v>
       </c>
@@ -40803,7 +40833,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="189" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B189" s="13" t="s">
         <v>69</v>
       </c>
@@ -40850,7 +40880,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="190" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B190" s="13">
         <v>43531</v>
       </c>
@@ -40897,7 +40927,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="191" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B191" s="13">
         <v>43569</v>
       </c>
@@ -40944,7 +40974,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="192" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B192" s="13">
         <v>43567</v>
       </c>
@@ -40991,7 +41021,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="193" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B193" s="13">
         <v>43532</v>
       </c>
@@ -41038,7 +41068,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="194" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B194" s="13" t="s">
         <v>69</v>
       </c>
@@ -41085,7 +41115,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="195" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B195" s="13">
         <v>43570</v>
       </c>
@@ -41132,7 +41162,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="196" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B196" s="13">
         <v>43536</v>
       </c>
@@ -41179,7 +41209,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="197" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B197" s="13">
         <v>43576</v>
       </c>
@@ -41226,7 +41256,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="198" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B198" s="13">
         <v>43543</v>
       </c>
@@ -41273,7 +41303,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="199" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B199" s="13">
         <v>43543</v>
       </c>
@@ -41320,7 +41350,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="200" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B200" s="13">
         <v>43586</v>
       </c>
@@ -41367,7 +41397,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="201" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B201" s="13">
         <v>43551</v>
       </c>
@@ -41414,7 +41444,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="202" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B202" s="13">
         <v>43557</v>
       </c>
@@ -41461,7 +41491,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="203" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B203" s="13">
         <v>43560</v>
       </c>
@@ -41508,7 +41538,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="204" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B204" s="13" t="s">
         <v>69</v>
       </c>
@@ -41555,7 +41585,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="205" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B205" s="13">
         <v>43647</v>
       </c>
@@ -41602,7 +41632,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="206" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B206" s="13">
         <v>43578</v>
       </c>
@@ -41649,7 +41679,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="207" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B207" s="13">
         <v>43584</v>
       </c>
@@ -41696,7 +41726,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="208" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B208" s="13">
         <v>43572</v>
       </c>
@@ -41743,7 +41773,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="209" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B209" s="13" t="s">
         <v>69</v>
       </c>
@@ -41790,7 +41820,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="210" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B210" s="13">
         <v>43586</v>
       </c>
@@ -41837,7 +41867,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="211" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B211" s="13">
         <v>43661</v>
       </c>
@@ -41884,7 +41914,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="212" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B212" s="13">
         <v>43622</v>
       </c>
@@ -41931,7 +41961,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="213" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B213" s="13">
         <v>43624</v>
       </c>
@@ -41978,7 +42008,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="214" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B214" s="13">
         <v>43595</v>
       </c>
@@ -42025,7 +42055,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="215" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B215" s="13">
         <v>43613</v>
       </c>
@@ -42072,7 +42102,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="216" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B216" s="13">
         <v>43623</v>
       </c>
@@ -42119,7 +42149,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="217" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B217" s="13">
         <v>43645</v>
       </c>
@@ -42166,7 +42196,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="218" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B218" s="13">
         <v>43614</v>
       </c>
@@ -42213,7 +42243,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="219" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B219" s="13">
         <v>43598</v>
       </c>
@@ -42260,7 +42290,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="220" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B220" s="13">
         <v>43601</v>
       </c>
@@ -42307,7 +42337,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="221" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B221" s="13">
         <v>43604</v>
       </c>
@@ -42354,7 +42384,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="222" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B222" s="13">
         <v>43626</v>
       </c>
@@ -42401,7 +42431,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="223" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B223" s="13">
         <v>43610</v>
       </c>
@@ -42448,7 +42478,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="224" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B224" s="13" t="s">
         <v>69</v>
       </c>
@@ -42495,7 +42525,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="225" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B225" s="13">
         <v>43628</v>
       </c>
@@ -42542,7 +42572,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="226" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B226" s="13">
         <v>43639</v>
       </c>
@@ -42589,7 +42619,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="227" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B227" s="13">
         <v>43625</v>
       </c>
@@ -42636,7 +42666,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="228" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B228" s="13">
         <v>43664</v>
       </c>
@@ -42683,7 +42713,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="229" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B229" s="13" t="s">
         <v>69</v>
       </c>
@@ -42730,7 +42760,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="230" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B230" s="13">
         <v>43637</v>
       </c>
@@ -42777,7 +42807,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="231" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B231" s="13">
         <v>43639</v>
       </c>
@@ -42824,7 +42854,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="232" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B232" s="13">
         <v>43653</v>
       </c>
@@ -42893,8 +42923,8 @@
   <sheetPr codeName="Plan9"/>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42945,7 +42975,7 @@
         <v>511</v>
       </c>
       <c r="C3" s="24">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -43064,51 +43094,51 @@
       </c>
       <c r="C8" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Ano Caixa],"&lt;"&amp;$C$3,TbRegistroEntradas[Ano Caixa],"&lt;&gt;0")-SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],"&lt;"&amp;$C$3,TbRegistroSaídas[Ano Caixa],"&lt;&gt;0")</f>
-        <v>-1041</v>
+        <v>55108</v>
       </c>
       <c r="D8" s="35">
         <f>C11</f>
-        <v>966</v>
+        <v>40555</v>
       </c>
       <c r="E8" s="35">
         <f t="shared" ref="E8:N8" si="0">D11</f>
-        <v>5553</v>
+        <v>41511</v>
       </c>
       <c r="F8" s="35">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>53246</v>
       </c>
       <c r="G8" s="35">
         <f t="shared" si="0"/>
-        <v>1894</v>
+        <v>39267</v>
       </c>
       <c r="H8" s="35">
         <f t="shared" si="0"/>
-        <v>22181</v>
+        <v>28688</v>
       </c>
       <c r="I8" s="35">
         <f t="shared" si="0"/>
-        <v>30931</v>
+        <v>19950</v>
       </c>
       <c r="J8" s="35">
         <f t="shared" si="0"/>
-        <v>22856</v>
+        <v>16469</v>
       </c>
       <c r="K8" s="35">
         <f t="shared" si="0"/>
-        <v>38235</v>
+        <v>19070</v>
       </c>
       <c r="L8" s="35">
         <f t="shared" si="0"/>
-        <v>44941</v>
+        <v>20549</v>
       </c>
       <c r="M8" s="35">
         <f t="shared" si="0"/>
-        <v>39552</v>
+        <v>21057</v>
       </c>
       <c r="N8" s="36">
         <f t="shared" si="0"/>
-        <v>58456</v>
+        <v>21057</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -43117,51 +43147,51 @@
       </c>
       <c r="C9" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Caixa],C5,TbRegistroEntradas[Ano Caixa],$C$3)</f>
-        <v>33220</v>
+        <v>17211</v>
       </c>
       <c r="D9" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Caixa],D5,TbRegistroEntradas[Ano Caixa],$C$3)</f>
-        <v>27618</v>
+        <v>25105</v>
       </c>
       <c r="E9" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Caixa],E5,TbRegistroEntradas[Ano Caixa],$C$3)</f>
-        <v>21553</v>
+        <v>34872</v>
       </c>
       <c r="F9" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Caixa],F5,TbRegistroEntradas[Ano Caixa],$C$3)</f>
-        <v>25910</v>
+        <v>13810</v>
       </c>
       <c r="G9" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Caixa],G5,TbRegistroEntradas[Ano Caixa],$C$3)</f>
-        <v>23254</v>
+        <v>16506</v>
       </c>
       <c r="H9" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Caixa],H5,TbRegistroEntradas[Ano Caixa],$C$3)</f>
-        <v>29499</v>
+        <v>12345</v>
       </c>
       <c r="I9" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Caixa],I5,TbRegistroEntradas[Ano Caixa],$C$3)</f>
-        <v>21232</v>
+        <v>4849</v>
       </c>
       <c r="J9" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Caixa],J5,TbRegistroEntradas[Ano Caixa],$C$3)</f>
-        <v>31767</v>
+        <v>2601</v>
       </c>
       <c r="K9" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Caixa],K5,TbRegistroEntradas[Ano Caixa],$C$3)</f>
-        <v>24029</v>
+        <v>1479</v>
       </c>
       <c r="L9" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Caixa],L5,TbRegistroEntradas[Ano Caixa],$C$3)</f>
-        <v>21580</v>
+        <v>508</v>
       </c>
       <c r="M9" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Caixa],M5,TbRegistroEntradas[Ano Caixa],$C$3)</f>
-        <v>38978</v>
+        <v>0</v>
       </c>
       <c r="N9" s="36">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Caixa],N5,TbRegistroEntradas[Ano Caixa],$C$3)</f>
-        <v>15074</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -43170,51 +43200,51 @@
       </c>
       <c r="C10" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Caixa],C5,TbRegistroSaídas[Ano Caixa],$C$3)</f>
-        <v>31213</v>
+        <v>31764</v>
       </c>
       <c r="D10" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Caixa],D5,TbRegistroSaídas[Ano Caixa],$C$3)</f>
-        <v>23031</v>
+        <v>24149</v>
       </c>
       <c r="E10" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Caixa],E5,TbRegistroSaídas[Ano Caixa],$C$3)</f>
-        <v>27113</v>
+        <v>23137</v>
       </c>
       <c r="F10" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Caixa],F5,TbRegistroSaídas[Ano Caixa],$C$3)</f>
-        <v>24009</v>
+        <v>27789</v>
       </c>
       <c r="G10" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Caixa],G5,TbRegistroSaídas[Ano Caixa],$C$3)</f>
-        <v>2967</v>
+        <v>27085</v>
       </c>
       <c r="H10" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Caixa],H5,TbRegistroSaídas[Ano Caixa],$C$3)</f>
-        <v>20749</v>
+        <v>21083</v>
       </c>
       <c r="I10" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Caixa],I5,TbRegistroSaídas[Ano Caixa],$C$3)</f>
-        <v>29307</v>
+        <v>8330</v>
       </c>
       <c r="J10" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Caixa],J5,TbRegistroSaídas[Ano Caixa],$C$3)</f>
-        <v>16388</v>
+        <v>0</v>
       </c>
       <c r="K10" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Caixa],K5,TbRegistroSaídas[Ano Caixa],$C$3)</f>
-        <v>17323</v>
+        <v>0</v>
       </c>
       <c r="L10" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Caixa],L5,TbRegistroSaídas[Ano Caixa],$C$3)</f>
-        <v>26969</v>
+        <v>0</v>
       </c>
       <c r="M10" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Caixa],M5,TbRegistroSaídas[Ano Caixa],$C$3)</f>
-        <v>20074</v>
+        <v>0</v>
       </c>
       <c r="N10" s="36">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Caixa],N5,TbRegistroSaídas[Ano Caixa],$C$3)</f>
-        <v>18422</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -43223,51 +43253,51 @@
       </c>
       <c r="C11" s="37">
         <f>C8+C9-C10</f>
-        <v>966</v>
+        <v>40555</v>
       </c>
       <c r="D11" s="37">
         <f t="shared" ref="D11:N11" si="1">D8+D9-D10</f>
-        <v>5553</v>
+        <v>41511</v>
       </c>
       <c r="E11" s="37">
         <f t="shared" si="1"/>
-        <v>-7</v>
+        <v>53246</v>
       </c>
       <c r="F11" s="37">
         <f t="shared" si="1"/>
-        <v>1894</v>
+        <v>39267</v>
       </c>
       <c r="G11" s="37">
         <f t="shared" si="1"/>
-        <v>22181</v>
+        <v>28688</v>
       </c>
       <c r="H11" s="37">
         <f t="shared" si="1"/>
-        <v>30931</v>
+        <v>19950</v>
       </c>
       <c r="I11" s="37">
         <f t="shared" si="1"/>
-        <v>22856</v>
+        <v>16469</v>
       </c>
       <c r="J11" s="37">
         <f t="shared" si="1"/>
-        <v>38235</v>
+        <v>19070</v>
       </c>
       <c r="K11" s="37">
         <f t="shared" si="1"/>
-        <v>44941</v>
+        <v>20549</v>
       </c>
       <c r="L11" s="37">
         <f t="shared" si="1"/>
-        <v>39552</v>
+        <v>21057</v>
       </c>
       <c r="M11" s="37">
         <f t="shared" si="1"/>
-        <v>58456</v>
+        <v>21057</v>
       </c>
       <c r="N11" s="38">
         <f t="shared" si="1"/>
-        <v>55108</v>
+        <v>21057</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -43323,51 +43353,51 @@
       </c>
       <c r="C15" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Ano Competência],"&lt;"&amp;$C$3,TbRegistroEntradas[Ano Competência],"&lt;&gt;0")-SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Competência],"&lt;"&amp;$C$3,TbRegistroSaídas[Ano Competência],"&lt;&gt;0")</f>
-        <v>23943</v>
+        <v>42367</v>
       </c>
       <c r="D15" s="35">
         <f>C18</f>
-        <v>2752</v>
+        <v>34684</v>
       </c>
       <c r="E15" s="35">
         <f t="shared" ref="E15:N15" si="2">D18</f>
-        <v>1935</v>
+        <v>40111</v>
       </c>
       <c r="F15" s="35">
         <f t="shared" si="2"/>
-        <v>15266</v>
+        <v>27220</v>
       </c>
       <c r="G15" s="35">
         <f t="shared" si="2"/>
-        <v>30813</v>
+        <v>23048</v>
       </c>
       <c r="H15" s="35">
         <f t="shared" si="2"/>
-        <v>25040</v>
+        <v>8340</v>
       </c>
       <c r="I15" s="35">
         <f t="shared" si="2"/>
-        <v>28824</v>
+        <v>3236</v>
       </c>
       <c r="J15" s="35">
         <f t="shared" si="2"/>
-        <v>28057</v>
+        <v>3236</v>
       </c>
       <c r="K15" s="35">
         <f t="shared" si="2"/>
-        <v>28632</v>
+        <v>3236</v>
       </c>
       <c r="L15" s="35">
         <f t="shared" si="2"/>
-        <v>34708</v>
+        <v>3236</v>
       </c>
       <c r="M15" s="35">
         <f t="shared" si="2"/>
-        <v>35415</v>
+        <v>3236</v>
       </c>
       <c r="N15" s="36">
         <f t="shared" si="2"/>
-        <v>43688</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -43376,51 +43406,51 @@
       </c>
       <c r="C16" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Competência],C5,TbRegistroEntradas[Ano Competência],$C$3)</f>
-        <v>20582</v>
+        <v>22897</v>
       </c>
       <c r="D16" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Competência],D5,TbRegistroEntradas[Ano Competência],$C$3)</f>
-        <v>24761</v>
+        <v>31755</v>
       </c>
       <c r="E16" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Competência],E5,TbRegistroEntradas[Ano Competência],$C$3)</f>
-        <v>37458</v>
+        <v>18601</v>
       </c>
       <c r="F16" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Competência],F5,TbRegistroEntradas[Ano Competência],$C$3)</f>
-        <v>30226</v>
+        <v>22939</v>
       </c>
       <c r="G16" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Competência],G5,TbRegistroEntradas[Ano Competência],$C$3)</f>
-        <v>19009</v>
+        <v>22602</v>
       </c>
       <c r="H16" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Competência],H5,TbRegistroEntradas[Ano Competência],$C$3)</f>
-        <v>28711</v>
+        <v>11865</v>
       </c>
       <c r="I16" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Competência],I5,TbRegistroEntradas[Ano Competência],$C$3)</f>
-        <v>33298</v>
+        <v>0</v>
       </c>
       <c r="J16" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Competência],J5,TbRegistroEntradas[Ano Competência],$C$3)</f>
-        <v>22302</v>
+        <v>0</v>
       </c>
       <c r="K16" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Competência],K5,TbRegistroEntradas[Ano Competência],$C$3)</f>
-        <v>26024</v>
+        <v>0</v>
       </c>
       <c r="L16" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Competência],L5,TbRegistroEntradas[Ano Competência],$C$3)</f>
-        <v>29400</v>
+        <v>0</v>
       </c>
       <c r="M16" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Competência],M5,TbRegistroEntradas[Ano Competência],$C$3)</f>
-        <v>30897</v>
+        <v>0</v>
       </c>
       <c r="N16" s="35">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Competência],N5,TbRegistroEntradas[Ano Competência],$C$3)</f>
-        <v>17906</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -43429,51 +43459,51 @@
       </c>
       <c r="C17" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Competência],C5,TbRegistroSaídas[Ano Competência],$C$3)</f>
-        <v>41773</v>
+        <v>30580</v>
       </c>
       <c r="D17" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Competência],D5,TbRegistroSaídas[Ano Competência],$C$3)</f>
-        <v>25578</v>
+        <v>26328</v>
       </c>
       <c r="E17" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Competência],E5,TbRegistroSaídas[Ano Competência],$C$3)</f>
-        <v>24127</v>
+        <v>31492</v>
       </c>
       <c r="F17" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Competência],F5,TbRegistroSaídas[Ano Competência],$C$3)</f>
-        <v>14679</v>
+        <v>27111</v>
       </c>
       <c r="G17" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Competência],G5,TbRegistroSaídas[Ano Competência],$C$3)</f>
-        <v>24782</v>
+        <v>37310</v>
       </c>
       <c r="H17" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Competência],H5,TbRegistroSaídas[Ano Competência],$C$3)</f>
-        <v>24927</v>
+        <v>16969</v>
       </c>
       <c r="I17" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Competência],I5,TbRegistroSaídas[Ano Competência],$C$3)</f>
-        <v>34065</v>
+        <v>0</v>
       </c>
       <c r="J17" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Competência],J5,TbRegistroSaídas[Ano Competência],$C$3)</f>
-        <v>21727</v>
+        <v>0</v>
       </c>
       <c r="K17" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Competência],K5,TbRegistroSaídas[Ano Competência],$C$3)</f>
-        <v>19948</v>
+        <v>0</v>
       </c>
       <c r="L17" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Competência],L5,TbRegistroSaídas[Ano Competência],$C$3)</f>
-        <v>28693</v>
+        <v>0</v>
       </c>
       <c r="M17" s="35">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Competência],M5,TbRegistroSaídas[Ano Competência],$C$3)</f>
-        <v>22624</v>
+        <v>0</v>
       </c>
       <c r="N17" s="36">
         <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Competência],N5,TbRegistroSaídas[Ano Competência],$C$3)</f>
-        <v>19227</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -43482,51 +43512,51 @@
       </c>
       <c r="C18" s="37">
         <f>C15+C16-C17</f>
-        <v>2752</v>
+        <v>34684</v>
       </c>
       <c r="D18" s="37">
         <f t="shared" ref="D18:N18" si="3">D15+D16-D17</f>
-        <v>1935</v>
+        <v>40111</v>
       </c>
       <c r="E18" s="37">
         <f t="shared" si="3"/>
-        <v>15266</v>
+        <v>27220</v>
       </c>
       <c r="F18" s="37">
         <f t="shared" si="3"/>
-        <v>30813</v>
+        <v>23048</v>
       </c>
       <c r="G18" s="37">
         <f t="shared" si="3"/>
-        <v>25040</v>
+        <v>8340</v>
       </c>
       <c r="H18" s="37">
         <f t="shared" si="3"/>
-        <v>28824</v>
+        <v>3236</v>
       </c>
       <c r="I18" s="37">
         <f t="shared" si="3"/>
-        <v>28057</v>
+        <v>3236</v>
       </c>
       <c r="J18" s="37">
         <f t="shared" si="3"/>
-        <v>28632</v>
+        <v>3236</v>
       </c>
       <c r="K18" s="37">
         <f t="shared" si="3"/>
-        <v>34708</v>
+        <v>3236</v>
       </c>
       <c r="L18" s="37">
         <f t="shared" si="3"/>
-        <v>35415</v>
+        <v>3236</v>
       </c>
       <c r="M18" s="37">
         <f t="shared" si="3"/>
-        <v>43688</v>
+        <v>3236</v>
       </c>
       <c r="N18" s="38">
         <f t="shared" si="3"/>
-        <v>42367</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -43582,51 +43612,51 @@
       </c>
       <c r="C22" s="35">
         <f>C16</f>
-        <v>20582</v>
+        <v>22897</v>
       </c>
       <c r="D22" s="35">
         <f t="shared" ref="D22:N22" si="4">D16</f>
-        <v>24761</v>
+        <v>31755</v>
       </c>
       <c r="E22" s="35">
         <f t="shared" si="4"/>
-        <v>37458</v>
+        <v>18601</v>
       </c>
       <c r="F22" s="35">
         <f t="shared" si="4"/>
-        <v>30226</v>
+        <v>22939</v>
       </c>
       <c r="G22" s="35">
         <f t="shared" si="4"/>
-        <v>19009</v>
+        <v>22602</v>
       </c>
       <c r="H22" s="35">
         <f t="shared" si="4"/>
-        <v>28711</v>
+        <v>11865</v>
       </c>
       <c r="I22" s="35">
         <f t="shared" si="4"/>
-        <v>33298</v>
+        <v>0</v>
       </c>
       <c r="J22" s="35">
         <f t="shared" si="4"/>
-        <v>22302</v>
+        <v>0</v>
       </c>
       <c r="K22" s="35">
         <f t="shared" si="4"/>
-        <v>26024</v>
+        <v>0</v>
       </c>
       <c r="L22" s="35">
         <f t="shared" si="4"/>
-        <v>29400</v>
+        <v>0</v>
       </c>
       <c r="M22" s="35">
         <f t="shared" si="4"/>
-        <v>30897</v>
+        <v>0</v>
       </c>
       <c r="N22" s="36">
         <f t="shared" si="4"/>
-        <v>17906</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -43635,51 +43665,51 @@
       </c>
       <c r="C23" s="35">
         <f>C17</f>
-        <v>41773</v>
+        <v>30580</v>
       </c>
       <c r="D23" s="35">
         <f t="shared" ref="D23:N23" si="5">D17</f>
-        <v>25578</v>
+        <v>26328</v>
       </c>
       <c r="E23" s="35">
         <f t="shared" si="5"/>
-        <v>24127</v>
+        <v>31492</v>
       </c>
       <c r="F23" s="35">
         <f t="shared" si="5"/>
-        <v>14679</v>
+        <v>27111</v>
       </c>
       <c r="G23" s="35">
         <f t="shared" si="5"/>
-        <v>24782</v>
+        <v>37310</v>
       </c>
       <c r="H23" s="35">
         <f t="shared" si="5"/>
-        <v>24927</v>
+        <v>16969</v>
       </c>
       <c r="I23" s="35">
         <f t="shared" si="5"/>
-        <v>34065</v>
+        <v>0</v>
       </c>
       <c r="J23" s="35">
         <f t="shared" si="5"/>
-        <v>21727</v>
+        <v>0</v>
       </c>
       <c r="K23" s="35">
         <f t="shared" si="5"/>
-        <v>19948</v>
+        <v>0</v>
       </c>
       <c r="L23" s="35">
         <f t="shared" si="5"/>
-        <v>28693</v>
+        <v>0</v>
       </c>
       <c r="M23" s="35">
         <f t="shared" si="5"/>
-        <v>22624</v>
+        <v>0</v>
       </c>
       <c r="N23" s="36">
         <f t="shared" si="5"/>
-        <v>19227</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -43692,15 +43722,15 @@
       </c>
       <c r="D24" s="39">
         <f t="shared" ref="D24:N24" si="6">IF(D22-D23&gt;0,D22-D23,0)</f>
-        <v>0</v>
+        <v>5427</v>
       </c>
       <c r="E24" s="39">
         <f t="shared" si="6"/>
-        <v>13331</v>
+        <v>0</v>
       </c>
       <c r="F24" s="39">
         <f t="shared" si="6"/>
-        <v>15547</v>
+        <v>0</v>
       </c>
       <c r="G24" s="39">
         <f t="shared" si="6"/>
@@ -43708,7 +43738,7 @@
       </c>
       <c r="H24" s="39">
         <f t="shared" si="6"/>
-        <v>3784</v>
+        <v>0</v>
       </c>
       <c r="I24" s="39">
         <f t="shared" si="6"/>
@@ -43716,19 +43746,19 @@
       </c>
       <c r="J24" s="39">
         <f t="shared" si="6"/>
-        <v>575</v>
+        <v>0</v>
       </c>
       <c r="K24" s="39">
         <f t="shared" si="6"/>
-        <v>6076</v>
+        <v>0</v>
       </c>
       <c r="L24" s="39">
         <f t="shared" si="6"/>
-        <v>707</v>
+        <v>0</v>
       </c>
       <c r="M24" s="39">
         <f t="shared" si="6"/>
-        <v>8273</v>
+        <v>0</v>
       </c>
       <c r="N24" s="40">
         <f t="shared" si="6"/>
@@ -43741,31 +43771,31 @@
       </c>
       <c r="C25" s="41">
         <f>IF(C22-C23&lt;0,C22-C23,0)</f>
-        <v>-21191</v>
+        <v>-7683</v>
       </c>
       <c r="D25" s="41">
         <f t="shared" ref="D25:N25" si="7">IF(D22-D23&lt;0,D22-D23,0)</f>
-        <v>-817</v>
+        <v>0</v>
       </c>
       <c r="E25" s="41">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-12891</v>
       </c>
       <c r="F25" s="41">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-4172</v>
       </c>
       <c r="G25" s="41">
         <f t="shared" si="7"/>
-        <v>-5773</v>
+        <v>-14708</v>
       </c>
       <c r="H25" s="41">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-5104</v>
       </c>
       <c r="I25" s="41">
         <f t="shared" si="7"/>
-        <v>-767</v>
+        <v>0</v>
       </c>
       <c r="J25" s="41">
         <f t="shared" si="7"/>
@@ -43785,7 +43815,7 @@
       </c>
       <c r="N25" s="42">
         <f t="shared" si="7"/>
-        <v>-1321</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -43794,51 +43824,51 @@
       </c>
       <c r="C26" s="41">
         <f>C22-C23</f>
-        <v>-21191</v>
+        <v>-7683</v>
       </c>
       <c r="D26" s="41">
         <f>C26+(D22-D23)</f>
-        <v>-22008</v>
+        <v>-2256</v>
       </c>
       <c r="E26" s="41">
         <f t="shared" ref="E26:N26" si="8">D26+(E22-E23)</f>
-        <v>-8677</v>
+        <v>-15147</v>
       </c>
       <c r="F26" s="41">
         <f t="shared" si="8"/>
-        <v>6870</v>
+        <v>-19319</v>
       </c>
       <c r="G26" s="41">
         <f t="shared" si="8"/>
-        <v>1097</v>
+        <v>-34027</v>
       </c>
       <c r="H26" s="41">
         <f t="shared" si="8"/>
-        <v>4881</v>
+        <v>-39131</v>
       </c>
       <c r="I26" s="41">
         <f t="shared" si="8"/>
-        <v>4114</v>
+        <v>-39131</v>
       </c>
       <c r="J26" s="41">
         <f t="shared" si="8"/>
-        <v>4689</v>
+        <v>-39131</v>
       </c>
       <c r="K26" s="41">
         <f t="shared" si="8"/>
-        <v>10765</v>
+        <v>-39131</v>
       </c>
       <c r="L26" s="41">
         <f t="shared" si="8"/>
-        <v>11472</v>
+        <v>-39131</v>
       </c>
       <c r="M26" s="41">
         <f t="shared" si="8"/>
-        <v>19745</v>
+        <v>-39131</v>
       </c>
       <c r="N26" s="42">
         <f t="shared" si="8"/>
-        <v>18424</v>
+        <v>-39131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aula 23 - Dashboard anual Contas a pagar e contas e receber
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="879" firstSheet="11" activeTab="16"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="879" firstSheet="11" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="605">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -2678,7 +2678,7 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -3083,6 +3083,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="12" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -14277,7 +14283,7 @@
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TdContasPagar" cacheId="75" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B6:J14" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <location ref="B6:I13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
     <pivotField numFmtId="14" showAll="0"/>
@@ -14349,18 +14355,15 @@
     <field x="3"/>
     <field x="4"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="5">
     <i>
       <x/>
     </i>
     <i r="1">
-      <x/>
+      <x v="2"/>
     </i>
     <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
+      <x v="3"/>
     </i>
     <i r="1">
       <x v="4"/>
@@ -14373,7 +14376,7 @@
     <field x="7"/>
     <field x="11"/>
   </colFields>
-  <colItems count="8">
+  <colItems count="7">
     <i>
       <x/>
       <x/>
@@ -14382,26 +14385,23 @@
       <x v="1"/>
     </i>
     <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
       <x v="4"/>
     </i>
     <i r="1">
       <x v="5"/>
     </i>
     <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
+      <x v="7"/>
     </i>
     <i t="default">
       <x/>
     </i>
   </colItems>
   <pageFields count="1">
-    <pageField fld="12" item="1" hier="-1"/>
+    <pageField fld="12" item="2" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Soma de Valor" fld="6" baseField="4" baseItem="2" numFmtId="4"/>
@@ -14789,15 +14789,15 @@
       <items count="12">
         <i x="4" s="1"/>
         <i x="5" s="1"/>
+        <i x="7" s="1"/>
         <i x="8" s="1"/>
         <i x="9" s="1"/>
-        <i x="10" s="1"/>
-        <i x="1" s="1"/>
-        <i x="2" s="1"/>
+        <i x="11" s="1"/>
         <i x="6" s="1" nd="1"/>
-        <i x="7" s="1" nd="1"/>
-        <i x="11" s="1" nd="1"/>
+        <i x="10" s="1" nd="1"/>
+        <i x="1" s="1" nd="1"/>
         <i x="0" s="1" nd="1"/>
+        <i x="2" s="1" nd="1"/>
         <i x="3" s="1" nd="1"/>
       </items>
     </tabular>
@@ -14814,8 +14814,8 @@
     <tabular pivotCacheId="2">
       <items count="3">
         <i x="0"/>
-        <i x="1" s="1"/>
-        <i x="2"/>
+        <i x="1"/>
+        <i x="2" s="1"/>
       </items>
     </tabular>
   </data>
@@ -16294,7 +16294,7 @@
         <v>546</v>
       </c>
       <c r="C4" s="48">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16310,7 +16310,7 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="J7" t="s">
+      <c r="I7" t="s">
         <v>547</v>
       </c>
     </row>
@@ -16325,19 +16325,16 @@
         <v>2</v>
       </c>
       <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
         <v>5</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>6</v>
       </c>
-      <c r="G8">
-        <v>7</v>
-      </c>
       <c r="H8">
-        <v>9</v>
-      </c>
-      <c r="I8">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -16345,151 +16342,112 @@
         <v>38</v>
       </c>
       <c r="C9" s="51">
-        <v>6816</v>
+        <v>3042</v>
       </c>
       <c r="D9" s="51">
-        <v>9291</v>
+        <v>7524</v>
       </c>
       <c r="E9" s="51">
-        <v>9778</v>
+        <v>3690</v>
       </c>
       <c r="F9" s="51">
-        <v>6321</v>
+        <v>7220</v>
       </c>
       <c r="G9" s="51">
-        <v>6846</v>
+        <v>3086</v>
       </c>
       <c r="H9" s="51">
-        <v>3092</v>
+        <v>2759</v>
       </c>
       <c r="I9" s="51">
-        <v>4672</v>
-      </c>
-      <c r="J9" s="51">
-        <v>46816</v>
+        <v>27321</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="49" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="51"/>
-      <c r="D10" s="51">
-        <v>3255</v>
-      </c>
-      <c r="E10" s="51">
-        <v>1996</v>
-      </c>
-      <c r="F10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51">
+        <v>2707</v>
+      </c>
       <c r="G10" s="51"/>
       <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51">
-        <v>5251</v>
+      <c r="I10" s="51">
+        <v>2707</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="51">
-        <v>3598</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C11" s="51"/>
       <c r="D11" s="51">
-        <v>2623</v>
-      </c>
-      <c r="E11" s="51">
-        <v>2975</v>
-      </c>
+        <v>533</v>
+      </c>
+      <c r="E11" s="51"/>
       <c r="F11" s="51"/>
-      <c r="G11" s="51">
-        <v>3411</v>
-      </c>
-      <c r="H11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51">
+        <v>2759</v>
+      </c>
       <c r="I11" s="51">
-        <v>819</v>
-      </c>
-      <c r="J11" s="51">
-        <v>13426</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="49" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C12" s="51">
-        <v>2247</v>
+        <v>3042</v>
       </c>
       <c r="D12" s="51">
-        <v>3413</v>
-      </c>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51">
-        <v>159</v>
-      </c>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51">
-        <v>5819</v>
+        <v>6991</v>
+      </c>
+      <c r="E12" s="51">
+        <v>3690</v>
+      </c>
+      <c r="F12" s="51">
+        <v>4513</v>
+      </c>
+      <c r="G12" s="51">
+        <v>3086</v>
+      </c>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51">
+        <v>21322</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="49" t="s">
-        <v>45</v>
+      <c r="B13" s="48" t="s">
+        <v>542</v>
       </c>
       <c r="C13" s="51">
-        <v>971</v>
-      </c>
-      <c r="D13" s="51"/>
+        <v>3042</v>
+      </c>
+      <c r="D13" s="51">
+        <v>7524</v>
+      </c>
       <c r="E13" s="51">
-        <v>4807</v>
+        <v>3690</v>
       </c>
       <c r="F13" s="51">
-        <v>6321</v>
+        <v>7220</v>
       </c>
       <c r="G13" s="51">
-        <v>3435</v>
+        <v>3086</v>
       </c>
       <c r="H13" s="51">
-        <v>2933</v>
+        <v>2759</v>
       </c>
       <c r="I13" s="51">
-        <v>3853</v>
-      </c>
-      <c r="J13" s="51">
-        <v>22320</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="48" t="s">
-        <v>542</v>
-      </c>
-      <c r="C14" s="51">
-        <v>6816</v>
-      </c>
-      <c r="D14" s="51">
-        <v>9291</v>
-      </c>
-      <c r="E14" s="51">
-        <v>9778</v>
-      </c>
-      <c r="F14" s="51">
-        <v>6321</v>
-      </c>
-      <c r="G14" s="51">
-        <v>6846</v>
-      </c>
-      <c r="H14" s="51">
-        <v>3092</v>
-      </c>
-      <c r="I14" s="51">
-        <v>4672</v>
-      </c>
-      <c r="J14" s="51">
-        <v>46816</v>
-      </c>
-    </row>
+        <v>27321</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18237,8 +18195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18362,8 +18320,9 @@
       </c>
     </row>
     <row r="8" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="64">
-        <v>123</v>
+      <c r="B8" s="148">
+        <f>DashBoardFinanceiroAnualD!$D$13</f>
+        <v>27321</v>
       </c>
       <c r="C8" s="53"/>
       <c r="D8" s="65"/>
@@ -18404,8 +18363,9 @@
       <c r="K10" s="67"/>
     </row>
     <row r="11" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="68">
-        <v>1234</v>
+      <c r="B11" s="149">
+        <f>DashBoardFinanceiroAnualD!$D$14</f>
+        <v>20687</v>
       </c>
       <c r="C11" s="53"/>
       <c r="D11" s="65"/>
@@ -18594,8 +18554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18868,7 +18828,10 @@
         <v>586</v>
       </c>
       <c r="C13" s="129"/>
-      <c r="D13" s="125"/>
+      <c r="D13" s="125">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Data do Caixa Realizado],"",TbRegistroSaídas[Ano Previsto],"="&amp;$C$4)</f>
+        <v>27321</v>
+      </c>
       <c r="E13" s="112"/>
       <c r="F13" s="112">
         <v>9</v>
@@ -18888,7 +18851,10 @@
         <v>588</v>
       </c>
       <c r="C14" s="130"/>
-      <c r="D14" s="131"/>
+      <c r="D14" s="131">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Data do Caixa Realizado],"",TbRegistroEntradas[Ano Previsto],$C$4)</f>
+        <v>20687</v>
+      </c>
       <c r="E14" s="112"/>
       <c r="F14" s="112">
         <v>10</v>

</xml_diff>

<commit_message>
Aula 24 - Dashboard anual Minigraficos
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="879" firstSheet="11" activeTab="17"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="879" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="606">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -1895,6 +1895,9 @@
   </si>
   <si>
     <t>HOJE:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   J   F   M  A  M   J    J    A    S   O  N  D </t>
   </si>
 </sst>
 </file>
@@ -18195,8 +18198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18282,7 +18285,9 @@
         <v>21057</v>
       </c>
       <c r="C5" s="53"/>
-      <c r="D5" s="57"/>
+      <c r="D5" s="57" t="s">
+        <v>605</v>
+      </c>
       <c r="E5" s="53"/>
       <c r="F5" s="58"/>
       <c r="G5" s="59"/>
@@ -18547,6 +18552,44 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF00B050"/>
+          <x14:colorNegative theme="5"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
+          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
+          <x14:colorLast theme="4" tint="0.39997558519241921"/>
+          <x14:colorHigh theme="4"/>
+          <x14:colorLow theme="4"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>DashBoardFinanceiroAnualD!H5:H16</xm:f>
+              <xm:sqref>D10</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FFFF0000"/>
+          <x14:colorNegative theme="4"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="4" tint="-0.249977111117893"/>
+          <x14:colorFirst theme="4" tint="-0.249977111117893"/>
+          <x14:colorLast theme="4" tint="-0.249977111117893"/>
+          <x14:colorHigh theme="4" tint="-0.249977111117893"/>
+          <x14:colorLow theme="4" tint="-0.249977111117893"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>DashBoardFinanceiroAnualD!G5:G16</xm:f>
+              <xm:sqref>D7</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -18554,8 +18597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18665,8 +18708,14 @@
       <c r="F5" s="121">
         <v>1</v>
       </c>
-      <c r="G5" s="122"/>
-      <c r="H5" s="122"/>
+      <c r="G5" s="122">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Previsto],F5,TbRegistroSaídas[Ano Previsto],$C$4,TbRegistroSaídas[Data do Caixa Realizado],"")</f>
+        <v>3042</v>
+      </c>
+      <c r="H5" s="122">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Previsto],F5,TbRegistroEntradas[Ano Previsto],$C$4,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>1209</v>
+      </c>
       <c r="I5" s="112"/>
       <c r="J5" s="122"/>
       <c r="K5" s="122"/>
@@ -18683,8 +18732,14 @@
       <c r="F6" s="112">
         <v>2</v>
       </c>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
+      <c r="G6" s="124">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Previsto],F6,TbRegistroSaídas[Ano Previsto],$C$4,TbRegistroSaídas[Data do Caixa Realizado],"")</f>
+        <v>7524</v>
+      </c>
+      <c r="H6" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Previsto],F6,TbRegistroEntradas[Ano Previsto],$C$4,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>1992</v>
+      </c>
       <c r="I6" s="112"/>
       <c r="J6" s="124"/>
       <c r="K6" s="124"/>
@@ -18703,8 +18758,14 @@
       <c r="F7" s="112">
         <v>3</v>
       </c>
-      <c r="G7" s="124"/>
-      <c r="H7" s="124"/>
+      <c r="G7" s="124">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Previsto],F7,TbRegistroSaídas[Ano Previsto],$C$4,TbRegistroSaídas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Previsto],F7,TbRegistroEntradas[Ano Previsto],$C$4,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
       <c r="I7" s="112"/>
       <c r="J7" s="124"/>
       <c r="K7" s="124"/>
@@ -18726,8 +18787,14 @@
       <c r="F8" s="112">
         <v>4</v>
       </c>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
+      <c r="G8" s="124">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Previsto],F8,TbRegistroSaídas[Ano Previsto],$C$4,TbRegistroSaídas[Data do Caixa Realizado],"")</f>
+        <v>3690</v>
+      </c>
+      <c r="H8" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Previsto],F8,TbRegistroEntradas[Ano Previsto],$C$4,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>4797</v>
+      </c>
       <c r="I8" s="112"/>
       <c r="J8" s="124"/>
       <c r="K8" s="124"/>
@@ -18749,8 +18816,14 @@
       <c r="F9" s="112">
         <v>5</v>
       </c>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
+      <c r="G9" s="124">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Previsto],F9,TbRegistroSaídas[Ano Previsto],$C$4,TbRegistroSaídas[Data do Caixa Realizado],"")</f>
+        <v>7220</v>
+      </c>
+      <c r="H9" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Previsto],F9,TbRegistroEntradas[Ano Previsto],$C$4,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>6672</v>
+      </c>
       <c r="I9" s="112"/>
       <c r="J9" s="124"/>
       <c r="K9" s="124"/>
@@ -18772,8 +18845,14 @@
       <c r="F10" s="112">
         <v>6</v>
       </c>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
+      <c r="G10" s="124">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Previsto],F10,TbRegistroSaídas[Ano Previsto],$C$4,TbRegistroSaídas[Data do Caixa Realizado],"")</f>
+        <v>3086</v>
+      </c>
+      <c r="H10" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Previsto],F10,TbRegistroEntradas[Ano Previsto],$C$4,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>1482</v>
+      </c>
       <c r="I10" s="112"/>
       <c r="J10" s="124"/>
       <c r="K10" s="124"/>
@@ -18795,8 +18874,14 @@
       <c r="F11" s="112">
         <v>7</v>
       </c>
-      <c r="G11" s="124"/>
-      <c r="H11" s="124"/>
+      <c r="G11" s="124">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Previsto],F11,TbRegistroSaídas[Ano Previsto],$C$4,TbRegistroSaídas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Previsto],F11,TbRegistroEntradas[Ano Previsto],$C$4,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>4535</v>
+      </c>
       <c r="I11" s="112"/>
       <c r="J11" s="124"/>
       <c r="K11" s="124"/>
@@ -18813,8 +18898,14 @@
       <c r="F12" s="112">
         <v>8</v>
       </c>
-      <c r="G12" s="124"/>
-      <c r="H12" s="124"/>
+      <c r="G12" s="124">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Previsto],F12,TbRegistroSaídas[Ano Previsto],$C$4,TbRegistroSaídas[Data do Caixa Realizado],"")</f>
+        <v>2759</v>
+      </c>
+      <c r="H12" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Previsto],F12,TbRegistroEntradas[Ano Previsto],$C$4,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
       <c r="I12" s="112"/>
       <c r="J12" s="124"/>
       <c r="K12" s="124"/>
@@ -18836,8 +18927,14 @@
       <c r="F13" s="112">
         <v>9</v>
       </c>
-      <c r="G13" s="124"/>
-      <c r="H13" s="124"/>
+      <c r="G13" s="124">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Previsto],F13,TbRegistroSaídas[Ano Previsto],$C$4,TbRegistroSaídas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Previsto],F13,TbRegistroEntradas[Ano Previsto],$C$4,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
       <c r="I13" s="112"/>
       <c r="J13" s="124"/>
       <c r="K13" s="124"/>
@@ -18859,8 +18956,14 @@
       <c r="F14" s="112">
         <v>10</v>
       </c>
-      <c r="G14" s="124"/>
-      <c r="H14" s="124"/>
+      <c r="G14" s="124">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Previsto],F14,TbRegistroSaídas[Ano Previsto],$C$4,TbRegistroSaídas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Previsto],F14,TbRegistroEntradas[Ano Previsto],$C$4,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
       <c r="I14" s="112"/>
       <c r="J14" s="124"/>
       <c r="K14" s="124"/>
@@ -18877,8 +18980,14 @@
       <c r="F15" s="112">
         <v>11</v>
       </c>
-      <c r="G15" s="124"/>
-      <c r="H15" s="124"/>
+      <c r="G15" s="124">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Previsto],F15,TbRegistroSaídas[Ano Previsto],$C$4,TbRegistroSaídas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Previsto],F15,TbRegistroEntradas[Ano Previsto],$C$4,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
       <c r="I15" s="112"/>
       <c r="J15" s="124"/>
       <c r="K15" s="124"/>
@@ -18895,8 +19004,14 @@
       <c r="F16" s="127">
         <v>12</v>
       </c>
-      <c r="G16" s="132"/>
-      <c r="H16" s="132"/>
+      <c r="G16" s="132">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Mês Previsto],F16,TbRegistroSaídas[Ano Previsto],$C$4,TbRegistroSaídas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="132">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês Previsto],F16,TbRegistroEntradas[Ano Previsto],$C$4,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
       <c r="I16" s="112"/>
       <c r="J16" s="132"/>
       <c r="K16" s="132"/>

</xml_diff>

<commit_message>
Aula 25 - Dashboard anual Evolucao de vendas
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -30,17 +30,11 @@
     <externalReference r:id="rId19"/>
   </externalReferences>
   <definedNames>
-    <definedName name="PCEntradasN1_Nível_1" localSheetId="16">TbPCEntradasN1[Nível 1]</definedName>
     <definedName name="PCEntradasN1_Nível_1">TbPCEntradasN1[Nível 1]</definedName>
-    <definedName name="PCEntradasN2_Nível_1" localSheetId="16">TbPCEntradasN2[Nível 1]</definedName>
     <definedName name="PCEntradasN2_Nível_1">TbPCEntradasN2[Nível 1]</definedName>
-    <definedName name="PCEntradasN2_Nível_2" localSheetId="16">TbPCEntradasN2[Nível 2]</definedName>
     <definedName name="PCEntradasN2_Nível_2">TbPCEntradasN2[Nível 2]</definedName>
-    <definedName name="PCSaídasN1_Nível_1" localSheetId="16">TbPCSaídasN1[Nível 1]</definedName>
     <definedName name="PCSaídasN1_Nível_1">TbPCSaídasN1[Nível 1]</definedName>
-    <definedName name="PCSaídasN2_Nível_1" localSheetId="16">TbPCSaídasN2[Nível 1]</definedName>
     <definedName name="PCSaídasN2_Nível_1">TbPCSaídasN2[Nível 1]</definedName>
-    <definedName name="PCSaídasN2_Nível_2" localSheetId="16">TbPCSaídasN2[Nível 2]</definedName>
     <definedName name="PCSaídasN2_Nível_2">TbPCSaídasN2[Nível 2]</definedName>
     <definedName name="SegmentaçãodeDados_Ano_Competência">#N/A</definedName>
     <definedName name="SegmentaçãodeDados_Ano_Competência1">#N/A</definedName>
@@ -79,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="606">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -1912,7 +1906,7 @@
     <numFmt numFmtId="169" formatCode="&quot;R$&quot;\ #,##0"/>
     <numFmt numFmtId="170" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2158,6 +2152,14 @@
       <color rgb="FF548235"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="6" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2681,7 +2683,7 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -3094,20 +3096,19 @@
     <xf numFmtId="43" fontId="17" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="29" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="32" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -3340,6 +3341,198 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>DashBoardFinanceiroAnualD!$L$5:$L$16</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fev</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mai</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ago</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Out</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dez</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DashBoardFinanceiroAnualD!$K$5:$K$16</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10916</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9948</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1620</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2194</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="161643136"/>
+        <c:axId val="161648000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="161643136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="161648000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="161648000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="161643136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5715,6 +5908,38 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -5729,7 +5954,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Retângulo 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
@@ -14920,7 +15145,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B9" totalsRowShown="0" headerRowDxfId="35">
   <autoFilter ref="B4:B9"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -14930,7 +15155,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C13" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN2" displayName="TbPCEntradasN2" ref="B4:C13" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33">
   <autoFilter ref="B4:C13"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
@@ -14941,7 +15166,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TbPCSaídasN1" displayName="TbPCSaídasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31">
   <autoFilter ref="B4:B10"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -14951,7 +15176,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C16" totalsRowShown="0" headerRowDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TbPCSaídasN2" displayName="TbPCSaídasN2" ref="B4:C16" totalsRowShown="0" headerRowDxfId="30">
   <autoFilter ref="B4:C16"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Nível 1"/>
@@ -14962,35 +15187,46 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B3:O234" totalsRowShown="0" headerRowDxfId="30">
-  <autoFilter ref="B3:O234"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B3:O234" totalsRowShown="0" headerRowDxfId="29">
+  <autoFilter ref="B3:O234">
+    <filterColumn colId="0">
+      <filters>
+        <dateGroupItem year="2019" dateTimeGrouping="year"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Livros"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="29"/>
-    <tableColumn id="2" name="Data da Competência" dataDxfId="28"/>
-    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="27"/>
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="28"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="27"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="26"/>
     <tableColumn id="4" name="Conta Nível 1"/>
     <tableColumn id="5" name="Conta Nível 2"/>
     <tableColumn id="6" name="Histórico"/>
-    <tableColumn id="7" name="Valor" dataDxfId="26"/>
-    <tableColumn id="8" name="Mês Caixa" dataDxfId="25">
+    <tableColumn id="7" name="Valor" dataDxfId="25"/>
+    <tableColumn id="8" name="Mês Caixa" dataDxfId="24">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]="",0,MONTH(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Ano Caixa" dataDxfId="24">
+    <tableColumn id="9" name="Ano Caixa" dataDxfId="23">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]="",0,YEAR(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Mês Competência" dataDxfId="23">
+    <tableColumn id="10" name="Mês Competência" dataDxfId="22">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data da Competência]]="",0,MONTH(TbRegistroEntradas[[#This Row],[Data da Competência]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Ano Competência" dataDxfId="22">
+    <tableColumn id="11" name="Ano Competência" dataDxfId="21">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data da Competência]]="",0,YEAR(TbRegistroEntradas[[#This Row],[Data da Competência]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Mês Previsto" dataDxfId="8">
+    <tableColumn id="12" name="Mês Previsto" dataDxfId="7">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]="",0,MONTH(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Ano Previsto" dataDxfId="7">
+    <tableColumn id="13" name="Ano Previsto" dataDxfId="6">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]="",0,YEAR(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Conta Vencida" dataDxfId="6">
+    <tableColumn id="14" name="Conta Vencida" dataDxfId="5">
       <calculatedColumnFormula>IF(AND(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]&lt;TODAY(),TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]=""),"Vencida","Não Vencida")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -14999,32 +15235,32 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TbRegistroSaídas" displayName="TbRegistroSaídas" ref="B3:N232" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TbRegistroSaídas" displayName="TbRegistroSaídas" ref="B3:N232" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18">
   <autoFilter ref="B3:N232"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="18"/>
-    <tableColumn id="2" name="Data da Competência" dataDxfId="17"/>
-    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="16"/>
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="17"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="16"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="15"/>
     <tableColumn id="4" name="Conta Nível 1"/>
     <tableColumn id="5" name="Conta Nível 2"/>
     <tableColumn id="6" name="Histórico"/>
-    <tableColumn id="7" name="Valor" dataDxfId="15"/>
-    <tableColumn id="8" name="Mês Caixa" dataDxfId="14">
+    <tableColumn id="7" name="Valor" dataDxfId="14"/>
+    <tableColumn id="8" name="Mês Caixa" dataDxfId="13">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data do Caixa Realizado]]="",0,MONTH(TbRegistroSaídas[[#This Row],[Data do Caixa Realizado]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Ano Caixa" dataDxfId="13">
+    <tableColumn id="9" name="Ano Caixa" dataDxfId="12">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data do Caixa Realizado]]="",0,YEAR(TbRegistroSaídas[[#This Row],[Data do Caixa Realizado]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Mês Competência" dataDxfId="12">
+    <tableColumn id="10" name="Mês Competência" dataDxfId="11">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data da Competência]]="",0,MONTH(TbRegistroSaídas[[#This Row],[Data da Competência]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Ano Competência" dataDxfId="11">
+    <tableColumn id="11" name="Ano Competência" dataDxfId="10">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data da Competência]]="",0,YEAR(TbRegistroSaídas[[#This Row],[Data da Competência]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Mês Previsto" dataDxfId="10">
+    <tableColumn id="12" name="Mês Previsto" dataDxfId="9">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data do Caixa Previsto]]="",0,MONTH(TbRegistroSaídas[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Ano Previsto" dataDxfId="9">
+    <tableColumn id="13" name="Ano Previsto" dataDxfId="8">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data do Caixa Previsto]]="",0,YEAR(TbRegistroSaídas[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -15408,13 +15644,16 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="15" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="3.42578125" customWidth="1"/>
+    <col min="17" max="16384" width="11.7109375" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -15824,16 +16063,15 @@
   <sheetPr codeName="Plan11"/>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="15" width="11.7109375" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" hidden="1"/>
+    <col min="16" max="16" width="3.5703125" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -17350,7 +17588,7 @@
     <mergeCell ref="F13:G13"/>
   </mergeCells>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17368,7 +17606,7 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18186,7 +18424,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18199,7 +18437,7 @@
   <dimension ref="B1:O21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18277,7 +18515,9 @@
         <v>552</v>
       </c>
       <c r="J4" s="55"/>
-      <c r="K4" s="109"/>
+      <c r="K4" s="109" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="147">
@@ -18337,8 +18577,9 @@
       <c r="H8" s="59"/>
       <c r="I8" s="60"/>
       <c r="J8" s="60"/>
-      <c r="K8" s="66">
-        <v>-123</v>
+      <c r="K8" s="151">
+        <f>SUM(DashBoardFinanceiroAnualD!J5:J16)</f>
+        <v>24678</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -18537,18 +18778,20 @@
     <mergeCell ref="F13:G13"/>
   </mergeCells>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conta Inexistente!" error="Selecione uma conta da lista." sqref="K14"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conta Inexisente!" error="Selecione um item da conta." sqref="K4"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conta Inexisente!" error="Selecione um item da conta." sqref="K4">
+      <formula1>PCEntradasN2_Nível_2</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18598,7 +18841,7 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H16"/>
+      <selection activeCell="J5" sqref="J5:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18613,7 +18856,7 @@
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -18665,7 +18908,10 @@
       <c r="K3" s="115" t="s">
         <v>567</v>
       </c>
-      <c r="L3" s="116"/>
+      <c r="L3" s="150">
+        <f>$C$4</f>
+        <v>2019</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="112"/>
@@ -18689,8 +18935,8 @@
       </c>
       <c r="I4" s="112"/>
       <c r="J4" s="120" t="str">
-        <f>[1]DashBoardFinanceiroAnual!K4</f>
-        <v>Som e imagem</v>
+        <f>DashBoardFinanceiroAnual!$K$4</f>
+        <v>Livros</v>
       </c>
       <c r="K4" s="118" t="s">
         <v>572</v>
@@ -18717,8 +18963,14 @@
         <v>1209</v>
       </c>
       <c r="I5" s="112"/>
-      <c r="J5" s="122"/>
-      <c r="K5" s="122"/>
+      <c r="J5" s="122">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$J$4,TbRegistroEntradas[Ano Caixa],$L$3,TbRegistroEntradas[Mês Caixa],F5)</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="122" t="e">
+        <f>IF(J5=0,NA(),J5)</f>
+        <v>#N/A</v>
+      </c>
       <c r="L5" s="123" t="s">
         <v>573</v>
       </c>
@@ -18741,8 +18993,14 @@
         <v>1992</v>
       </c>
       <c r="I6" s="112"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="124"/>
+      <c r="J6" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$J$4,TbRegistroEntradas[Ano Caixa],$L$3,TbRegistroEntradas[Mês Caixa],F6)</f>
+        <v>10916</v>
+      </c>
+      <c r="K6" s="124">
+        <f t="shared" ref="K6:K16" si="0">IF(J6=0,NA(),J6)</f>
+        <v>10916</v>
+      </c>
       <c r="L6" s="115" t="s">
         <v>574</v>
       </c>
@@ -18767,8 +19025,14 @@
         <v>0</v>
       </c>
       <c r="I7" s="112"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="124"/>
+      <c r="J7" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$J$4,TbRegistroEntradas[Ano Caixa],$L$3,TbRegistroEntradas[Mês Caixa],F7)</f>
+        <v>9948</v>
+      </c>
+      <c r="K7" s="124">
+        <f t="shared" si="0"/>
+        <v>9948</v>
+      </c>
       <c r="L7" s="115" t="s">
         <v>576</v>
       </c>
@@ -18796,8 +19060,14 @@
         <v>4797</v>
       </c>
       <c r="I8" s="112"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="124"/>
+      <c r="J8" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$J$4,TbRegistroEntradas[Ano Caixa],$L$3,TbRegistroEntradas[Mês Caixa],F8)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="124" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
       <c r="L8" s="115" t="s">
         <v>578</v>
       </c>
@@ -18825,8 +19095,14 @@
         <v>6672</v>
       </c>
       <c r="I9" s="112"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
+      <c r="J9" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$J$4,TbRegistroEntradas[Ano Caixa],$L$3,TbRegistroEntradas[Mês Caixa],F9)</f>
+        <v>1620</v>
+      </c>
+      <c r="K9" s="124">
+        <f t="shared" si="0"/>
+        <v>1620</v>
+      </c>
       <c r="L9" s="115" t="s">
         <v>580</v>
       </c>
@@ -18854,8 +19130,14 @@
         <v>1482</v>
       </c>
       <c r="I10" s="112"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
+      <c r="J10" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$J$4,TbRegistroEntradas[Ano Caixa],$L$3,TbRegistroEntradas[Mês Caixa],F10)</f>
+        <v>2194</v>
+      </c>
+      <c r="K10" s="124">
+        <f t="shared" si="0"/>
+        <v>2194</v>
+      </c>
       <c r="L10" s="115" t="s">
         <v>582</v>
       </c>
@@ -18883,8 +19165,14 @@
         <v>4535</v>
       </c>
       <c r="I11" s="112"/>
-      <c r="J11" s="124"/>
-      <c r="K11" s="124"/>
+      <c r="J11" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$J$4,TbRegistroEntradas[Ano Caixa],$L$3,TbRegistroEntradas[Mês Caixa],F11)</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="124" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
       <c r="L11" s="115" t="s">
         <v>584</v>
       </c>
@@ -18907,8 +19195,14 @@
         <v>0</v>
       </c>
       <c r="I12" s="112"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="124"/>
+      <c r="J12" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$J$4,TbRegistroEntradas[Ano Caixa],$L$3,TbRegistroEntradas[Mês Caixa],F12)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="124" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
       <c r="L12" s="115" t="s">
         <v>585</v>
       </c>
@@ -18936,8 +19230,14 @@
         <v>0</v>
       </c>
       <c r="I13" s="112"/>
-      <c r="J13" s="124"/>
-      <c r="K13" s="124"/>
+      <c r="J13" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$J$4,TbRegistroEntradas[Ano Caixa],$L$3,TbRegistroEntradas[Mês Caixa],F13)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="124" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
       <c r="L13" s="115" t="s">
         <v>587</v>
       </c>
@@ -18965,8 +19265,14 @@
         <v>0</v>
       </c>
       <c r="I14" s="112"/>
-      <c r="J14" s="124"/>
-      <c r="K14" s="124"/>
+      <c r="J14" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$J$4,TbRegistroEntradas[Ano Caixa],$L$3,TbRegistroEntradas[Mês Caixa],F14)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="124" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
       <c r="L14" s="115" t="s">
         <v>589</v>
       </c>
@@ -18989,8 +19295,14 @@
         <v>0</v>
       </c>
       <c r="I15" s="112"/>
-      <c r="J15" s="124"/>
-      <c r="K15" s="124"/>
+      <c r="J15" s="124">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$J$4,TbRegistroEntradas[Ano Caixa],$L$3,TbRegistroEntradas[Mês Caixa],F15)</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="124" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
       <c r="L15" s="115" t="s">
         <v>590</v>
       </c>
@@ -19013,8 +19325,14 @@
         <v>0</v>
       </c>
       <c r="I16" s="112"/>
-      <c r="J16" s="132"/>
-      <c r="K16" s="132"/>
+      <c r="J16" s="132">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$J$4,TbRegistroEntradas[Ano Caixa],$L$3,TbRegistroEntradas[Mês Caixa],F16)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="132" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
       <c r="L16" s="133" t="s">
         <v>591</v>
       </c>
@@ -19506,7 +19824,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19723,7 +20041,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20242,8 +20560,8 @@
   <dimension ref="B1:O234"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H135" sqref="H135:H234"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H185" activeCellId="1" sqref="H175:H181 H185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20330,7 +20648,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13">
         <v>42994</v>
       </c>
@@ -20381,7 +20699,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13">
         <v>42985</v>
       </c>
@@ -20432,7 +20750,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13">
         <v>43007</v>
       </c>
@@ -20483,7 +20801,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13">
         <v>43020</v>
       </c>
@@ -20534,7 +20852,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13">
         <v>43014</v>
       </c>
@@ -20585,7 +20903,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13">
         <v>43054</v>
       </c>
@@ -20636,7 +20954,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13">
         <v>43087</v>
       </c>
@@ -20687,7 +21005,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13">
         <v>43004</v>
       </c>
@@ -20738,7 +21056,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13">
         <v>43015</v>
       </c>
@@ -20789,7 +21107,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
         <v>69</v>
       </c>
@@ -20840,7 +21158,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="13">
         <v>42997</v>
       </c>
@@ -20891,7 +21209,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="15" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="13">
         <v>43002</v>
       </c>
@@ -20942,7 +21260,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="13">
         <v>43001</v>
       </c>
@@ -20993,7 +21311,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="17" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="13">
         <v>43056</v>
       </c>
@@ -21044,7 +21362,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13">
         <v>43018</v>
       </c>
@@ -21095,7 +21413,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="13">
         <v>43019</v>
       </c>
@@ -21146,7 +21464,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="13">
         <v>43076</v>
       </c>
@@ -21197,7 +21515,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="13">
         <v>43052</v>
       </c>
@@ -21248,7 +21566,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="13">
         <v>43043</v>
       </c>
@@ -21299,7 +21617,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="13">
         <v>43060</v>
       </c>
@@ -21350,7 +21668,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="13" t="s">
         <v>69</v>
       </c>
@@ -21401,7 +21719,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="13">
         <v>43113</v>
       </c>
@@ -21452,7 +21770,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="13">
         <v>43030</v>
       </c>
@@ -21503,7 +21821,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="13">
         <v>43032</v>
       </c>
@@ -21554,7 +21872,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="13">
         <v>43122</v>
       </c>
@@ -21605,7 +21923,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="13">
         <v>43034</v>
       </c>
@@ -21656,7 +21974,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="13">
         <v>43052</v>
       </c>
@@ -21707,7 +22025,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="13" t="s">
         <v>69</v>
       </c>
@@ -21758,7 +22076,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="13">
         <v>43117</v>
       </c>
@@ -21809,7 +22127,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="13">
         <v>43047</v>
       </c>
@@ -21860,7 +22178,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="13">
         <v>43077</v>
       </c>
@@ -21911,7 +22229,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="13">
         <v>43101</v>
       </c>
@@ -21962,7 +22280,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="13">
         <v>43055</v>
       </c>
@@ -22013,7 +22331,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="13" t="s">
         <v>69</v>
       </c>
@@ -22064,7 +22382,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="13">
         <v>43090</v>
       </c>
@@ -22115,7 +22433,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="13">
         <v>43059</v>
       </c>
@@ -22166,7 +22484,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="13">
         <v>43122</v>
       </c>
@@ -22217,7 +22535,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="13">
         <v>43114</v>
       </c>
@@ -22268,7 +22586,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="13">
         <v>43073</v>
       </c>
@@ -22319,7 +22637,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="13">
         <v>43073</v>
       </c>
@@ -22370,7 +22688,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="13">
         <v>43103</v>
       </c>
@@ -22421,7 +22739,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="13">
         <v>43103</v>
       </c>
@@ -22472,7 +22790,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="13">
         <v>43086</v>
       </c>
@@ -22523,7 +22841,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="13">
         <v>43122</v>
       </c>
@@ -22574,7 +22892,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="13">
         <v>43123</v>
       </c>
@@ -22625,7 +22943,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="13">
         <v>43125</v>
       </c>
@@ -22676,7 +22994,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" s="13">
         <v>43089</v>
       </c>
@@ -22727,7 +23045,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" s="13">
         <v>43133</v>
       </c>
@@ -22778,7 +23096,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" s="13">
         <v>43182</v>
       </c>
@@ -22829,7 +23147,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" s="13">
         <v>43101</v>
       </c>
@@ -22880,7 +23198,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" s="13">
         <v>43144</v>
       </c>
@@ -22931,7 +23249,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="13" t="s">
         <v>69</v>
       </c>
@@ -22982,7 +23300,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" s="13">
         <v>43155</v>
       </c>
@@ -23033,7 +23351,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="13">
         <v>43117</v>
       </c>
@@ -23084,7 +23402,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="13">
         <v>43166</v>
       </c>
@@ -23135,7 +23453,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" s="13">
         <v>43145</v>
       </c>
@@ -23186,7 +23504,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B60" s="13">
         <v>43142</v>
       </c>
@@ -23237,7 +23555,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" s="13">
         <v>43206</v>
       </c>
@@ -23288,7 +23606,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" s="13">
         <v>43137</v>
       </c>
@@ -23339,7 +23657,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B63" s="13">
         <v>43161</v>
       </c>
@@ -23390,7 +23708,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B64" s="13">
         <v>43178</v>
       </c>
@@ -23441,7 +23759,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B65" s="13">
         <v>43138</v>
       </c>
@@ -23492,7 +23810,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="66" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="13" t="s">
         <v>69</v>
       </c>
@@ -23543,7 +23861,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="67" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B67" s="13">
         <v>43145</v>
       </c>
@@ -23594,7 +23912,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="68" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" s="13">
         <v>43146</v>
       </c>
@@ -23645,7 +23963,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="69" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" s="13">
         <v>43193</v>
       </c>
@@ -23696,7 +24014,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="70" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="13">
         <v>43193</v>
       </c>
@@ -23747,7 +24065,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="71" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B71" s="13">
         <v>43154</v>
       </c>
@@ -23798,7 +24116,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="72" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B72" s="13" t="s">
         <v>69</v>
       </c>
@@ -23849,7 +24167,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="73" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" s="13">
         <v>43246</v>
       </c>
@@ -23900,7 +24218,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" s="13">
         <v>43169</v>
       </c>
@@ -23951,7 +24269,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="75" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B75" s="13" t="s">
         <v>69</v>
       </c>
@@ -24002,7 +24320,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" s="13">
         <v>43287</v>
       </c>
@@ -24053,7 +24371,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" s="13">
         <v>43203</v>
       </c>
@@ -24104,7 +24422,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" s="13">
         <v>43169</v>
       </c>
@@ -24155,7 +24473,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" s="13">
         <v>43274</v>
       </c>
@@ -24206,7 +24524,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" s="13">
         <v>43176</v>
       </c>
@@ -24257,7 +24575,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="13">
         <v>43177</v>
       </c>
@@ -24308,7 +24626,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="13">
         <v>43225</v>
       </c>
@@ -24359,7 +24677,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="13">
         <v>43199</v>
       </c>
@@ -24410,7 +24728,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B84" s="13">
         <v>43187</v>
       </c>
@@ -24461,7 +24779,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" s="13">
         <v>43257</v>
       </c>
@@ -24512,7 +24830,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B86" s="13">
         <v>43214</v>
       </c>
@@ -24563,7 +24881,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="13">
         <v>43306</v>
       </c>
@@ -24614,7 +24932,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B88" s="13">
         <v>43193</v>
       </c>
@@ -24665,7 +24983,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B89" s="13">
         <v>43196</v>
       </c>
@@ -24716,7 +25034,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B90" s="13">
         <v>43251</v>
       </c>
@@ -24767,7 +25085,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B91" s="13" t="s">
         <v>69</v>
       </c>
@@ -24818,7 +25136,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B92" s="13">
         <v>43224</v>
       </c>
@@ -24869,7 +25187,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B93" s="13">
         <v>43295</v>
       </c>
@@ -24920,7 +25238,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B94" s="13">
         <v>43234</v>
       </c>
@@ -24971,7 +25289,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="13">
         <v>43216</v>
       </c>
@@ -25022,7 +25340,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B96" s="13">
         <v>43226</v>
       </c>
@@ -25073,7 +25391,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B97" s="13">
         <v>43283</v>
       </c>
@@ -25124,7 +25442,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="98" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B98" s="13">
         <v>43311</v>
       </c>
@@ -25175,7 +25493,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="99" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B99" s="13">
         <v>43233</v>
       </c>
@@ -25226,7 +25544,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="100" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B100" s="13">
         <v>43252</v>
       </c>
@@ -25277,7 +25595,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="101" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B101" s="13">
         <v>43275</v>
       </c>
@@ -25328,7 +25646,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="102" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B102" s="13">
         <v>43275</v>
       </c>
@@ -25379,7 +25697,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="103" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B103" s="13">
         <v>43265</v>
       </c>
@@ -25430,7 +25748,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="104" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B104" s="13">
         <v>43340</v>
       </c>
@@ -25481,7 +25799,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="105" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B105" s="13">
         <v>43255</v>
       </c>
@@ -25532,7 +25850,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="106" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B106" s="13">
         <v>43267</v>
       </c>
@@ -25583,7 +25901,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="107" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B107" s="13">
         <v>43259</v>
       </c>
@@ -25634,7 +25952,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="108" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B108" s="13">
         <v>43276</v>
       </c>
@@ -25685,7 +26003,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="109" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B109" s="13">
         <v>43320</v>
       </c>
@@ -25736,7 +26054,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="110" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B110" s="13">
         <v>43303</v>
       </c>
@@ -25787,7 +26105,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="111" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B111" s="13">
         <v>43293</v>
       </c>
@@ -25838,7 +26156,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="112" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B112" s="13">
         <v>43268</v>
       </c>
@@ -25889,7 +26207,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="113" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B113" s="13">
         <v>43326</v>
       </c>
@@ -25940,7 +26258,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="114" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B114" s="13">
         <v>43313</v>
       </c>
@@ -25991,7 +26309,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="115" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B115" s="13">
         <v>43317</v>
       </c>
@@ -26042,7 +26360,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="116" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B116" s="13">
         <v>43328</v>
       </c>
@@ -26093,7 +26411,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="117" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B117" s="13">
         <v>43398</v>
       </c>
@@ -26144,7 +26462,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="118" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B118" s="13">
         <v>43343</v>
       </c>
@@ -26195,7 +26513,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="119" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B119" s="13">
         <v>43316</v>
       </c>
@@ -26246,7 +26564,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="120" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B120" s="13">
         <v>43336</v>
       </c>
@@ -26297,7 +26615,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="121" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B121" s="13">
         <v>43323</v>
       </c>
@@ -26348,7 +26666,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="122" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B122" s="13">
         <v>43311</v>
       </c>
@@ -26399,7 +26717,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="123" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B123" s="13">
         <v>43302</v>
       </c>
@@ -26450,7 +26768,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="124" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B124" s="13" t="s">
         <v>69</v>
       </c>
@@ -26501,7 +26819,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="125" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B125" s="13" t="s">
         <v>69</v>
       </c>
@@ -26552,7 +26870,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="126" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B126" s="13">
         <v>43350</v>
       </c>
@@ -26603,7 +26921,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="127" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B127" s="13" t="s">
         <v>69</v>
       </c>
@@ -26654,7 +26972,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="128" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B128" s="13">
         <v>43409</v>
       </c>
@@ -26705,7 +27023,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="129" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B129" s="13">
         <v>43368</v>
       </c>
@@ -26756,7 +27074,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="130" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B130" s="13">
         <v>43341</v>
       </c>
@@ -26807,7 +27125,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="131" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B131" s="13">
         <v>43323</v>
       </c>
@@ -26858,7 +27176,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="132" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B132" s="13">
         <v>43360</v>
       </c>
@@ -26909,7 +27227,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="133" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B133" s="13">
         <v>43329</v>
       </c>
@@ -26960,7 +27278,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="134" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B134" s="13">
         <v>43336</v>
       </c>
@@ -27011,7 +27329,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="135" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B135" s="13">
         <v>43475</v>
       </c>
@@ -27062,7 +27380,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="136" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B136" s="13">
         <v>43393</v>
       </c>
@@ -27113,7 +27431,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="137" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B137" s="13">
         <v>43405</v>
       </c>
@@ -27164,7 +27482,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="138" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B138" s="13">
         <v>43370</v>
       </c>
@@ -27215,7 +27533,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="139" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B139" s="13">
         <v>43350</v>
       </c>
@@ -27266,7 +27584,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="140" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B140" s="13">
         <v>43365</v>
       </c>
@@ -27317,7 +27635,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="141" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B141" s="13">
         <v>43383</v>
       </c>
@@ -27368,7 +27686,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="142" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B142" s="13">
         <v>43412</v>
       </c>
@@ -27419,7 +27737,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="143" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B143" s="13">
         <v>43374</v>
       </c>
@@ -27470,7 +27788,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="144" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B144" s="13">
         <v>43422</v>
       </c>
@@ -27521,7 +27839,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="145" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B145" s="13">
         <v>43405</v>
       </c>
@@ -27572,7 +27890,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="146" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B146" s="13">
         <v>43369</v>
       </c>
@@ -27623,7 +27941,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="147" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B147" s="13">
         <v>43392</v>
       </c>
@@ -27674,7 +27992,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="148" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B148" s="13">
         <v>43399</v>
       </c>
@@ -27725,7 +28043,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="149" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B149" s="13">
         <v>43432</v>
       </c>
@@ -27776,7 +28094,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="150" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B150" s="13">
         <v>43382</v>
       </c>
@@ -27827,7 +28145,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="151" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B151" s="13">
         <v>43400</v>
       </c>
@@ -27878,7 +28196,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="152" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B152" s="13" t="s">
         <v>69</v>
       </c>
@@ -27929,7 +28247,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="153" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B153" s="13">
         <v>43435</v>
       </c>
@@ -27980,7 +28298,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="154" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B154" s="13">
         <v>43424</v>
       </c>
@@ -28031,7 +28349,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="155" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B155" s="13">
         <v>43398</v>
       </c>
@@ -28082,7 +28400,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="156" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B156" s="13" t="s">
         <v>69</v>
       </c>
@@ -28133,7 +28451,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="157" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B157" s="13">
         <v>43442</v>
       </c>
@@ -28184,7 +28502,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="158" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B158" s="13">
         <v>43431</v>
       </c>
@@ -28235,7 +28553,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="159" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B159" s="13">
         <v>43421</v>
       </c>
@@ -28286,7 +28604,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="160" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B160" s="13">
         <v>43418</v>
       </c>
@@ -28337,7 +28655,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="161" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B161" s="13">
         <v>43537</v>
       </c>
@@ -28388,7 +28706,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="162" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B162" s="13">
         <v>43425</v>
       </c>
@@ -28439,7 +28757,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="163" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B163" s="13">
         <v>43465</v>
       </c>
@@ -28490,7 +28808,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="164" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B164" s="13">
         <v>43457</v>
       </c>
@@ -28541,7 +28859,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="165" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B165" s="13">
         <v>43431</v>
       </c>
@@ -28592,7 +28910,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="166" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B166" s="13">
         <v>43434</v>
       </c>
@@ -28643,7 +28961,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="167" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B167" s="13" t="s">
         <v>69</v>
       </c>
@@ -28694,7 +29012,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="168" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B168" s="13">
         <v>43560</v>
       </c>
@@ -28745,7 +29063,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="169" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B169" s="13">
         <v>43503</v>
       </c>
@@ -28796,7 +29114,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="170" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B170" s="13">
         <v>43459</v>
       </c>
@@ -28847,7 +29165,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="171" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B171" s="13">
         <v>43497</v>
       </c>
@@ -28898,7 +29216,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="172" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B172" s="13">
         <v>43457</v>
       </c>
@@ -28949,7 +29267,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="173" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B173" s="13">
         <v>43519</v>
       </c>
@@ -29000,7 +29318,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="174" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B174" s="13">
         <v>43483</v>
       </c>
@@ -29102,7 +29420,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="176" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B176" s="13">
         <v>43473</v>
       </c>
@@ -29153,7 +29471,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="177" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B177" s="13">
         <v>43478</v>
       </c>
@@ -29204,7 +29522,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="178" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B178" s="13">
         <v>43538</v>
       </c>
@@ -29255,7 +29573,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="179" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B179" s="13">
         <v>43485</v>
       </c>
@@ -29306,7 +29624,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="180" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B180" s="13" t="s">
         <v>69</v>
       </c>
@@ -29408,7 +29726,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="182" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B182" s="13" t="s">
         <v>69</v>
       </c>
@@ -29459,7 +29777,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="183" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B183" s="13">
         <v>43494</v>
       </c>
@@ -29612,7 +29930,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="186" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B186" s="13">
         <v>43532</v>
       </c>
@@ -29663,7 +29981,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="187" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B187" s="13">
         <v>43540</v>
       </c>
@@ -29714,7 +30032,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="188" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B188" s="13">
         <v>43541</v>
       </c>
@@ -29765,7 +30083,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="189" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B189" s="13">
         <v>43549</v>
       </c>
@@ -29816,7 +30134,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="190" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B190" s="13">
         <v>43509</v>
       </c>
@@ -29867,7 +30185,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="191" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B191" s="13">
         <v>43512</v>
       </c>
@@ -29918,7 +30236,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="192" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B192" s="13">
         <v>43533</v>
       </c>
@@ -29969,7 +30287,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="193" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B193" s="13">
         <v>43540</v>
       </c>
@@ -30020,7 +30338,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="194" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B194" s="13">
         <v>43548</v>
       </c>
@@ -30071,7 +30389,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="195" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B195" s="13">
         <v>43522</v>
       </c>
@@ -30122,7 +30440,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="196" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B196" s="13">
         <v>43525</v>
       </c>
@@ -30173,7 +30491,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="197" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B197" s="13">
         <v>43527</v>
       </c>
@@ -30224,7 +30542,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="198" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B198" s="13">
         <v>43563</v>
       </c>
@@ -30275,7 +30593,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="199" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B199" s="13">
         <v>43578</v>
       </c>
@@ -30428,7 +30746,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="202" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B202" s="13" t="s">
         <v>69</v>
       </c>
@@ -30479,7 +30797,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="203" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B203" s="13">
         <v>43643</v>
       </c>
@@ -30530,7 +30848,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="204" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B204" s="13">
         <v>43558</v>
       </c>
@@ -30581,7 +30899,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="205" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B205" s="13">
         <v>43561</v>
       </c>
@@ -30632,7 +30950,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="206" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B206" s="13">
         <v>43625</v>
       </c>
@@ -30683,7 +31001,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="207" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B207" s="13">
         <v>43609</v>
       </c>
@@ -30734,7 +31052,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="208" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B208" s="13">
         <v>43615</v>
       </c>
@@ -30785,7 +31103,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="209" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B209" s="13">
         <v>43569</v>
       </c>
@@ -30836,7 +31154,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="210" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B210" s="13" t="s">
         <v>69</v>
       </c>
@@ -30938,7 +31256,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="212" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B212" s="13">
         <v>43683</v>
       </c>
@@ -30989,7 +31307,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="213" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B213" s="13">
         <v>43595</v>
       </c>
@@ -31040,7 +31358,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="214" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B214" s="13">
         <v>43594</v>
       </c>
@@ -31091,7 +31409,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="215" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B215" s="13">
         <v>43587</v>
       </c>
@@ -31142,7 +31460,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="216" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B216" s="13">
         <v>43626</v>
       </c>
@@ -31193,7 +31511,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="217" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B217" s="13">
         <v>43592</v>
       </c>
@@ -31244,7 +31562,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="218" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B218" s="13">
         <v>43603</v>
       </c>
@@ -31295,7 +31613,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="219" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B219" s="13">
         <v>43597</v>
       </c>
@@ -31346,7 +31664,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="220" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B220" s="13">
         <v>43631</v>
       </c>
@@ -31397,7 +31715,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="221" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B221" s="13">
         <v>43635</v>
       </c>
@@ -31499,7 +31817,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="223" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B223" s="13" t="s">
         <v>69</v>
       </c>
@@ -31550,7 +31868,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="224" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B224" s="13">
         <v>43655</v>
       </c>
@@ -31601,7 +31919,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="225" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B225" s="13" t="s">
         <v>69</v>
       </c>
@@ -31652,7 +31970,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="226" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B226" s="13">
         <v>43641</v>
       </c>
@@ -31703,7 +32021,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="227" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B227" s="13">
         <v>43649</v>
       </c>
@@ -31754,7 +32072,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="228" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B228" s="13">
         <v>43743</v>
       </c>
@@ -31805,7 +32123,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="229" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B229" s="13" t="s">
         <v>69</v>
       </c>
@@ -31856,7 +32174,7 @@
         <v>Vencida</v>
       </c>
     </row>
-    <row r="230" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B230" s="13">
         <v>43647</v>
       </c>
@@ -31907,7 +32225,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="231" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B231" s="13">
         <v>43687</v>
       </c>
@@ -31958,7 +32276,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="232" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B232" s="13">
         <v>43702</v>
       </c>
@@ -32009,7 +32327,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="233" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B233" s="13">
         <v>43710</v>
       </c>
@@ -32060,7 +32378,7 @@
         <v>Não Vencida</v>
       </c>
     </row>
-    <row r="234" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B234" s="13">
         <v>43647</v>
       </c>
@@ -32133,9 +32451,9 @@
   <sheetPr codeName="Plan8"/>
   <dimension ref="B1:N232"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H232" sqref="H3:H232"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F211" sqref="F211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43005,7 +43323,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aula 28 - Dashboard Anual Resultado Acumulado
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="879" firstSheet="11" activeTab="17"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="879" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="1" r:id="rId1"/>
@@ -2690,7 +2690,7 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -3114,6 +3114,9 @@
     </xf>
     <xf numFmtId="172" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="28" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3661,6 +3664,175 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.2700116271067987E-2"/>
+          <c:y val="0.11901312814762001"/>
+          <c:w val="0.95459976745786401"/>
+          <c:h val="0.64244832807639951"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>DashBoardFinanceiroAnualD!$C$31:$D$31</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Entradas</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Saídas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DashBoardFinanceiroAnualD!$C$32:$D$32</c:f>
+              <c:numCache>
+                <c:formatCode>"R$"\ #,##0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>129286</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>163337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="10"/>
+        <c:axId val="90639744"/>
+        <c:axId val="90724224"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="90639744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90724224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90724224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="&quot;R$&quot;\ #,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90639744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
     <a:ln>
       <a:noFill/>
     </a:ln>
@@ -6173,6 +6345,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>10026</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2247900</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>333374</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -18419,8 +18623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18651,7 +18855,8 @@
       </c>
       <c r="H14" s="67"/>
       <c r="I14" s="71">
-        <v>-12</v>
+        <f>DashBoardFinanceiroAnualD!E32</f>
+        <v>-34051</v>
       </c>
       <c r="J14" s="49"/>
       <c r="K14" s="99"/>
@@ -18825,8 +19030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView showGridLines="0" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19617,10 +19822,22 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="103"/>
-      <c r="B32" s="132"/>
-      <c r="C32" s="133"/>
-      <c r="D32" s="133"/>
-      <c r="E32" s="134"/>
+      <c r="B32" s="154">
+        <f>$C$4</f>
+        <v>2019</v>
+      </c>
+      <c r="C32" s="133">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Ano Caixa],$B$32)</f>
+        <v>129286</v>
+      </c>
+      <c r="D32" s="133">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$B$32)</f>
+        <v>163337</v>
+      </c>
+      <c r="E32" s="134">
+        <f>C32-D32</f>
+        <v>-34051</v>
+      </c>
       <c r="F32" s="103"/>
       <c r="G32" s="103">
         <v>1</v>

</xml_diff>

<commit_message>
Aula 29 - Dashboard Anual Despesa Mensal
</commit_message>
<xml_diff>
--- a/ProjetoFluxoCaixa.xlsx
+++ b/ProjetoFluxoCaixa.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1823" uniqueCount="616">
   <si>
     <t>FLUXO DE CAIXA EMPRESARIAL</t>
   </si>
@@ -1898,6 +1898,30 @@
   </si>
   <si>
     <t>Dias de Atraso</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -2690,7 +2714,7 @@
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -3118,6 +3142,9 @@
     <xf numFmtId="1" fontId="28" fillId="7" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -3125,15 +3152,6 @@
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="39">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -3166,6 +3184,15 @@
         <i val="0"/>
         <color rgb="FFFF0000"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3823,6 +3850,196 @@
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>DashBoardFinanceiroAnualD!$I$32:$I$43</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>F</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>M</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>M</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>J</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>S</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>O</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>N</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>DashBoardFinanceiroAnualD!$H$32:$H$43</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1628</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3519</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3695</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>802</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6262</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6281</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="15"/>
+        <c:axId val="75681152"/>
+        <c:axId val="90748800"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="75681152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90748800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90748800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75681152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
         </a:ln>
       </c:spPr>
@@ -6377,6 +6594,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>209549</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2428875</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -15378,10 +15627,10 @@
     <tableColumn id="14" name="Conta Vencida" dataDxfId="21">
       <calculatedColumnFormula>IF(AND(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]&lt;TODAY(),TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]=""),"Vencida","Não Vencida")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Venda à Vista" dataDxfId="2">
+    <tableColumn id="15" name="Venda à Vista" dataDxfId="7">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data da Competência]]=TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]],"Vista","Prazo")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Dias de Atraso" dataDxfId="1">
+    <tableColumn id="16" name="Dias de Atraso" dataDxfId="6">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]&lt;&gt;"",
  IF(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]&gt;TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]],
   TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]-TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]],
@@ -15401,15 +15650,15 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TbRegistroSaídas" displayName="TbRegistroSaídas" ref="B3:O232" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18">
   <autoFilter ref="B3:O232">
-    <filterColumn colId="2">
+    <filterColumn colId="0">
       <filters>
-        <dateGroupItem year="2019" dateTimeGrouping="year"/>
+        <dateGroupItem year="2019" month="1" dateTimeGrouping="month"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="13">
-      <customFilters>
-        <customFilter operator="greaterThan" val="0"/>
-      </customFilters>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Informática"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="14">
@@ -15438,7 +15687,7 @@
     <tableColumn id="13" name="Ano Previsto" dataDxfId="8">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data do Caixa Previsto]]="",0,YEAR(TbRegistroSaídas[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Dias de Atraso" dataDxfId="0">
+    <tableColumn id="14" name="Dias de Atraso" dataDxfId="5">
       <calculatedColumnFormula>IF(TbRegistroSaídas[[#This Row],[Data do Caixa Realizado]]&lt;&gt;"",
  IF(TbRegistroSaídas[[#This Row],[Data do Caixa Realizado]]&gt;TbRegistroSaídas[[#This Row],[Data do Caixa Previsto]],
   TbRegistroSaídas[[#This Row],[Data do Caixa Realizado]]-TbRegistroSaídas[[#This Row],[Data do Caixa Previsto]],
@@ -17775,7 +18024,7 @@
     <mergeCell ref="F13:G13"/>
   </mergeCells>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18611,7 +18860,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18624,7 +18873,7 @@
   <dimension ref="B1:O21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18859,7 +19108,9 @@
         <v>-34051</v>
       </c>
       <c r="J14" s="49"/>
-      <c r="K14" s="99"/>
+      <c r="K14" s="99" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="68"/>
@@ -18872,7 +19123,8 @@
       <c r="I15" s="74"/>
       <c r="J15" s="49"/>
       <c r="K15" s="97">
-        <v>48</v>
+        <f>DashBoardFinanceiroAnualD!H44</f>
+        <v>22187</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -18968,17 +19220,19 @@
     <mergeCell ref="F13:G13"/>
   </mergeCells>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conta Inexistente!" error="Selecione uma conta da lista." sqref="K14"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conta Inexistente!" error="Selecione uma conta da lista." sqref="K14">
+      <formula1>PCSaídasN2_Nível_2</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Conta Inexisente!" error="Selecione um item da conta." sqref="K4">
       <formula1>PCEntradasN2_Nível_2</formula1>
     </dataValidation>
@@ -19030,8 +19284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView showGridLines="0" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19787,7 +20041,10 @@
       <c r="G30" s="105" t="s">
         <v>601</v>
       </c>
-      <c r="H30" s="129"/>
+      <c r="H30" s="129">
+        <f>$C$4</f>
+        <v>2019</v>
+      </c>
       <c r="I30" s="103"/>
       <c r="J30" s="103"/>
       <c r="K30" s="103"/>
@@ -19811,9 +20068,9 @@
       <c r="G31" s="109" t="s">
         <v>569</v>
       </c>
-      <c r="H31" s="131" t="str">
-        <f>[1]DashBoardFinanceiroAnual!K14</f>
-        <v>Vestuário</v>
+      <c r="H31" s="155" t="str">
+        <f>DashBoardFinanceiroAnual!$K$14</f>
+        <v>Informática</v>
       </c>
       <c r="I31" s="103"/>
       <c r="J31" s="103"/>
@@ -19838,12 +20095,16 @@
         <f>C32-D32</f>
         <v>-34051</v>
       </c>
-      <c r="F32" s="103"/>
       <c r="G32" s="103">
         <v>1</v>
       </c>
-      <c r="H32" s="115"/>
-      <c r="I32" s="103"/>
+      <c r="H32" s="115">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$H$30,TbRegistroSaídas[Conta Nível 2],$H$31,TbRegistroSaídas[Mês Caixa],G32)</f>
+        <v>1628</v>
+      </c>
+      <c r="I32" s="103" t="s">
+        <v>608</v>
+      </c>
       <c r="J32" s="103"/>
       <c r="K32" s="103"/>
       <c r="L32" s="103"/>
@@ -19854,12 +20115,16 @@
       <c r="C33" s="103"/>
       <c r="D33" s="103"/>
       <c r="E33" s="103"/>
-      <c r="F33" s="103"/>
       <c r="G33" s="103">
         <v>2</v>
       </c>
-      <c r="H33" s="115"/>
-      <c r="I33" s="103"/>
+      <c r="H33" s="115">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$H$30,TbRegistroSaídas[Conta Nível 2],$H$31,TbRegistroSaídas[Mês Caixa],G33)</f>
+        <v>3519</v>
+      </c>
+      <c r="I33" s="103" t="s">
+        <v>609</v>
+      </c>
       <c r="J33" s="103"/>
       <c r="K33" s="103"/>
       <c r="L33" s="103"/>
@@ -19870,12 +20135,16 @@
       <c r="C34" s="103"/>
       <c r="D34" s="103"/>
       <c r="E34" s="103"/>
-      <c r="F34" s="103"/>
       <c r="G34" s="103">
         <v>3</v>
       </c>
-      <c r="H34" s="115"/>
-      <c r="I34" s="103"/>
+      <c r="H34" s="115">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$H$30,TbRegistroSaídas[Conta Nível 2],$H$31,TbRegistroSaídas[Mês Caixa],G34)</f>
+        <v>3695</v>
+      </c>
+      <c r="I34" s="103" t="s">
+        <v>610</v>
+      </c>
       <c r="J34" s="103"/>
       <c r="K34" s="103"/>
       <c r="L34" s="103"/>
@@ -19886,12 +20155,16 @@
       <c r="C35" s="103"/>
       <c r="D35" s="103"/>
       <c r="E35" s="103"/>
-      <c r="F35" s="103"/>
       <c r="G35" s="103">
         <v>4</v>
       </c>
-      <c r="H35" s="115"/>
-      <c r="I35" s="103"/>
+      <c r="H35" s="115">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$H$30,TbRegistroSaídas[Conta Nível 2],$H$31,TbRegistroSaídas[Mês Caixa],G35)</f>
+        <v>802</v>
+      </c>
+      <c r="I35" s="103" t="s">
+        <v>611</v>
+      </c>
       <c r="J35" s="103"/>
       <c r="K35" s="103"/>
       <c r="L35" s="103"/>
@@ -19902,12 +20175,16 @@
       <c r="C36" s="103"/>
       <c r="D36" s="103"/>
       <c r="E36" s="103"/>
-      <c r="F36" s="103"/>
       <c r="G36" s="103">
         <v>5</v>
       </c>
-      <c r="H36" s="115"/>
-      <c r="I36" s="103"/>
+      <c r="H36" s="115">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$H$30,TbRegistroSaídas[Conta Nível 2],$H$31,TbRegistroSaídas[Mês Caixa],G36)</f>
+        <v>6262</v>
+      </c>
+      <c r="I36" s="103" t="s">
+        <v>610</v>
+      </c>
       <c r="J36" s="103"/>
       <c r="K36" s="103"/>
       <c r="L36" s="103"/>
@@ -19918,12 +20195,16 @@
       <c r="C37" s="103"/>
       <c r="D37" s="103"/>
       <c r="E37" s="103"/>
-      <c r="F37" s="103"/>
       <c r="G37" s="103">
         <v>6</v>
       </c>
-      <c r="H37" s="115"/>
-      <c r="I37" s="103"/>
+      <c r="H37" s="115">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$H$30,TbRegistroSaídas[Conta Nível 2],$H$31,TbRegistroSaídas[Mês Caixa],G37)</f>
+        <v>6281</v>
+      </c>
+      <c r="I37" s="103" t="s">
+        <v>608</v>
+      </c>
       <c r="J37" s="103"/>
       <c r="K37" s="103"/>
       <c r="L37" s="103"/>
@@ -19934,12 +20215,16 @@
       <c r="C38" s="103"/>
       <c r="D38" s="103"/>
       <c r="E38" s="103"/>
-      <c r="F38" s="103"/>
       <c r="G38" s="103">
         <v>7</v>
       </c>
-      <c r="H38" s="115"/>
-      <c r="I38" s="103"/>
+      <c r="H38" s="115">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$H$30,TbRegistroSaídas[Conta Nível 2],$H$31,TbRegistroSaídas[Mês Caixa],G38)</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="103" t="s">
+        <v>608</v>
+      </c>
       <c r="J38" s="103"/>
       <c r="K38" s="103"/>
       <c r="L38" s="103"/>
@@ -19950,12 +20235,16 @@
       <c r="C39" s="103"/>
       <c r="D39" s="103"/>
       <c r="E39" s="103"/>
-      <c r="F39" s="103"/>
       <c r="G39" s="103">
         <v>8</v>
       </c>
-      <c r="H39" s="115"/>
-      <c r="I39" s="103"/>
+      <c r="H39" s="115">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$H$30,TbRegistroSaídas[Conta Nível 2],$H$31,TbRegistroSaídas[Mês Caixa],G39)</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="103" t="s">
+        <v>611</v>
+      </c>
       <c r="J39" s="103"/>
       <c r="K39" s="103"/>
       <c r="L39" s="103"/>
@@ -19966,12 +20255,16 @@
       <c r="C40" s="103"/>
       <c r="D40" s="103"/>
       <c r="E40" s="103"/>
-      <c r="F40" s="103"/>
       <c r="G40" s="103">
         <v>9</v>
       </c>
-      <c r="H40" s="115"/>
-      <c r="I40" s="103"/>
+      <c r="H40" s="115">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$H$30,TbRegistroSaídas[Conta Nível 2],$H$31,TbRegistroSaídas[Mês Caixa],G40)</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="103" t="s">
+        <v>612</v>
+      </c>
       <c r="J40" s="103"/>
       <c r="K40" s="103"/>
       <c r="L40" s="103"/>
@@ -19982,12 +20275,16 @@
       <c r="C41" s="103"/>
       <c r="D41" s="103"/>
       <c r="E41" s="103"/>
-      <c r="F41" s="103"/>
       <c r="G41" s="103">
         <v>10</v>
       </c>
-      <c r="H41" s="115"/>
-      <c r="I41" s="103"/>
+      <c r="H41" s="115">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$H$30,TbRegistroSaídas[Conta Nível 2],$H$31,TbRegistroSaídas[Mês Caixa],G41)</f>
+        <v>0</v>
+      </c>
+      <c r="I41" s="103" t="s">
+        <v>613</v>
+      </c>
       <c r="J41" s="103"/>
       <c r="K41" s="103"/>
       <c r="L41" s="103"/>
@@ -19998,12 +20295,16 @@
       <c r="C42" s="103"/>
       <c r="D42" s="103"/>
       <c r="E42" s="103"/>
-      <c r="F42" s="103"/>
       <c r="G42" s="103">
         <v>11</v>
       </c>
-      <c r="H42" s="115"/>
-      <c r="I42" s="103"/>
+      <c r="H42" s="115">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$H$30,TbRegistroSaídas[Conta Nível 2],$H$31,TbRegistroSaídas[Mês Caixa],G42)</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="103" t="s">
+        <v>614</v>
+      </c>
       <c r="J42" s="103"/>
       <c r="K42" s="103"/>
       <c r="L42" s="103"/>
@@ -20014,12 +20315,16 @@
       <c r="C43" s="103"/>
       <c r="D43" s="103"/>
       <c r="E43" s="103"/>
-      <c r="F43" s="103"/>
       <c r="G43" s="118">
         <v>12</v>
       </c>
-      <c r="H43" s="115"/>
-      <c r="I43" s="103"/>
+      <c r="H43" s="115">
+        <f>SUMIFS(TbRegistroSaídas[Valor],TbRegistroSaídas[Ano Caixa],$H$30,TbRegistroSaídas[Conta Nível 2],$H$31,TbRegistroSaídas[Mês Caixa],G43)</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="103" t="s">
+        <v>615</v>
+      </c>
       <c r="J43" s="103"/>
       <c r="K43" s="103"/>
       <c r="L43" s="103"/>
@@ -20034,7 +20339,10 @@
       <c r="G44" s="109" t="s">
         <v>554</v>
       </c>
-      <c r="H44" s="135"/>
+      <c r="H44" s="135">
+        <f>SUM(H32:H43)</f>
+        <v>22187</v>
+      </c>
       <c r="I44" s="103"/>
       <c r="J44" s="103"/>
       <c r="K44" s="103"/>
@@ -20062,7 +20370,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C11">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20595,7 +20903,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36622,9 +36930,9 @@
   <sheetPr codeName="Plan8"/>
   <dimension ref="B1:O232"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O156" sqref="O156:O229"/>
+      <selection pane="bottomLeft" activeCell="H156" sqref="H156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46491,7 +46799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B167" s="13" t="s">
         <v>69</v>
       </c>
@@ -47031,7 +47339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B176" s="13">
         <v>43569</v>
       </c>
@@ -47331,7 +47639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B181" s="13" t="s">
         <v>69</v>
       </c>
@@ -47511,7 +47819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B184" s="13" t="s">
         <v>69</v>
       </c>
@@ -47811,7 +48119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B189" s="13" t="s">
         <v>69</v>
       </c>
@@ -48111,7 +48419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B194" s="13" t="s">
         <v>69</v>
       </c>
@@ -48711,7 +49019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B204" s="13" t="s">
         <v>69</v>
       </c>
@@ -48771,7 +49079,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="205" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B205" s="13">
         <v>43647</v>
       </c>
@@ -48831,7 +49139,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="206" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B206" s="13">
         <v>43578</v>
       </c>
@@ -49011,7 +49319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B209" s="13" t="s">
         <v>69</v>
       </c>
@@ -49131,7 +49439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B211" s="13">
         <v>43661</v>
       </c>
@@ -49911,7 +50219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B224" s="13" t="s">
         <v>69</v>
       </c>
@@ -50211,7 +50519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B229" s="13" t="s">
         <v>69</v>
       </c>

</xml_diff>